<commit_message>
A little bit of data updated
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clemens/Documents/Uni/GIT/MatlabWD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB9E7F8-2774-AD44-B09E-FA78B8106493}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18800"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>parvariable</t>
   </si>
@@ -60,9 +61,6 @@
     <t>Nitrogen</t>
   </si>
   <si>
-    <t>Oxygen</t>
-  </si>
-  <si>
     <t>chemform</t>
   </si>
   <si>
@@ -105,21 +103,6 @@
     <t>entity D</t>
   </si>
   <si>
-    <t>Cooling Water</t>
-  </si>
-  <si>
-    <t>$H_{2}O$</t>
-  </si>
-  <si>
-    <t>$N_{2}$</t>
-  </si>
-  <si>
-    <t>ChemFormulaLatex</t>
-  </si>
-  <si>
-    <t>$O_{2}$</t>
-  </si>
-  <si>
     <t>Molecular Weight</t>
   </si>
   <si>
@@ -147,33 +130,12 @@
     <t>Reactor</t>
   </si>
   <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Sparger</t>
-  </si>
-  <si>
-    <t>Crystalizer</t>
-  </si>
-  <si>
     <t>Volume</t>
   </si>
   <si>
     <t>V</t>
   </si>
   <si>
-    <t>Inlet flow</t>
-  </si>
-  <si>
-    <t>Qin</t>
-  </si>
-  <si>
-    <t>Outlet Flow</t>
-  </si>
-  <si>
-    <t>Qout</t>
-  </si>
-  <si>
     <t>Optimal conversion</t>
   </si>
   <si>
@@ -213,19 +175,76 @@
     <t>totex</t>
   </si>
   <si>
-    <t>RedBull</t>
-  </si>
-  <si>
     <t>tspan</t>
   </si>
   <si>
-    <t>reactir simulation time</t>
+    <t>NH3Absorber</t>
+  </si>
+  <si>
+    <t>HCNAbsorber</t>
+  </si>
+  <si>
+    <t>Distillation</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>rad</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>En</t>
+  </si>
+  <si>
+    <t>unit simulation time</t>
+  </si>
+  <si>
+    <t>Lebensdauer</t>
+  </si>
+  <si>
+    <t>lspan</t>
+  </si>
+  <si>
+    <t>H20</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>ChemFormula</t>
+  </si>
+  <si>
+    <t>Methane</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>HCN</t>
+  </si>
+  <si>
+    <t>VolumeVoid</t>
+  </si>
+  <si>
+    <t>epsilon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -276,7 +295,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -587,11 +606,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,21 +635,21 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -659,38 +678,41 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
       </c>
       <c r="C5">
         <v>7</v>
@@ -707,10 +729,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -727,10 +749,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>13</v>
@@ -747,10 +769,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -767,10 +789,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>1.7999999999999999E-2</v>
@@ -787,10 +809,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -800,11 +822,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -820,27 +842,27 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -860,166 +882,123 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
         <v>40</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>9</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>11</v>
-      </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7">
-        <v>0.1</v>
-      </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1000000</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1300000</v>
-      </c>
-      <c r="D9">
-        <v>20</v>
-      </c>
-      <c r="F9">
-        <v>889</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10">
-        <v>3.141</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1.0000000000000001E-9</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13">
+        <f>10*365*24*3600</f>
+        <v>315360000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14">
+        <v>0.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New data (enthalpies, Gibbs, entropies)
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="230">
   <si>
     <t>parvariable</t>
   </si>
@@ -654,13 +654,76 @@
   </si>
   <si>
     <t>4.5</t>
+  </si>
+  <si>
+    <t>Lange, CRC(H2SO4)</t>
+  </si>
+  <si>
+    <t>Enthalpy of formation</t>
+  </si>
+  <si>
+    <t>Gibbs of formation</t>
+  </si>
+  <si>
+    <t>deltaHf</t>
+  </si>
+  <si>
+    <t>deltaGf</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>J.mol-1</t>
+  </si>
+  <si>
+    <t>J.K-1.mol-1</t>
+  </si>
+  <si>
+    <t>186.3</t>
+  </si>
+  <si>
+    <t>Hm</t>
+  </si>
+  <si>
+    <t>Hv</t>
+  </si>
+  <si>
+    <t>Enthalpy of melting at mp</t>
+  </si>
+  <si>
+    <t>Enthalpy of vaporization at bp</t>
+  </si>
+  <si>
+    <t>192.78</t>
+  </si>
+  <si>
+    <t>220.1</t>
+  </si>
+  <si>
+    <t>130.68</t>
+  </si>
+  <si>
+    <t>112.84</t>
+  </si>
+  <si>
+    <t>69.95</t>
+  </si>
+  <si>
+    <t>156.90</t>
+  </si>
+  <si>
+    <t>191.61</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -708,11 +771,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri (Corps)"/>
@@ -723,7 +781,7 @@
       <name val="TT1AAt00"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -742,6 +800,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -752,7 +816,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -784,8 +848,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -794,11 +860,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -814,6 +881,7 @@
     <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -829,6 +897,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1143,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1204,141 +1273,141 @@
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>2</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>3</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>4</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>5</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>6</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>7</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="7">
         <v>8</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="7">
         <v>9</v>
       </c>
-      <c r="L2" s="8"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="16">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="8"/>
+      <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:13" ht="16">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:13" ht="16">
       <c r="A5" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8" t="s">
+      <c r="K5" s="7"/>
+      <c r="L5" s="7" t="s">
         <v>162</v>
       </c>
       <c r="M5" t="s">
@@ -1349,33 +1418,33 @@
       <c r="A6" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="11">
         <v>20</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="11">
         <v>40</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
       <c r="M6" t="s">
         <v>184</v>
       </c>
@@ -1384,33 +1453,33 @@
       <c r="A7" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="11">
         <v>50</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="11">
         <v>70</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
       <c r="M7" t="s">
         <v>184</v>
       </c>
@@ -1419,33 +1488,33 @@
       <c r="A8" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="11">
         <v>0</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="11">
         <v>0</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
       <c r="M8" t="s">
         <v>184</v>
       </c>
@@ -1454,33 +1523,33 @@
       <c r="A9" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="11">
         <v>0</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="11">
         <v>0</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
       <c r="M9" t="s">
         <v>184</v>
       </c>
@@ -1489,33 +1558,33 @@
       <c r="A10" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="11">
         <v>0</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="11">
         <v>0</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <v>0</v>
       </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
       <c r="M10" t="s">
         <v>184</v>
       </c>
@@ -1524,33 +1593,33 @@
       <c r="A11" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="11">
         <v>0</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="11">
         <v>0</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <v>0</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
       <c r="M11" t="s">
         <v>184</v>
       </c>
@@ -1559,38 +1628,38 @@
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8" t="s">
+      <c r="K12" s="7"/>
+      <c r="L12" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="7" t="s">
         <v>171</v>
       </c>
     </row>
@@ -1598,56 +1667,56 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:13" ht="16">
       <c r="A14" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>14</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8" t="s">
+      <c r="K14" s="7"/>
+      <c r="L14" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="M14" s="7" t="s">
         <v>171</v>
       </c>
     </row>
@@ -1655,36 +1724,36 @@
       <c r="A15" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8" t="s">
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="M15" s="8" t="s">
+      <c r="M15" s="7" t="s">
         <v>171</v>
       </c>
     </row>
@@ -1692,61 +1761,241 @@
       <c r="A16" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>997</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7">
         <v>687</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="7">
         <v>1831</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="7">
         <v>1769</v>
       </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8" t="s">
+      <c r="K16" s="7"/>
+      <c r="L16" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="M16" s="8" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="16">
+      <c r="M16" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="16">
       <c r="A17" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="16">
+    <row r="18" spans="1:13" ht="16">
       <c r="A18" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>193</v>
       </c>
       <c r="K18" t="s">
         <v>208</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="L18" s="9" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="16">
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+    <row r="19" spans="1:13" ht="16">
+      <c r="A19" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19">
+        <v>-285830</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>-74600</v>
+      </c>
+      <c r="F19">
+        <v>-45940</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>108870</v>
+      </c>
+      <c r="I19">
+        <v>-814000</v>
+      </c>
+      <c r="J19">
+        <v>-1180900</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="16">
+      <c r="A20" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C20">
+        <v>-237140</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>-50500</v>
+      </c>
+      <c r="F20">
+        <v>-16400</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>124930</v>
+      </c>
+      <c r="I20">
+        <v>-689900</v>
+      </c>
+      <c r="J20">
+        <v>-901700</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="16">
+      <c r="A21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C21" t="s">
+        <v>227</v>
+      </c>
+      <c r="D21" t="s">
+        <v>229</v>
+      </c>
+      <c r="E21" t="s">
+        <v>218</v>
+      </c>
+      <c r="F21" t="s">
+        <v>223</v>
+      </c>
+      <c r="G21" t="s">
+        <v>225</v>
+      </c>
+      <c r="H21" t="s">
+        <v>226</v>
+      </c>
+      <c r="I21" t="s">
+        <v>228</v>
+      </c>
+      <c r="J21" t="s">
+        <v>224</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="16">
+      <c r="A22" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C22">
+        <v>6009</v>
+      </c>
+      <c r="D22">
+        <v>720</v>
+      </c>
+      <c r="E22">
+        <v>940</v>
+      </c>
+      <c r="F22">
+        <v>5660</v>
+      </c>
+      <c r="G22">
+        <v>117</v>
+      </c>
+      <c r="H22">
+        <v>8406</v>
+      </c>
+      <c r="I22">
+        <v>10710</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="16">
+      <c r="A23" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C23">
+        <v>40660</v>
+      </c>
+      <c r="D23">
+        <v>5577</v>
+      </c>
+      <c r="E23">
+        <v>8200</v>
+      </c>
+      <c r="F23">
+        <v>23350</v>
+      </c>
+      <c r="G23">
+        <v>904</v>
+      </c>
+      <c r="H23">
+        <v>25220</v>
+      </c>
+      <c r="I23">
+        <v>50200</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>183</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1763,8 +2012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1963,7 +2212,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Van der Waals parameters added
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="251">
   <si>
     <t>parvariable</t>
   </si>
@@ -726,6 +726,60 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Van der Waals Parameter A</t>
+  </si>
+  <si>
+    <t>vdwa</t>
+  </si>
+  <si>
+    <t>Van der Waals Parameter B</t>
+  </si>
+  <si>
+    <t>vdwb</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>0.04301e-6</t>
+  </si>
+  <si>
+    <t>1.518</t>
+  </si>
+  <si>
+    <t>0.1288e-6</t>
+  </si>
+  <si>
+    <t>0.02484</t>
+  </si>
+  <si>
+    <t>m6.Pa.mol-2</t>
+  </si>
+  <si>
+    <t>m6.mol-1</t>
+  </si>
+  <si>
+    <t>0.02651e-6</t>
+  </si>
+  <si>
+    <t>0.4225</t>
+  </si>
+  <si>
+    <t>0.03713e-6</t>
+  </si>
+  <si>
+    <t>1.129</t>
+  </si>
+  <si>
+    <t>0.08806e-6</t>
+  </si>
+  <si>
+    <t>0.5537</t>
+  </si>
+  <si>
+    <t>0.03052e-6</t>
   </si>
 </sst>
 </file>
@@ -825,8 +879,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -876,7 +932,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="37">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -894,6 +950,7 @@
     <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -911,6 +968,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1223,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1237,7 +1295,7 @@
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
     <col min="10" max="11" width="18.83203125" customWidth="1"/>
-    <col min="12" max="12" width="12.5" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
     <col min="13" max="13" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2007,6 +2065,70 @@
         <v>214</v>
       </c>
       <c r="M23" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="16">
+      <c r="A24" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" t="s">
+        <v>249</v>
+      </c>
+      <c r="D24" t="s">
+        <v>239</v>
+      </c>
+      <c r="E24" t="s">
+        <v>237</v>
+      </c>
+      <c r="F24" t="s">
+        <v>245</v>
+      </c>
+      <c r="G24" t="s">
+        <v>241</v>
+      </c>
+      <c r="H24" t="s">
+        <v>247</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="16">
+      <c r="A25" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C25" t="s">
+        <v>250</v>
+      </c>
+      <c r="D25" t="s">
+        <v>240</v>
+      </c>
+      <c r="E25" t="s">
+        <v>238</v>
+      </c>
+      <c r="F25" t="s">
+        <v>246</v>
+      </c>
+      <c r="G25" t="s">
+        <v>244</v>
+      </c>
+      <c r="H25" t="s">
+        <v>248</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="M25" s="7" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2025,8 +2147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
New heat capacity parameters
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="296">
   <si>
     <t>parvariable</t>
   </si>
@@ -338,9 +338,6 @@
     <t>unit</t>
   </si>
   <si>
-    <t>J.kg-1.K-1</t>
-  </si>
-  <si>
     <t>kg.mol-1</t>
   </si>
   <si>
@@ -815,88 +812,109 @@
     <t>pare</t>
   </si>
   <si>
-    <t>J.kg-1.K-2</t>
-  </si>
-  <si>
-    <t>J.kg-1.K-3</t>
-  </si>
-  <si>
-    <t>J.kg-1.K-4</t>
-  </si>
-  <si>
-    <t>J.kg-1.K-5</t>
-  </si>
-  <si>
-    <t>27.26</t>
-  </si>
-  <si>
-    <t>2.313e-4</t>
-  </si>
-  <si>
-    <t>2.243e-7</t>
-  </si>
-  <si>
-    <t>-2.169e-10</t>
-  </si>
-  <si>
-    <t>5.41e-14</t>
-  </si>
-  <si>
-    <t>26.69</t>
-  </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
-    <t>-2.384e-5</t>
-  </si>
-  <si>
-    <t>2.004e-8</t>
-  </si>
-  <si>
-    <t>-5.427e-12</t>
-  </si>
-  <si>
-    <t>26.39</t>
-  </si>
-  <si>
-    <t>6.236e-3</t>
-  </si>
-  <si>
-    <t>1.076e-4</t>
-  </si>
-  <si>
-    <t>-9.015e-8</t>
-  </si>
-  <si>
-    <t>2.28e-11</t>
-  </si>
-  <si>
-    <t>31.44</t>
-  </si>
-  <si>
-    <t>-0.01</t>
-  </si>
-  <si>
-    <t>3.669e-5</t>
-  </si>
-  <si>
-    <t>-2.419e-8</t>
-  </si>
-  <si>
-    <t>5.433e-12</t>
-  </si>
-  <si>
-    <t>34.51</t>
-  </si>
-  <si>
-    <t>4.686e-5</t>
-  </si>
-  <si>
-    <t>-3.781e-8</t>
-  </si>
-  <si>
-    <t>1.173e-11</t>
+    <t>K-1</t>
+  </si>
+  <si>
+    <t>K-2</t>
+  </si>
+  <si>
+    <t>K-3</t>
+  </si>
+  <si>
+    <t>K-4</t>
+  </si>
+  <si>
+    <t>2.6770</t>
+  </si>
+  <si>
+    <t>2.9732e-3</t>
+  </si>
+  <si>
+    <t>-7.7377e-7</t>
+  </si>
+  <si>
+    <t>9.4434e-11</t>
+  </si>
+  <si>
+    <t>-42690e-15</t>
+  </si>
+  <si>
+    <t>2.9526</t>
+  </si>
+  <si>
+    <t>1.3969e-3</t>
+  </si>
+  <si>
+    <t>-4.9263e-7</t>
+  </si>
+  <si>
+    <t>7.8601e-11</t>
+  </si>
+  <si>
+    <t>-4.6076e-15</t>
+  </si>
+  <si>
+    <t>1.6355</t>
+  </si>
+  <si>
+    <t>1.0084e-2</t>
+  </si>
+  <si>
+    <t>-3.3692e-6</t>
+  </si>
+  <si>
+    <t>5.3496e-3</t>
+  </si>
+  <si>
+    <t>3.1552e-14</t>
+  </si>
+  <si>
+    <t>McBride</t>
+  </si>
+  <si>
+    <t>2.7171</t>
+  </si>
+  <si>
+    <t>5.5686e-3</t>
+  </si>
+  <si>
+    <t>-1.7689e-6</t>
+  </si>
+  <si>
+    <t>2.6742e-10</t>
+  </si>
+  <si>
+    <t>-1.5273e-14</t>
+  </si>
+  <si>
+    <t>2.9329</t>
+  </si>
+  <si>
+    <t>8.2661e-4</t>
+  </si>
+  <si>
+    <t>-1.4640e-7</t>
+  </si>
+  <si>
+    <t>1.5410e-11</t>
+  </si>
+  <si>
+    <t>-6.8880e-16</t>
+  </si>
+  <si>
+    <t>3.8023</t>
+  </si>
+  <si>
+    <t>3.1463e-3</t>
+  </si>
+  <si>
+    <t>-1.0632e-6</t>
+  </si>
+  <si>
+    <t>1.6619e-9</t>
+  </si>
+  <si>
+    <t>-9.7989e-15</t>
   </si>
 </sst>
 </file>
@@ -996,8 +1014,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1052,7 +1092,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="61">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1072,6 +1112,17 @@
     <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1091,6 +1142,17 @@
     <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1395,7 +1457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1405,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1459,7 +1521,7 @@
         <v>102</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16">
@@ -1515,22 +1577,22 @@
         <v>55</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L3" s="8"/>
     </row>
@@ -1551,7 +1613,7 @@
         <v>56</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>58</v>
@@ -1560,217 +1622,217 @@
         <v>59</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:13" ht="16">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>183</v>
-      </c>
       <c r="E5" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>170</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16">
       <c r="A6" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E6" s="12">
         <v>20</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G6" s="12">
         <v>40</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="16">
       <c r="A7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="C7" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E7" s="12">
         <v>50</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G7" s="12">
         <v>70</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="16">
       <c r="A8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E8" s="12">
         <v>0</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G8" s="12">
         <v>0</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="16">
       <c r="A9" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E9" s="12">
         <v>0</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G9" s="12">
         <v>0</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="16">
       <c r="A10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" s="12">
         <v>0</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G10" s="12">
         <v>0</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I10" s="8">
         <v>0</v>
@@ -1779,33 +1841,33 @@
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
       <c r="M10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16">
       <c r="A11" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E11" s="12">
         <v>0</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G11" s="12">
         <v>0</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I11" s="8">
         <v>0</v>
@@ -1814,7 +1876,7 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="16">
@@ -1825,35 +1887,35 @@
         <v>17</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K12" s="8"/>
       <c r="L12" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="16">
@@ -1876,86 +1938,86 @@
     </row>
     <row r="14" spans="1:13" ht="16">
       <c r="A14" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="D14" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G14" s="8">
         <v>14</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16">
       <c r="A15" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16">
       <c r="A16" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" s="8">
         <v>997</v>
@@ -1975,43 +2037,43 @@
       </c>
       <c r="K16" s="8"/>
       <c r="L16" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="16">
       <c r="A17" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>157</v>
-      </c>
       <c r="L17" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="16">
       <c r="A18" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>192</v>
-      </c>
       <c r="K18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="16">
       <c r="A19" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C19">
         <v>-285830</v>
@@ -2038,18 +2100,18 @@
         <v>-1180900</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="16">
       <c r="A20" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C20">
         <v>-237140</v>
@@ -2076,56 +2138,56 @@
         <v>-901700</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="16">
       <c r="A21" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>214</v>
-      </c>
       <c r="C21" t="s">
+        <v>225</v>
+      </c>
+      <c r="D21" t="s">
+        <v>227</v>
+      </c>
+      <c r="E21" t="s">
+        <v>216</v>
+      </c>
+      <c r="F21" t="s">
+        <v>221</v>
+      </c>
+      <c r="G21" t="s">
+        <v>223</v>
+      </c>
+      <c r="H21" t="s">
+        <v>224</v>
+      </c>
+      <c r="I21" t="s">
         <v>226</v>
       </c>
-      <c r="D21" t="s">
-        <v>228</v>
-      </c>
-      <c r="E21" t="s">
-        <v>217</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="J21" t="s">
         <v>222</v>
       </c>
-      <c r="G21" t="s">
-        <v>224</v>
-      </c>
-      <c r="H21" t="s">
-        <v>225</v>
-      </c>
-      <c r="I21" t="s">
-        <v>227</v>
-      </c>
-      <c r="J21" t="s">
-        <v>223</v>
-      </c>
       <c r="L21" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="16">
       <c r="A22" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C22">
         <v>6009</v>
@@ -2149,18 +2211,18 @@
         <v>10710</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="16">
       <c r="A23" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C23">
         <v>40660</v>
@@ -2184,204 +2246,232 @@
         <v>50200</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="16">
       <c r="A24" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>235</v>
-      </c>
       <c r="C24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G24" t="s">
+        <v>241</v>
+      </c>
+      <c r="H24" t="s">
+        <v>247</v>
+      </c>
+      <c r="L24" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="H24" t="s">
-        <v>248</v>
-      </c>
-      <c r="L24" s="8" t="s">
-        <v>243</v>
-      </c>
       <c r="M24" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="16">
       <c r="A25" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>237</v>
-      </c>
       <c r="C25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="16">
       <c r="A26" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>253</v>
-      </c>
       <c r="C26" t="s">
+        <v>265</v>
+      </c>
+      <c r="D26" t="s">
+        <v>270</v>
+      </c>
+      <c r="E26" t="s">
+        <v>275</v>
+      </c>
+      <c r="F26" t="s">
+        <v>281</v>
+      </c>
+      <c r="G26" t="s">
         <v>286</v>
       </c>
-      <c r="D26" t="s">
-        <v>281</v>
-      </c>
-      <c r="E26" t="s">
-        <v>276</v>
-      </c>
-      <c r="F26" t="s">
-        <v>266</v>
-      </c>
-      <c r="G26" t="s">
-        <v>271</v>
-      </c>
-      <c r="L26" s="8" t="s">
-        <v>103</v>
+      <c r="H26" t="s">
+        <v>291</v>
+      </c>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="16">
       <c r="A27" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C27" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E27" t="s">
+        <v>276</v>
+      </c>
+      <c r="F27" t="s">
         <v>282</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="E27" t="s">
-        <v>277</v>
-      </c>
-      <c r="F27" t="s">
-        <v>267</v>
-      </c>
       <c r="G27" t="s">
-        <v>272</v>
+        <v>287</v>
+      </c>
+      <c r="H27" t="s">
+        <v>292</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="16">
       <c r="A28" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C28" t="s">
-        <v>287</v>
-      </c>
-      <c r="D28" t="s">
+        <v>258</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="E28" t="s">
-        <v>278</v>
-      </c>
-      <c r="F28" t="s">
-        <v>268</v>
-      </c>
       <c r="G28" s="7" t="s">
-        <v>273</v>
+        <v>288</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>293</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="16">
       <c r="A29" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>269</v>
-      </c>
       <c r="G29" t="s">
-        <v>274</v>
+        <v>289</v>
+      </c>
+      <c r="H29" t="s">
+        <v>294</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="16">
       <c r="A30" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="C30" t="s">
-        <v>289</v>
-      </c>
-      <c r="D30" t="s">
+        <v>260</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E30" t="s">
+        <v>279</v>
+      </c>
+      <c r="F30" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="E30" t="s">
+      <c r="G30" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="M30" s="8" t="s">
         <v>280</v>
-      </c>
-      <c r="F30" t="s">
-        <v>270</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2431,7 +2521,7 @@
         <v>31</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2567,7 +2657,7 @@
         <v>315360000</v>
       </c>
       <c r="H13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2583,30 +2673,30 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B15" t="s">
         <v>229</v>
-      </c>
-      <c r="B15" t="s">
-        <v>230</v>
       </c>
       <c r="C15">
         <v>229410</v>
       </c>
       <c r="H15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C16">
         <v>91880</v>
       </c>
       <c r="H16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2674,7 +2764,7 @@
         <v>66</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2726,37 +2816,37 @@
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2767,7 +2857,7 @@
         <v>69</v>
       </c>
       <c r="N4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2778,7 +2868,7 @@
         <v>71</v>
       </c>
       <c r="N5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2789,7 +2879,7 @@
         <v>73</v>
       </c>
       <c r="N6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -2800,7 +2890,7 @@
         <v>75</v>
       </c>
       <c r="N7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -2813,7 +2903,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" t="s">
         <v>78</v>
@@ -2869,7 +2959,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Correction of an error for methane heat capacity parameter d
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -863,9 +863,6 @@
     <t>-3.3692e-6</t>
   </si>
   <si>
-    <t>5.3496e-3</t>
-  </si>
-  <si>
     <t>3.1552e-14</t>
   </si>
   <si>
@@ -915,6 +912,9 @@
   </si>
   <si>
     <t>-9.7989e-15</t>
+  </si>
+  <si>
+    <t>5.3496e-10</t>
   </si>
 </sst>
 </file>
@@ -1468,7 +1468,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:H30"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2333,17 +2333,17 @@
         <v>275</v>
       </c>
       <c r="F26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L26" s="8"/>
       <c r="M26" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="16">
@@ -2363,19 +2363,19 @@
         <v>276</v>
       </c>
       <c r="F27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>261</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="16">
@@ -2395,19 +2395,19 @@
         <v>277</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>262</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="16">
@@ -2424,22 +2424,22 @@
         <v>273</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L29" s="8" t="s">
         <v>263</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="16">
@@ -2456,22 +2456,22 @@
         <v>274</v>
       </c>
       <c r="E30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>264</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Critical pressure, temperature and molar volume added
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="322">
   <si>
     <t>parvariable</t>
   </si>
@@ -915,6 +915,84 @@
   </si>
   <si>
     <t>5.3496e-10</t>
+  </si>
+  <si>
+    <t>Critical temperature</t>
+  </si>
+  <si>
+    <t>Tc</t>
+  </si>
+  <si>
+    <t>Critical pressure</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>190.56</t>
+  </si>
+  <si>
+    <t>4.60e6</t>
+  </si>
+  <si>
+    <t>Critical molar volume</t>
+  </si>
+  <si>
+    <t>Vmc</t>
+  </si>
+  <si>
+    <t>m3.mol-1</t>
+  </si>
+  <si>
+    <t>9.9e-5</t>
+  </si>
+  <si>
+    <t>32.94</t>
+  </si>
+  <si>
+    <t>1.2858e6</t>
+  </si>
+  <si>
+    <t>6.5e-5</t>
+  </si>
+  <si>
+    <t>405.56</t>
+  </si>
+  <si>
+    <t>11.357e6</t>
+  </si>
+  <si>
+    <t>6.98e-5</t>
+  </si>
+  <si>
+    <t>126.19</t>
+  </si>
+  <si>
+    <t>3.3958e6</t>
+  </si>
+  <si>
+    <t>9.0e-5</t>
+  </si>
+  <si>
+    <t>647.10</t>
+  </si>
+  <si>
+    <t>22.06e6</t>
+  </si>
+  <si>
+    <t>5.6e-5</t>
+  </si>
+  <si>
+    <t>456.66</t>
+  </si>
+  <si>
+    <t>CRC, Lange(HCN)</t>
+  </si>
+  <si>
+    <t>5.3905e6</t>
+  </si>
+  <si>
+    <t>1.39e-4</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1535,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1465,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2472,6 +2550,102 @@
       </c>
       <c r="M30" s="8" t="s">
         <v>279</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="16">
+      <c r="A31" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="C31" t="s">
+        <v>315</v>
+      </c>
+      <c r="D31" t="s">
+        <v>312</v>
+      </c>
+      <c r="E31" t="s">
+        <v>300</v>
+      </c>
+      <c r="F31" t="s">
+        <v>309</v>
+      </c>
+      <c r="G31" t="s">
+        <v>306</v>
+      </c>
+      <c r="H31" t="s">
+        <v>318</v>
+      </c>
+      <c r="L31" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="M31" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="16">
+      <c r="A32" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C32" t="s">
+        <v>316</v>
+      </c>
+      <c r="D32" t="s">
+        <v>313</v>
+      </c>
+      <c r="E32" t="s">
+        <v>301</v>
+      </c>
+      <c r="F32" t="s">
+        <v>310</v>
+      </c>
+      <c r="G32" t="s">
+        <v>307</v>
+      </c>
+      <c r="H32" t="s">
+        <v>320</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="M32" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="16">
+      <c r="A33" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C33" t="s">
+        <v>317</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E33" t="s">
+        <v>305</v>
+      </c>
+      <c r="F33" t="s">
+        <v>311</v>
+      </c>
+      <c r="G33" t="s">
+        <v>308</v>
+      </c>
+      <c r="H33" t="s">
+        <v>321</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="M33" s="8" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Molar fraction of nitrogen added
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,33 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mithu/CS/MatlabWD/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16343C7-9D07-6E4D-976E-62AF13D23F41}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="324">
   <si>
     <t>parvariable</t>
   </si>
@@ -993,13 +999,19 @@
   </si>
   <si>
     <t>1.39e-4</t>
+  </si>
+  <si>
+    <t>Gas molar fraction nitrogen</t>
+  </si>
+  <si>
+    <t>yN2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1171,67 +1183,67 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="61">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1535,21 +1547,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="31" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -1602,7 +1614,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1638,7 +1650,7 @@
       </c>
       <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:13" ht="16">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1674,7 +1686,7 @@
       </c>
       <c r="L3" s="8"/>
     </row>
-    <row r="4" spans="1:13" ht="16">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -1708,7 +1720,7 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:13" ht="16">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>167</v>
       </c>
@@ -1747,7 +1759,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="16">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>139</v>
       </c>
@@ -1782,7 +1794,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="16">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>132</v>
       </c>
@@ -1817,7 +1829,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>140</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="16">
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>146</v>
       </c>
@@ -1887,7 +1899,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>141</v>
       </c>
@@ -1922,7 +1934,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="16">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>147</v>
       </c>
@@ -1957,7 +1969,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="16">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1996,7 +2008,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="16">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2014,7 +2026,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="1:13" ht="16">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>105</v>
       </c>
@@ -2053,7 +2065,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="16">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>121</v>
       </c>
@@ -2090,7 +2102,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="16">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>192</v>
       </c>
@@ -2121,7 +2133,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="16">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>155</v>
       </c>
@@ -2132,7 +2144,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="16">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>190</v>
       </c>
@@ -2146,7 +2158,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16">
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>208</v>
       </c>
@@ -2184,7 +2196,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16">
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>209</v>
       </c>
@@ -2222,7 +2234,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="16">
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>212</v>
       </c>
@@ -2260,7 +2272,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="16">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>219</v>
       </c>
@@ -2295,7 +2307,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="16">
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>220</v>
       </c>
@@ -2330,7 +2342,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="16">
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>233</v>
       </c>
@@ -2362,7 +2374,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="16">
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>235</v>
       </c>
@@ -2394,7 +2406,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="16">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>251</v>
       </c>
@@ -2424,7 +2436,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="16">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>253</v>
       </c>
@@ -2456,7 +2468,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="16">
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>254</v>
       </c>
@@ -2488,7 +2500,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16">
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>255</v>
       </c>
@@ -2520,7 +2532,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="16">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>256</v>
       </c>
@@ -2552,7 +2564,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="16">
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
         <v>296</v>
       </c>
@@ -2584,7 +2596,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="16">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>298</v>
       </c>
@@ -2616,7 +2628,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="16">
+    <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
         <v>302</v>
       </c>
@@ -2660,14 +2672,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -2885,14 +2897,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>
@@ -3177,6 +3189,14 @@
       </c>
       <c r="B21" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B22" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor Data Changes, Reactor Optimizer integrated in MAIN
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,33 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721DAEB4-6B31-684F-AC64-E31B9D20EA9D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28460" windowHeight="17100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="405">
   <si>
     <t>parvariable</t>
   </si>
@@ -1239,13 +1245,16 @@
   </si>
   <si>
     <t>2.9675</t>
+  </si>
+  <si>
+    <t>Ideal Gas Constant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1443,92 +1452,92 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="87">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1833,21 +1842,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
@@ -1901,7 +1910,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1937,7 +1946,7 @@
       </c>
       <c r="L2" s="8"/>
     </row>
-    <row r="3" spans="1:13" ht="16">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1973,7 +1982,7 @@
       </c>
       <c r="L3" s="8"/>
     </row>
-    <row r="4" spans="1:13" ht="16">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -2007,7 +2016,7 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
-    <row r="5" spans="1:13" ht="16">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>167</v>
       </c>
@@ -2046,7 +2055,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="16">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>139</v>
       </c>
@@ -2081,7 +2090,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="16">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>132</v>
       </c>
@@ -2116,7 +2125,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>140</v>
       </c>
@@ -2151,7 +2160,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="16">
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>146</v>
       </c>
@@ -2186,7 +2195,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>141</v>
       </c>
@@ -2221,7 +2230,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="16">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>147</v>
       </c>
@@ -2256,7 +2265,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="16">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -2295,7 +2304,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="16">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2313,7 +2322,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="1:13" ht="16">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>105</v>
       </c>
@@ -2352,7 +2361,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="16">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>121</v>
       </c>
@@ -2389,7 +2398,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="16">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>192</v>
       </c>
@@ -2420,7 +2429,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="16">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>155</v>
       </c>
@@ -2431,7 +2440,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="16">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>190</v>
       </c>
@@ -2445,7 +2454,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16">
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>208</v>
       </c>
@@ -2483,7 +2492,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16">
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>209</v>
       </c>
@@ -2521,7 +2530,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="16">
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>212</v>
       </c>
@@ -2559,7 +2568,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="16">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>219</v>
       </c>
@@ -2594,7 +2603,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="16">
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>220</v>
       </c>
@@ -2629,7 +2638,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="16">
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>233</v>
       </c>
@@ -2661,7 +2670,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="16">
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>235</v>
       </c>
@@ -2693,7 +2702,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="16">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>286</v>
       </c>
@@ -2725,7 +2734,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="16">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>288</v>
       </c>
@@ -2757,7 +2766,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="16">
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>292</v>
       </c>
@@ -2789,7 +2798,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16">
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>314</v>
       </c>
@@ -2815,7 +2824,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="16">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>334</v>
       </c>
@@ -2845,7 +2854,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="16">
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
         <v>335</v>
       </c>
@@ -2877,7 +2886,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="16">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>332</v>
       </c>
@@ -2909,7 +2918,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="16">
+    <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
         <v>333</v>
       </c>
@@ -2941,7 +2950,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="16">
+    <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
         <v>336</v>
       </c>
@@ -2973,7 +2982,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="16">
+    <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
         <v>342</v>
       </c>
@@ -3005,7 +3014,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="16">
+    <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
         <v>343</v>
       </c>
@@ -3034,7 +3043,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="16">
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
         <v>339</v>
       </c>
@@ -3063,7 +3072,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="16">
+    <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
         <v>340</v>
       </c>
@@ -3095,7 +3104,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="16">
+    <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
         <v>337</v>
       </c>
@@ -3127,7 +3136,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="16">
+    <row r="40" spans="1:13">
       <c r="A40" s="1" t="s">
         <v>338</v>
       </c>
@@ -3159,7 +3168,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="16">
+    <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
         <v>341</v>
       </c>
@@ -3191,7 +3200,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="16">
+    <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
         <v>346</v>
       </c>
@@ -3223,7 +3232,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="16">
+    <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
         <v>347</v>
       </c>
@@ -3264,14 +3273,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -3475,6 +3484,17 @@
       </c>
       <c r="H16" t="s">
         <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G17">
+        <v>8.3140000000000001</v>
+      </c>
+      <c r="H17" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -3489,14 +3509,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Ideal Gas Constant added
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721DAEB4-6B31-684F-AC64-E31B9D20EA9D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F57C8C-D20E-CB47-A5C6-419DC219113D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28460" windowHeight="17100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="406">
   <si>
     <t>parvariable</t>
   </si>
@@ -1248,6 +1248,9 @@
   </si>
   <si>
     <t>Ideal Gas Constant</t>
+  </si>
+  <si>
+    <t>idgc</t>
   </si>
 </sst>
 </file>
@@ -3277,7 +3280,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3489,6 +3492,9 @@
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>404</v>
+      </c>
+      <c r="B17" t="s">
+        <v>405</v>
       </c>
       <c r="G17">
         <v>8.3140000000000001</v>

</xml_diff>

<commit_message>
Change For Parser, Two Last Columns of each sheet get deleted
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F57C8C-D20E-CB47-A5C6-419DC219113D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4484D76-94F3-984C-8926-0705D5B84C92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28460" windowHeight="17100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28460" windowHeight="17100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="407">
   <si>
     <t>parvariable</t>
   </si>
@@ -1251,6 +1251,9 @@
   </si>
   <si>
     <t>idgc</t>
+  </si>
+  <si>
+    <t>Dummy</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1602,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1651,7 +1654,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3277,10 +3280,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3288,7 +3291,7 @@
     <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3313,8 +3316,11 @@
       <c r="H1" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -3337,7 +3343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -3360,7 +3366,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -3368,7 +3374,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -3376,7 +3382,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -3384,7 +3390,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -3392,7 +3398,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -3401,7 +3407,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -3410,7 +3416,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -3418,7 +3424,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -3427,7 +3433,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -3435,7 +3441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -3450,7 +3456,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -3461,7 +3467,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>228</v>
       </c>
@@ -3475,7 +3481,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>231</v>
       </c>
@@ -3516,10 +3522,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3527,7 +3533,7 @@
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -3570,8 +3576,11 @@
       <c r="N1" s="5" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="5" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -3612,7 +3621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="5" t="s">
         <v>67</v>
       </c>
@@ -3653,7 +3662,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -3664,7 +3673,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
@@ -3675,18 +3684,21 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B6" t="s">
         <v>73</v>
       </c>
+      <c r="C6">
+        <v>500000</v>
+      </c>
       <c r="N6" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -3697,7 +3709,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -3705,7 +3717,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>164</v>
       </c>
@@ -3713,7 +3725,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
         <v>79</v>
       </c>
@@ -3721,7 +3733,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
@@ -3729,7 +3741,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" s="5" t="s">
         <v>83</v>
       </c>
@@ -3737,7 +3749,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -3745,7 +3757,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" s="5" t="s">
         <v>87</v>
       </c>
@@ -3753,7 +3765,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
         <v>89</v>
       </c>
@@ -3761,7 +3773,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
         <v>165</v>
       </c>

</xml_diff>

<commit_message>
Stream Table has no some FOOOOO Data
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4484D76-94F3-984C-8926-0705D5B84C92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83211E20-2427-C047-84EC-6F5AD273B9DF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28460" windowHeight="17100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3525,7 +3525,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3669,6 +3669,39 @@
       <c r="B4" t="s">
         <v>69</v>
       </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
       <c r="N4" t="s">
         <v>188</v>
       </c>
@@ -3680,6 +3713,39 @@
       <c r="B5" t="s">
         <v>71</v>
       </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
       <c r="N5" t="s">
         <v>188</v>
       </c>
@@ -3694,6 +3760,36 @@
       <c r="C6">
         <v>500000</v>
       </c>
+      <c r="D6">
+        <v>500000</v>
+      </c>
+      <c r="E6">
+        <v>500000</v>
+      </c>
+      <c r="F6">
+        <v>500000</v>
+      </c>
+      <c r="G6">
+        <v>500000</v>
+      </c>
+      <c r="H6">
+        <v>500000</v>
+      </c>
+      <c r="I6">
+        <v>500000</v>
+      </c>
+      <c r="J6">
+        <v>500000</v>
+      </c>
+      <c r="K6">
+        <v>500000</v>
+      </c>
+      <c r="L6">
+        <v>500000</v>
+      </c>
+      <c r="M6">
+        <v>500000</v>
+      </c>
       <c r="N6" t="s">
         <v>189</v>
       </c>
@@ -3705,6 +3801,39 @@
       <c r="B7" t="s">
         <v>75</v>
       </c>
+      <c r="C7">
+        <v>370</v>
+      </c>
+      <c r="D7">
+        <v>370</v>
+      </c>
+      <c r="E7">
+        <v>370</v>
+      </c>
+      <c r="F7">
+        <v>370</v>
+      </c>
+      <c r="G7">
+        <v>370</v>
+      </c>
+      <c r="H7">
+        <v>370</v>
+      </c>
+      <c r="I7">
+        <v>370</v>
+      </c>
+      <c r="J7">
+        <v>370</v>
+      </c>
+      <c r="K7">
+        <v>370</v>
+      </c>
+      <c r="L7">
+        <v>370</v>
+      </c>
+      <c r="M7">
+        <v>370</v>
+      </c>
       <c r="N7" t="s">
         <v>111</v>
       </c>
@@ -3716,6 +3845,39 @@
       <c r="B8" t="s">
         <v>77</v>
       </c>
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+      <c r="F8">
+        <v>0.1</v>
+      </c>
+      <c r="G8">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>0.1</v>
+      </c>
+      <c r="I8">
+        <v>0.1</v>
+      </c>
+      <c r="J8">
+        <v>0.1</v>
+      </c>
+      <c r="K8">
+        <v>0.1</v>
+      </c>
+      <c r="L8">
+        <v>0.1</v>
+      </c>
+      <c r="M8">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
@@ -3724,6 +3886,39 @@
       <c r="B9" t="s">
         <v>78</v>
       </c>
+      <c r="C9">
+        <v>0.2</v>
+      </c>
+      <c r="D9">
+        <v>0.2</v>
+      </c>
+      <c r="E9">
+        <v>0.2</v>
+      </c>
+      <c r="F9">
+        <v>0.2</v>
+      </c>
+      <c r="G9">
+        <v>0.2</v>
+      </c>
+      <c r="H9">
+        <v>0.2</v>
+      </c>
+      <c r="I9">
+        <v>0.2</v>
+      </c>
+      <c r="J9">
+        <v>0.2</v>
+      </c>
+      <c r="K9">
+        <v>0.2</v>
+      </c>
+      <c r="L9">
+        <v>0.2</v>
+      </c>
+      <c r="M9">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
@@ -3732,6 +3927,39 @@
       <c r="B10" t="s">
         <v>80</v>
       </c>
+      <c r="C10">
+        <v>0.3</v>
+      </c>
+      <c r="D10">
+        <v>0.3</v>
+      </c>
+      <c r="E10">
+        <v>0.3</v>
+      </c>
+      <c r="F10">
+        <v>0.3</v>
+      </c>
+      <c r="G10">
+        <v>0.3</v>
+      </c>
+      <c r="H10">
+        <v>0.3</v>
+      </c>
+      <c r="I10">
+        <v>0.3</v>
+      </c>
+      <c r="J10">
+        <v>0.3</v>
+      </c>
+      <c r="K10">
+        <v>0.3</v>
+      </c>
+      <c r="L10">
+        <v>0.3</v>
+      </c>
+      <c r="M10">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="5" t="s">
@@ -3740,6 +3968,39 @@
       <c r="B11" t="s">
         <v>82</v>
       </c>
+      <c r="C11">
+        <v>0.4</v>
+      </c>
+      <c r="D11">
+        <v>0.4</v>
+      </c>
+      <c r="E11">
+        <v>0.4</v>
+      </c>
+      <c r="F11">
+        <v>0.4</v>
+      </c>
+      <c r="G11">
+        <v>0.4</v>
+      </c>
+      <c r="H11">
+        <v>0.4</v>
+      </c>
+      <c r="I11">
+        <v>0.4</v>
+      </c>
+      <c r="J11">
+        <v>0.4</v>
+      </c>
+      <c r="K11">
+        <v>0.4</v>
+      </c>
+      <c r="L11">
+        <v>0.4</v>
+      </c>
+      <c r="M11">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="5" t="s">
@@ -3748,6 +4009,39 @@
       <c r="B12" t="s">
         <v>84</v>
       </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="5" t="s">
@@ -3756,6 +4050,39 @@
       <c r="B13" t="s">
         <v>86</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="5" t="s">
@@ -3764,6 +4091,39 @@
       <c r="B14" t="s">
         <v>88</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
@@ -3772,6 +4132,39 @@
       <c r="B15" t="s">
         <v>95</v>
       </c>
+      <c r="C15">
+        <v>0.1</v>
+      </c>
+      <c r="D15">
+        <v>0.1</v>
+      </c>
+      <c r="E15">
+        <v>0.1</v>
+      </c>
+      <c r="F15">
+        <v>0.1</v>
+      </c>
+      <c r="G15">
+        <v>0.1</v>
+      </c>
+      <c r="H15">
+        <v>0.1</v>
+      </c>
+      <c r="I15">
+        <v>0.1</v>
+      </c>
+      <c r="J15">
+        <v>0.1</v>
+      </c>
+      <c r="K15">
+        <v>0.1</v>
+      </c>
+      <c r="L15">
+        <v>0.1</v>
+      </c>
+      <c r="M15">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
@@ -3780,53 +4173,284 @@
       <c r="B16" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <v>0.2</v>
+      </c>
+      <c r="D16">
+        <v>0.2</v>
+      </c>
+      <c r="E16">
+        <v>0.2</v>
+      </c>
+      <c r="F16">
+        <v>0.2</v>
+      </c>
+      <c r="G16">
+        <v>0.2</v>
+      </c>
+      <c r="H16">
+        <v>0.2</v>
+      </c>
+      <c r="I16">
+        <v>0.2</v>
+      </c>
+      <c r="J16">
+        <v>0.2</v>
+      </c>
+      <c r="K16">
+        <v>0.2</v>
+      </c>
+      <c r="L16">
+        <v>0.2</v>
+      </c>
+      <c r="M16">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B17" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <v>0.3</v>
+      </c>
+      <c r="D17">
+        <v>0.3</v>
+      </c>
+      <c r="E17">
+        <v>0.3</v>
+      </c>
+      <c r="F17">
+        <v>0.3</v>
+      </c>
+      <c r="G17">
+        <v>0.3</v>
+      </c>
+      <c r="H17">
+        <v>0.3</v>
+      </c>
+      <c r="I17">
+        <v>0.3</v>
+      </c>
+      <c r="J17">
+        <v>0.3</v>
+      </c>
+      <c r="K17">
+        <v>0.3</v>
+      </c>
+      <c r="L17">
+        <v>0.3</v>
+      </c>
+      <c r="M17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="5" t="s">
         <v>94</v>
       </c>
       <c r="B18" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <v>0.4</v>
+      </c>
+      <c r="D18">
+        <v>0.4</v>
+      </c>
+      <c r="E18">
+        <v>0.4</v>
+      </c>
+      <c r="F18">
+        <v>0.4</v>
+      </c>
+      <c r="G18">
+        <v>0.4</v>
+      </c>
+      <c r="H18">
+        <v>0.4</v>
+      </c>
+      <c r="I18">
+        <v>0.4</v>
+      </c>
+      <c r="J18">
+        <v>0.4</v>
+      </c>
+      <c r="K18">
+        <v>0.4</v>
+      </c>
+      <c r="L18">
+        <v>0.4</v>
+      </c>
+      <c r="M18">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B19" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B20" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="5" t="s">
         <v>93</v>
       </c>
       <c r="B21" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="5" t="s">
         <v>312</v>
       </c>
       <c r="B22" t="s">
         <v>313</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Henry's constants for calculation
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="234">
   <si>
     <t>parvariable</t>
   </si>
@@ -717,6 +717,18 @@
   </si>
   <si>
     <t>Dummy</t>
+  </si>
+  <si>
+    <t>Henry's calculation std. conditions solubility constant</t>
+  </si>
+  <si>
+    <t>kHstd</t>
+  </si>
+  <si>
+    <t>Henry's calculation deltaHsol/R</t>
+  </si>
+  <si>
+    <t>deltaHsolR</t>
   </si>
 </sst>
 </file>
@@ -1324,19 +1336,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
@@ -2801,6 +2813,58 @@
       <c r="M42" s="7" t="s">
         <v>185</v>
       </c>
+    </row>
+    <row r="43" spans="1:13" ht="16">
+      <c r="A43" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13">
+        <v>6.4999999999999997E-4</v>
+      </c>
+      <c r="E43" s="13">
+        <v>1.4E-3</v>
+      </c>
+      <c r="F43" s="13">
+        <v>61</v>
+      </c>
+      <c r="G43" s="13">
+        <v>7.7999999999999999E-4</v>
+      </c>
+      <c r="H43" s="13">
+        <v>12</v>
+      </c>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+    </row>
+    <row r="44" spans="1:13" ht="16">
+      <c r="A44" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13">
+        <v>1300</v>
+      </c>
+      <c r="E44" s="13">
+        <v>1600</v>
+      </c>
+      <c r="F44" s="13">
+        <v>4200</v>
+      </c>
+      <c r="G44" s="13">
+        <v>500</v>
+      </c>
+      <c r="H44" s="13">
+        <v>5000</v>
+      </c>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3059,7 +3123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor change: unit of two last parameters added
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="235">
   <si>
     <t>parvariable</t>
   </si>
@@ -729,6 +729,9 @@
   </si>
   <si>
     <t>deltaHsolR</t>
+  </si>
+  <si>
+    <t>M.atm-1</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1354,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2851,6 +2854,9 @@
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
+      <c r="L43" s="7" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="44" spans="1:13" ht="16">
       <c r="A44" s="1" t="s">
@@ -2877,6 +2883,9 @@
       </c>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
+      <c r="L44" s="7" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implementation of hcn_distillation into main
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clemens/CS/MatlabWD/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="239">
   <si>
     <t>parvariable</t>
   </si>
@@ -732,6 +737,18 @@
   </si>
   <si>
     <t>M.atm-1</t>
+  </si>
+  <si>
+    <t>Liquid molar fraction water</t>
+  </si>
+  <si>
+    <t>xH2O</t>
+  </si>
+  <si>
+    <t>Gas molar fraction water</t>
+  </si>
+  <si>
+    <t>yH2O</t>
   </si>
 </sst>
 </file>
@@ -947,99 +964,99 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="93">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1343,7 +1360,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1353,11 +1370,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
@@ -1372,7 +1389,7 @@
     <col min="13" max="13" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1413,7 +1430,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1449,7 +1466,7 @@
       </c>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="16">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1485,7 +1502,7 @@
       </c>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:13" ht="16">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -1519,7 +1536,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:13" ht="16">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -1558,7 +1575,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="16">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
@@ -1593,7 +1610,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="16">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
@@ -1628,7 +1645,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -1663,7 +1680,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="16">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -1698,7 +1715,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -1733,7 +1750,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="16">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>127</v>
       </c>
@@ -1768,7 +1785,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="16">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1807,7 +1824,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="16">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1825,7 +1842,7 @@
       <c r="K13" s="9"/>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="1:13" ht="16">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -1864,7 +1881,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="16">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>110</v>
       </c>
@@ -1901,7 +1918,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="16">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>143</v>
       </c>
@@ -1932,7 +1949,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="16">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>141</v>
       </c>
@@ -1954,7 +1971,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="16">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
@@ -1993,7 +2010,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>159</v>
       </c>
@@ -2032,7 +2049,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="16">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>162</v>
       </c>
@@ -2071,7 +2088,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="16">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>168</v>
       </c>
@@ -2108,7 +2125,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="16">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>169</v>
       </c>
@@ -2145,7 +2162,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="16">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>175</v>
       </c>
@@ -2180,7 +2197,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="16">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>177</v>
       </c>
@@ -2215,7 +2232,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="16">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>186</v>
       </c>
@@ -2250,7 +2267,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="16">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>188</v>
       </c>
@@ -2285,7 +2302,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="16">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>190</v>
       </c>
@@ -2320,7 +2337,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="16">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>196</v>
       </c>
@@ -2350,7 +2367,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>211</v>
       </c>
@@ -2383,7 +2400,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="16">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>212</v>
       </c>
@@ -2418,7 +2435,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="16">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>209</v>
       </c>
@@ -2453,7 +2470,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="16">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>210</v>
       </c>
@@ -2488,7 +2505,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="16">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>213</v>
       </c>
@@ -2523,7 +2540,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="16">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>219</v>
       </c>
@@ -2558,7 +2575,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="16">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>220</v>
       </c>
@@ -2590,7 +2607,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="16">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>216</v>
       </c>
@@ -2622,7 +2639,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="16">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>217</v>
       </c>
@@ -2657,7 +2674,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="16">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>214</v>
       </c>
@@ -2692,7 +2709,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="16">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>215</v>
       </c>
@@ -2727,7 +2744,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="16">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>218</v>
       </c>
@@ -2762,7 +2779,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="16">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>223</v>
       </c>
@@ -2797,7 +2814,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="16">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>224</v>
       </c>
@@ -2829,7 +2846,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="16">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>230</v>
       </c>
@@ -2858,7 +2875,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="16">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>232</v>
       </c>
@@ -2890,11 +2907,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2906,12 +2918,12 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2940,7 +2952,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -2963,7 +2975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -2986,7 +2998,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -2994,7 +3006,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -3002,7 +3014,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -3010,7 +3022,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -3018,7 +3030,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -3027,7 +3039,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -3036,7 +3048,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -3044,7 +3056,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -3053,7 +3065,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -3061,7 +3073,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -3076,7 +3088,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -3087,7 +3099,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>170</v>
       </c>
@@ -3101,7 +3113,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>173</v>
       </c>
@@ -3115,7 +3127,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>227</v>
       </c>
@@ -3132,28 +3144,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -3200,7 +3207,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -3241,7 +3248,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>67</v>
       </c>
@@ -3282,7 +3289,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -3326,7 +3333,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
@@ -3370,7 +3377,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -3401,11 +3408,11 @@
       <c r="J6">
         <v>500000</v>
       </c>
-      <c r="K6">
-        <v>500000</v>
-      </c>
-      <c r="L6">
-        <v>500000</v>
+      <c r="K6" s="3">
+        <v>100000</v>
+      </c>
+      <c r="L6" s="3">
+        <v>100000</v>
       </c>
       <c r="M6">
         <v>500000</v>
@@ -3414,7 +3421,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -3458,7 +3465,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -3499,7 +3506,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>131</v>
       </c>
@@ -3540,7 +3547,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>79</v>
       </c>
@@ -3581,7 +3588,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
@@ -3622,7 +3629,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>83</v>
       </c>
@@ -3663,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -3704,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>87</v>
       </c>
@@ -3745,341 +3752,418 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15" t="s">
+        <v>236</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>95</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>0.1</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>0.1</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>0.1</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>0.1</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>0.1</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>0.1</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <v>0.1</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <v>0.1</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>0.1</v>
       </c>
-      <c r="L15">
+      <c r="L16">
         <v>0.1</v>
       </c>
-      <c r="M15">
+      <c r="M16">
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>96</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>0.2</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>0.2</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>0.2</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>0.2</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>0.2</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>0.2</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>0.2</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>0.2</v>
       </c>
-      <c r="K16">
+      <c r="K17">
         <v>0.2</v>
       </c>
-      <c r="L16">
+      <c r="L17">
         <v>0.2</v>
       </c>
-      <c r="M16">
+      <c r="M17">
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>97</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>0.3</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>0.3</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>0.3</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>0.3</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>0.3</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>0.3</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>0.3</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>0.3</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>0.3</v>
       </c>
-      <c r="L17">
+      <c r="L18">
         <v>0.3</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>98</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>0.4</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>0.4</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>0.4</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>0.4</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>0.4</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>0.4</v>
       </c>
-      <c r="I18">
+      <c r="I19">
         <v>0.4</v>
       </c>
-      <c r="J18">
+      <c r="J19">
         <v>0.4</v>
       </c>
-      <c r="K18">
+      <c r="K19">
         <v>0.4</v>
       </c>
-      <c r="L18">
+      <c r="L19">
         <v>0.4</v>
       </c>
-      <c r="M18">
+      <c r="M19">
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>99</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="5" t="s">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>100</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="5" t="s">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>101</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="5" t="s">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>195</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B24" t="s">
+        <v>238</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mole fractions for H2O in Data.xlsx fixed implementation of hcn_distillation into main
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1370,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3152,7 +3152,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3497,7 +3497,7 @@
         <v>0.1</v>
       </c>
       <c r="K8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <v>0.1</v>
@@ -3538,7 +3538,7 @@
         <v>0.2</v>
       </c>
       <c r="K9">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <v>0.2</v>
@@ -3579,7 +3579,7 @@
         <v>0.3</v>
       </c>
       <c r="K10">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>0.3</v>
@@ -3620,7 +3620,7 @@
         <v>0.4</v>
       </c>
       <c r="K11">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>0.4</v>
@@ -3661,7 +3661,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -3784,7 +3784,7 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -3825,7 +3825,7 @@
         <v>0.1</v>
       </c>
       <c r="K16">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <v>0.1</v>
@@ -3866,7 +3866,7 @@
         <v>0.2</v>
       </c>
       <c r="K17">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <v>0.2</v>
@@ -3907,7 +3907,7 @@
         <v>0.3</v>
       </c>
       <c r="K18">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <v>0.3</v>
@@ -3948,7 +3948,7 @@
         <v>0.4</v>
       </c>
       <c r="K19">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="L19">
         <v>0.4</v>

</xml_diff>

<commit_message>
Excel Updated, Peng Bug ix
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clemens/CS/MatlabWD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F32772-62C6-FF43-A9A2-64EECAB4E51D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -628,9 +629,6 @@
     <t>omega</t>
   </si>
   <si>
-    <t>Poling</t>
-  </si>
-  <si>
     <t>a1_hcparhigh</t>
   </si>
   <si>
@@ -749,16 +747,19 @@
   </si>
   <si>
     <t>yH2O</t>
+  </si>
+  <si>
+    <t>Poling/Koretsky</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -964,52 +965,52 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="93">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1056,7 +1057,7 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1367,14 +1368,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
@@ -1389,7 +1390,7 @@
     <col min="13" max="13" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1430,7 +1431,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1466,7 +1467,7 @@
       </c>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1502,7 +1503,7 @@
       </c>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -1536,7 +1537,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
@@ -1610,7 +1611,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
@@ -1645,7 +1646,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -1715,7 +1716,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -1750,7 +1751,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>127</v>
       </c>
@@ -1785,7 +1786,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1824,7 +1825,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1842,7 +1843,7 @@
       <c r="K13" s="9"/>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -1881,7 +1882,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>110</v>
       </c>
@@ -1918,7 +1919,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>143</v>
       </c>
@@ -1949,7 +1950,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>141</v>
       </c>
@@ -1971,7 +1972,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
@@ -2010,7 +2011,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>159</v>
       </c>
@@ -2049,7 +2050,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>162</v>
       </c>
@@ -2088,7 +2089,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>168</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>169</v>
       </c>
@@ -2162,7 +2163,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>175</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>177</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>186</v>
       </c>
@@ -2267,7 +2268,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>188</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>190</v>
       </c>
@@ -2337,7 +2338,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>196</v>
       </c>
@@ -2359,20 +2360,22 @@
       <c r="G28" s="14">
         <v>-0.216</v>
       </c>
-      <c r="H28" s="13"/>
+      <c r="H28" s="13">
+        <v>0.40699999999999997</v>
+      </c>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
       <c r="M28" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C29" s="13">
         <v>2.677</v>
@@ -2400,12 +2403,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C30" s="14">
         <v>2.9732000000000001E-3</v>
@@ -2435,12 +2438,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C31" s="14">
         <v>-7.7377000000000003E-7</v>
@@ -2470,12 +2473,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C32" s="14">
         <v>9.4433999999999999E-11</v>
@@ -2505,12 +2508,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C33" s="14">
         <v>-4.2689999999999998E-15</v>
@@ -2540,12 +2543,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C34" s="14">
         <v>-29886</v>
@@ -2575,12 +2578,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C35" s="13">
         <v>6.8826000000000001</v>
@@ -2607,12 +2610,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C36" s="13">
         <v>4.1985999999999999</v>
@@ -2639,12 +2642,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C37" s="14">
         <v>-2.0363999999999998E-3</v>
@@ -2674,12 +2677,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C38" s="13">
         <v>6.5204000000000003E-6</v>
@@ -2709,12 +2712,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C39" s="14">
         <v>-5.4880000000000001E-9</v>
@@ -2744,12 +2747,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13">
       <c r="A40" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C40" s="13">
         <v>1.7719999999999999E-12</v>
@@ -2779,12 +2782,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C41" s="14">
         <v>-30294</v>
@@ -2814,12 +2817,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C42" s="14">
         <v>-0.84902999999999995</v>
@@ -2846,12 +2849,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="13">
@@ -2872,15 +2875,15 @@
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
       <c r="L43" s="7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>232</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>233</v>
       </c>
       <c r="C44" s="13"/>
       <c r="D44" s="13">
@@ -2911,19 +2914,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2952,7 +2955,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -2975,7 +2978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -2998,7 +3001,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -3006,7 +3009,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -3014,7 +3017,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -3022,7 +3025,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -3030,7 +3033,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -3039,7 +3042,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -3048,7 +3051,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -3056,7 +3059,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -3065,7 +3068,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -3073,7 +3076,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -3088,7 +3091,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -3099,7 +3102,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>170</v>
       </c>
@@ -3113,7 +3116,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>173</v>
       </c>
@@ -3127,12 +3130,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B17" t="s">
         <v>227</v>
-      </c>
-      <c r="B17" t="s">
-        <v>228</v>
       </c>
       <c r="G17">
         <v>8.3140000000000001</v>
@@ -3148,19 +3151,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -3204,10 +3207,10 @@
         <v>138</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -3248,7 +3251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" s="5" t="s">
         <v>67</v>
       </c>
@@ -3289,7 +3292,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -3333,7 +3336,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -3421,7 +3424,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -3465,7 +3468,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -3506,7 +3509,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>131</v>
       </c>
@@ -3547,7 +3550,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
         <v>79</v>
       </c>
@@ -3588,7 +3591,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
       <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
@@ -3629,7 +3632,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="A12" s="5" t="s">
         <v>83</v>
       </c>
@@ -3670,7 +3673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -3711,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15">
       <c r="A14" s="5" t="s">
         <v>87</v>
       </c>
@@ -3752,12 +3755,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15">
       <c r="A15" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" t="s">
         <v>235</v>
-      </c>
-      <c r="B15" t="s">
-        <v>236</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -3793,7 +3796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
         <v>89</v>
       </c>
@@ -3834,7 +3837,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>132</v>
       </c>
@@ -3875,7 +3878,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" s="5" t="s">
         <v>90</v>
       </c>
@@ -3916,7 +3919,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" s="5" t="s">
         <v>94</v>
       </c>
@@ -3957,7 +3960,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" s="5" t="s">
         <v>91</v>
       </c>
@@ -3998,7 +4001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" s="5" t="s">
         <v>92</v>
       </c>
@@ -4039,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" s="5" t="s">
         <v>93</v>
       </c>
@@ -4080,7 +4083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" s="5" t="s">
         <v>194</v>
       </c>
@@ -4121,12 +4124,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B24" t="s">
         <v>237</v>
-      </c>
-      <c r="B24" t="s">
-        <v>238</v>
       </c>
       <c r="C24">
         <v>0</v>

</xml_diff>

<commit_message>
added xN2 to STREAMS
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,39 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clemens/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F32772-62C6-FF43-A9A2-64EECAB4E51D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="244">
   <si>
     <t>parvariable</t>
   </si>
@@ -750,16 +749,31 @@
   </si>
   <si>
     <t>Poling/Koretsky</t>
+  </si>
+  <si>
+    <t>cpl</t>
+  </si>
+  <si>
+    <t>Heat capacity liquid (assumed constant)</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Liquid molar fraction nitrogen</t>
+  </si>
+  <si>
+    <t>xN2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -965,52 +979,52 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="93">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1057,7 +1071,7 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1368,14 +1382,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
@@ -1390,7 +1404,7 @@
     <col min="13" max="13" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1431,7 +1445,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1467,7 +1481,7 @@
       </c>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1503,7 +1517,7 @@
       </c>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -1537,7 +1551,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -1576,7 +1590,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
@@ -1611,7 +1625,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
@@ -1646,7 +1660,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -1681,7 +1695,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -1716,7 +1730,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -1751,7 +1765,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>127</v>
       </c>
@@ -1786,7 +1800,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1825,7 +1839,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1843,7 +1857,7 @@
       <c r="K13" s="9"/>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -1882,7 +1896,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>110</v>
       </c>
@@ -1919,7 +1933,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>143</v>
       </c>
@@ -1950,7 +1964,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>141</v>
       </c>
@@ -1972,7 +1986,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
@@ -2011,7 +2025,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>159</v>
       </c>
@@ -2050,7 +2064,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>162</v>
       </c>
@@ -2089,7 +2103,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>168</v>
       </c>
@@ -2126,7 +2140,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>169</v>
       </c>
@@ -2163,7 +2177,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>175</v>
       </c>
@@ -2198,7 +2212,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>177</v>
       </c>
@@ -2233,7 +2247,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>186</v>
       </c>
@@ -2268,7 +2282,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>188</v>
       </c>
@@ -2303,7 +2317,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>190</v>
       </c>
@@ -2338,7 +2352,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>196</v>
       </c>
@@ -2370,7 +2384,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>210</v>
       </c>
@@ -2403,7 +2417,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>211</v>
       </c>
@@ -2438,7 +2452,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>208</v>
       </c>
@@ -2473,7 +2487,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>209</v>
       </c>
@@ -2508,7 +2522,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>212</v>
       </c>
@@ -2543,7 +2557,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>218</v>
       </c>
@@ -2578,7 +2592,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>219</v>
       </c>
@@ -2610,7 +2624,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>215</v>
       </c>
@@ -2642,7 +2656,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>216</v>
       </c>
@@ -2677,7 +2691,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>213</v>
       </c>
@@ -2712,7 +2726,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>214</v>
       </c>
@@ -2747,7 +2761,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>217</v>
       </c>
@@ -2782,7 +2796,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>222</v>
       </c>
@@ -2817,7 +2831,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>223</v>
       </c>
@@ -2849,7 +2863,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>229</v>
       </c>
@@ -2878,7 +2892,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>231</v>
       </c>
@@ -2905,6 +2919,20 @@
       <c r="J44" s="13"/>
       <c r="L44" s="7" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C45" s="13">
+        <v>72</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -2914,19 +2942,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -2955,7 +2983,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -2978,7 +3006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -3001,7 +3029,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -3009,7 +3037,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -3017,7 +3045,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -3025,7 +3053,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -3033,7 +3061,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -3042,7 +3070,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -3051,7 +3079,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -3059,7 +3087,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -3068,7 +3096,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -3076,7 +3104,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -3091,7 +3119,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -3102,7 +3130,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>170</v>
       </c>
@@ -3116,7 +3144,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>173</v>
       </c>
@@ -3130,7 +3158,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>226</v>
       </c>
@@ -3151,19 +3179,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -3210,7 +3238,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -3251,7 +3279,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>67</v>
       </c>
@@ -3292,7 +3320,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -3336,7 +3364,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
@@ -3380,7 +3408,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -3424,7 +3452,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -3468,7 +3496,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -3509,7 +3537,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>131</v>
       </c>
@@ -3550,7 +3578,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>79</v>
       </c>
@@ -3591,7 +3619,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
@@ -3632,7 +3660,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>83</v>
       </c>
@@ -3673,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -3714,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>87</v>
       </c>
@@ -3755,7 +3783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>234</v>
       </c>
@@ -3796,372 +3824,413 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B16" t="s">
+        <v>243</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>95</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>0.1</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>0.1</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>0.1</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>0.1</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>0.1</v>
       </c>
-      <c r="H16">
+      <c r="H17">
         <v>0.1</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <v>0.1</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <v>0.1</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
         <v>0.1</v>
       </c>
-      <c r="M16">
+      <c r="M17">
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>96</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>0.2</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>0.2</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>0.2</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>0.2</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>0.2</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>0.2</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>0.2</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>0.2</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>0.2</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>97</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>0.3</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>0.3</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>0.3</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>0.3</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>0.3</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>0.3</v>
       </c>
-      <c r="I18">
+      <c r="I19">
         <v>0.3</v>
       </c>
-      <c r="J18">
+      <c r="J19">
         <v>0.3</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
         <v>0.3</v>
       </c>
-      <c r="M18">
+      <c r="M19">
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>98</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>0.4</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>0.4</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>0.4</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>0.4</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>0.4</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <v>0.4</v>
       </c>
-      <c r="I19">
+      <c r="I20">
         <v>0.4</v>
       </c>
-      <c r="J19">
+      <c r="J20">
         <v>0.4</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
         <v>0.4</v>
       </c>
-      <c r="M19">
+      <c r="M20">
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>99</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="5" t="s">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>100</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="5" t="s">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>101</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" s="5" t="s">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>195</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" s="5" t="s">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>237</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected R*T in enthalpy_temperature, progress in hcn_distillation, added cpl (bullshit values) in Data.xlsv
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="243">
   <si>
     <t>parvariable</t>
   </si>
@@ -755,9 +755,6 @@
   </si>
   <si>
     <t>Heat capacity liquid (assumed constant)</t>
-  </si>
-  <si>
-    <t>J</t>
   </si>
   <si>
     <t>Liquid molar fraction nitrogen</t>
@@ -773,7 +770,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -830,8 +827,15 @@
       <color theme="1"/>
       <name val="TT1AAt00"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -856,6 +860,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -866,7 +875,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -960,8 +969,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -977,8 +987,9 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="93" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="94">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1071,6 +1082,7 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Schlecht" xfId="93" builtinId="27"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1385,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2928,11 +2940,32 @@
       <c r="B45" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C45" s="13">
+      <c r="C45" s="15">
         <v>72</v>
       </c>
+      <c r="D45" s="15">
+        <v>72</v>
+      </c>
+      <c r="E45" s="15">
+        <v>72</v>
+      </c>
+      <c r="F45" s="15">
+        <v>72</v>
+      </c>
+      <c r="G45" s="15">
+        <v>72</v>
+      </c>
+      <c r="H45" s="15">
+        <v>72</v>
+      </c>
+      <c r="I45" s="15">
+        <v>72</v>
+      </c>
+      <c r="J45" s="15">
+        <v>72</v>
+      </c>
       <c r="L45" s="7" t="s">
-        <v>241</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3182,7 +3215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
@@ -3826,10 +3859,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B16" t="s">
         <v>242</v>
-      </c>
-      <c r="B16" t="s">
-        <v>243</v>
       </c>
       <c r="C16">
         <v>0</v>

</xml_diff>

<commit_message>
Data for natural gas added
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,30 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clemens/CS/MatlabWD/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -32,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="269">
   <si>
     <t>parvariable</t>
   </si>
@@ -761,6 +756,84 @@
   </si>
   <si>
     <t>xN2</t>
+  </si>
+  <si>
+    <t>Ethane</t>
+  </si>
+  <si>
+    <t>Propane</t>
+  </si>
+  <si>
+    <t>Isobutane</t>
+  </si>
+  <si>
+    <t>Butane</t>
+  </si>
+  <si>
+    <t>Isopentane</t>
+  </si>
+  <si>
+    <t>Pentane</t>
+  </si>
+  <si>
+    <t>Hexane</t>
+  </si>
+  <si>
+    <t>Carbon dioxide</t>
+  </si>
+  <si>
+    <t>Oxygen</t>
+  </si>
+  <si>
+    <t>C2H6</t>
+  </si>
+  <si>
+    <t>C3H8</t>
+  </si>
+  <si>
+    <t>entity L</t>
+  </si>
+  <si>
+    <t>entity M</t>
+  </si>
+  <si>
+    <t>entity N</t>
+  </si>
+  <si>
+    <t>C4H10</t>
+  </si>
+  <si>
+    <t>entity O</t>
+  </si>
+  <si>
+    <t>entity P</t>
+  </si>
+  <si>
+    <t>entity Q</t>
+  </si>
+  <si>
+    <t>entity R</t>
+  </si>
+  <si>
+    <t>entity S</t>
+  </si>
+  <si>
+    <t>C5H12</t>
+  </si>
+  <si>
+    <t>C6H14</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>Mole fraction in the natural gas</t>
+  </si>
+  <si>
+    <t>xNatGas</t>
   </si>
 </sst>
 </file>
@@ -875,7 +948,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="94">
+  <cellStyleXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -970,6 +1043,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -989,101 +1072,111 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="93" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="94">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Schlecht" xfId="93" builtinId="27"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+  <cellStyles count="104">
+    <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1387,7 +1480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1395,13 +1488,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
@@ -1411,12 +1504,20 @@
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="11" width="18.83203125" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="15" width="13.83203125" customWidth="1"/>
+    <col min="16" max="17" width="16.1640625" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="16.1640625" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="13" customWidth="1"/>
+    <col min="22" max="22" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1451,13 +1552,40 @@
         <v>64</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="16">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1491,9 +1619,36 @@
       <c r="K2" s="7">
         <v>9</v>
       </c>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L2" s="7">
+        <v>10</v>
+      </c>
+      <c r="M2" s="7">
+        <v>11</v>
+      </c>
+      <c r="N2" s="7">
+        <v>12</v>
+      </c>
+      <c r="O2" s="7">
+        <v>13</v>
+      </c>
+      <c r="P2" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>15</v>
+      </c>
+      <c r="R2" s="7">
+        <v>16</v>
+      </c>
+      <c r="S2" s="7">
+        <v>17</v>
+      </c>
+      <c r="T2" s="7">
+        <v>18</v>
+      </c>
+      <c r="U2" s="7"/>
+    </row>
+    <row r="3" spans="1:22" ht="16">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1527,9 +1682,36 @@
       <c r="K3" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L3" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="U3" s="7"/>
+    </row>
+    <row r="4" spans="1:22" ht="16">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -1561,9 +1743,36 @@
         <v>125</v>
       </c>
       <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L4" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="U4" s="7"/>
+    </row>
+    <row r="5" spans="1:22" ht="16">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -1595,14 +1804,23 @@
         <v>187.49</v>
       </c>
       <c r="K5" s="9"/>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="M5" t="s">
+      <c r="V5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="16">
       <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
@@ -1632,12 +1850,21 @@
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-      <c r="L6" s="7"/>
-      <c r="M6" t="s">
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="7"/>
+      <c r="V6" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" ht="16">
       <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
@@ -1667,12 +1894,21 @@
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-      <c r="L7" s="7"/>
-      <c r="M7" t="s">
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="7"/>
+      <c r="V7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="16">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -1702,12 +1938,21 @@
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
-      <c r="L8" s="7"/>
-      <c r="M8" t="s">
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="7"/>
+      <c r="V8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="16">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -1737,12 +1982,21 @@
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="7"/>
-      <c r="M9" t="s">
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="7"/>
+      <c r="V9" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" ht="16">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -1772,12 +2026,21 @@
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
-      <c r="L10" s="7"/>
-      <c r="M10" t="s">
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="7"/>
+      <c r="V10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" ht="16">
       <c r="A11" s="1" t="s">
         <v>127</v>
       </c>
@@ -1807,12 +2070,21 @@
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
-      <c r="L11" s="7"/>
-      <c r="M11" t="s">
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="7"/>
+      <c r="V11" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="16">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1844,14 +2116,41 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="K12" s="9"/>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="9">
+        <v>3.0068999999999999E-2</v>
+      </c>
+      <c r="M12" s="9">
+        <v>4.4096000000000003E-2</v>
+      </c>
+      <c r="N12" s="9">
+        <v>5.8122E-2</v>
+      </c>
+      <c r="O12" s="9">
+        <v>5.8122E-2</v>
+      </c>
+      <c r="P12" s="9">
+        <v>7.2149000000000005E-2</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>7.2149000000000005E-2</v>
+      </c>
+      <c r="R12" s="9">
+        <v>8.6175000000000002E-2</v>
+      </c>
+      <c r="S12" s="9">
+        <v>4.4010000000000001E-2</v>
+      </c>
+      <c r="T12" s="9">
+        <v>3.1997999999999999E-2</v>
+      </c>
+      <c r="U12" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="M12" s="7" t="s">
+      <c r="V12" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" ht="16">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1867,9 +2166,18 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" spans="1:22" ht="16">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -1901,14 +2209,23 @@
         <v>553.16</v>
       </c>
       <c r="K14" s="9"/>
-      <c r="L14" s="7" t="s">
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="V14" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" ht="16">
       <c r="A15" s="1" t="s">
         <v>110</v>
       </c>
@@ -1938,14 +2255,23 @@
       </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="V15" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" ht="16">
       <c r="A16" s="1" t="s">
         <v>143</v>
       </c>
@@ -1969,14 +2295,23 @@
         <v>1769</v>
       </c>
       <c r="K16" s="9"/>
-      <c r="L16" s="7" t="s">
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="M16" s="7" t="s">
+      <c r="V16" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" ht="16">
       <c r="A17" s="1" t="s">
         <v>141</v>
       </c>
@@ -1994,11 +2329,20 @@
       <c r="K17" s="13">
         <v>4.5</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" ht="16">
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
@@ -2030,14 +2374,23 @@
         <v>-1180900</v>
       </c>
       <c r="K18" s="13"/>
-      <c r="L18" s="7" t="s">
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="V18" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" ht="16">
       <c r="A19" s="1" t="s">
         <v>159</v>
       </c>
@@ -2069,14 +2422,23 @@
         <v>-901700</v>
       </c>
       <c r="K19" s="13"/>
-      <c r="L19" s="7" t="s">
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="V19" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" ht="16">
       <c r="A20" s="1" t="s">
         <v>162</v>
       </c>
@@ -2108,14 +2470,23 @@
         <v>220.1</v>
       </c>
       <c r="K20" s="13"/>
-      <c r="L20" s="7" t="s">
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="M20" s="7" t="s">
+      <c r="V20" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" ht="16">
       <c r="A21" s="1" t="s">
         <v>168</v>
       </c>
@@ -2145,14 +2516,23 @@
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
-      <c r="L21" s="7" t="s">
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="M21" s="7" t="s">
+      <c r="V21" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" ht="16">
       <c r="A22" s="1" t="s">
         <v>169</v>
       </c>
@@ -2182,14 +2562,23 @@
       </c>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
-      <c r="L22" s="7" t="s">
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="M22" s="7" t="s">
+      <c r="V22" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" ht="16">
       <c r="A23" s="1" t="s">
         <v>175</v>
       </c>
@@ -2217,14 +2606,23 @@
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
-      <c r="L23" s="7" t="s">
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="M23" s="7" t="s">
+      <c r="V23" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" ht="16">
       <c r="A24" s="1" t="s">
         <v>177</v>
       </c>
@@ -2252,14 +2650,23 @@
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
-      <c r="L24" s="7" t="s">
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="M24" s="7" t="s">
+      <c r="V24" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" ht="16">
       <c r="A25" s="1" t="s">
         <v>186</v>
       </c>
@@ -2287,14 +2694,41 @@
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
-      <c r="L25" s="7" t="s">
+      <c r="L25" s="13">
+        <v>305.36</v>
+      </c>
+      <c r="M25" s="13">
+        <v>369.9</v>
+      </c>
+      <c r="N25" s="13">
+        <v>407.84</v>
+      </c>
+      <c r="O25" s="13">
+        <v>425.2</v>
+      </c>
+      <c r="P25" s="13">
+        <v>460.37</v>
+      </c>
+      <c r="Q25" s="13">
+        <v>469.7</v>
+      </c>
+      <c r="R25" s="13">
+        <v>507.5</v>
+      </c>
+      <c r="S25" s="13">
+        <v>304.13</v>
+      </c>
+      <c r="T25" s="13">
+        <v>154.58000000000001</v>
+      </c>
+      <c r="U25" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="M25" s="7" t="s">
+      <c r="V25" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" ht="16">
       <c r="A26" s="1" t="s">
         <v>188</v>
       </c>
@@ -2322,14 +2756,23 @@
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
-      <c r="L26" s="7" t="s">
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="M26" s="7" t="s">
+      <c r="V26" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" ht="16">
       <c r="A27" s="1" t="s">
         <v>190</v>
       </c>
@@ -2357,14 +2800,23 @@
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
-      <c r="L27" s="7" t="s">
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="M27" s="7" t="s">
+      <c r="V27" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" ht="16">
       <c r="A28" s="1" t="s">
         <v>196</v>
       </c>
@@ -2392,11 +2844,20 @@
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
-      <c r="M28" s="7" t="s">
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="V28" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" ht="16">
       <c r="A29" s="1" t="s">
         <v>210</v>
       </c>
@@ -2424,12 +2885,21 @@
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7" t="s">
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" ht="16">
       <c r="A30" s="1" t="s">
         <v>211</v>
       </c>
@@ -2457,14 +2927,23 @@
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
-      <c r="L30" s="7" t="s">
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="M30" s="7" t="s">
+      <c r="V30" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" ht="16">
       <c r="A31" s="1" t="s">
         <v>208</v>
       </c>
@@ -2492,14 +2971,23 @@
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
-      <c r="L31" s="7" t="s">
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="M31" s="7" t="s">
+      <c r="V31" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" ht="16">
       <c r="A32" s="1" t="s">
         <v>209</v>
       </c>
@@ -2527,14 +3015,23 @@
       <c r="I32" s="13"/>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
-      <c r="L32" s="7" t="s">
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="M32" s="7" t="s">
+      <c r="V32" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" ht="16">
       <c r="A33" s="1" t="s">
         <v>212</v>
       </c>
@@ -2562,14 +3059,23 @@
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
-      <c r="L33" s="7" t="s">
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13"/>
+      <c r="T33" s="13"/>
+      <c r="U33" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="M33" s="7" t="s">
+      <c r="V33" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" ht="16">
       <c r="A34" s="1" t="s">
         <v>218</v>
       </c>
@@ -2597,14 +3103,23 @@
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
-      <c r="L34" s="7" t="s">
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13"/>
+      <c r="T34" s="13"/>
+      <c r="U34" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="M34" s="7" t="s">
+      <c r="V34" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" ht="16">
       <c r="A35" s="1" t="s">
         <v>219</v>
       </c>
@@ -2632,11 +3147,20 @@
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
-      <c r="M35" s="7" t="s">
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13"/>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13"/>
+      <c r="T35" s="13"/>
+      <c r="V35" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" ht="16">
       <c r="A36" s="1" t="s">
         <v>215</v>
       </c>
@@ -2664,11 +3188,20 @@
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
-      <c r="M36" s="7" t="s">
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="V36" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" ht="16">
       <c r="A37" s="1" t="s">
         <v>216</v>
       </c>
@@ -2696,14 +3229,23 @@
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
-      <c r="L37" s="7" t="s">
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13"/>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="M37" s="7" t="s">
+      <c r="V37" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" ht="16">
       <c r="A38" s="1" t="s">
         <v>213</v>
       </c>
@@ -2731,14 +3273,23 @@
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
-      <c r="L38" s="7" t="s">
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="M38" s="7" t="s">
+      <c r="V38" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" ht="16">
       <c r="A39" s="1" t="s">
         <v>214</v>
       </c>
@@ -2766,14 +3317,23 @@
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
-      <c r="L39" s="7" t="s">
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="M39" s="7" t="s">
+      <c r="V39" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" ht="16">
       <c r="A40" s="1" t="s">
         <v>217</v>
       </c>
@@ -2801,14 +3361,23 @@
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
-      <c r="L40" s="7" t="s">
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+      <c r="N40" s="13"/>
+      <c r="O40" s="13"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13"/>
+      <c r="T40" s="13"/>
+      <c r="U40" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="M40" s="7" t="s">
+      <c r="V40" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" ht="16">
       <c r="A41" s="1" t="s">
         <v>222</v>
       </c>
@@ -2836,14 +3405,23 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
-      <c r="L41" s="7" t="s">
+      <c r="L41" s="13"/>
+      <c r="M41" s="13"/>
+      <c r="N41" s="13"/>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13"/>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="M41" s="7" t="s">
+      <c r="V41" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" ht="16">
       <c r="A42" s="1" t="s">
         <v>223</v>
       </c>
@@ -2871,11 +3449,20 @@
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
-      <c r="M42" s="7" t="s">
+      <c r="L42" s="13"/>
+      <c r="M42" s="13"/>
+      <c r="N42" s="13"/>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13"/>
+      <c r="T42" s="13"/>
+      <c r="V42" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" ht="16">
       <c r="A43" s="1" t="s">
         <v>229</v>
       </c>
@@ -2900,11 +3487,11 @@
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
-      <c r="L43" s="7" t="s">
+      <c r="U43" s="7" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" ht="16">
       <c r="A44" s="1" t="s">
         <v>231</v>
       </c>
@@ -2929,11 +3516,11 @@
       </c>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
-      <c r="L44" s="7" t="s">
+      <c r="U44" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" ht="16">
       <c r="A45" s="1" t="s">
         <v>240</v>
       </c>
@@ -2964,13 +3551,59 @@
       <c r="J45" s="15">
         <v>72</v>
       </c>
-      <c r="L45" s="7" t="s">
+      <c r="U45" s="7" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" ht="16">
+      <c r="A46" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D46" s="13">
+        <v>0.01</v>
+      </c>
+      <c r="E46">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="L46" s="3">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="M46" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="N46" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="O46" s="3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="P46" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="R46" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="S46" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="T46" s="3">
+        <v>1E-4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2982,12 +3615,12 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3016,7 +3649,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -3039,7 +3672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -3062,7 +3695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -3070,7 +3703,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -3078,7 +3711,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>45</v>
       </c>
@@ -3086,7 +3719,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -3094,7 +3727,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -3103,7 +3736,7 @@
       </c>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -3112,7 +3745,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -3120,7 +3753,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -3129,7 +3762,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -3137,7 +3770,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -3152,7 +3785,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -3163,7 +3796,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>170</v>
       </c>
@@ -3177,7 +3810,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
         <v>173</v>
       </c>
@@ -3191,7 +3824,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>226</v>
       </c>
@@ -3208,6 +3841,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3219,12 +3857,12 @@
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -3271,7 +3909,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -3312,7 +3950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" s="5" t="s">
         <v>67</v>
       </c>
@@ -3353,7 +3991,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -3397,7 +4035,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
@@ -3441,7 +4079,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -3485,7 +4123,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -3529,7 +4167,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
@@ -3570,7 +4208,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>131</v>
       </c>
@@ -3611,7 +4249,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
         <v>79</v>
       </c>
@@ -3652,7 +4290,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
       <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
@@ -3693,7 +4331,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="A12" s="5" t="s">
         <v>83</v>
       </c>
@@ -3734,7 +4372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -3775,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15">
       <c r="A14" s="5" t="s">
         <v>87</v>
       </c>
@@ -3816,7 +4454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15">
       <c r="A15" s="5" t="s">
         <v>234</v>
       </c>
@@ -3857,7 +4495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15">
       <c r="A16" s="5" t="s">
         <v>241</v>
       </c>
@@ -3898,7 +4536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>89</v>
       </c>
@@ -3939,7 +4577,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>132</v>
       </c>
@@ -3980,7 +4618,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" s="5" t="s">
         <v>90</v>
       </c>
@@ -4021,7 +4659,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" s="5" t="s">
         <v>94</v>
       </c>
@@ -4062,7 +4700,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" s="5" t="s">
         <v>91</v>
       </c>
@@ -4103,7 +4741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" s="5" t="s">
         <v>92</v>
       </c>
@@ -4144,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" s="5" t="s">
         <v>93</v>
       </c>
@@ -4185,7 +4823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" s="5" t="s">
         <v>194</v>
       </c>
@@ -4226,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" s="5" t="s">
         <v>236</v>
       </c>
@@ -4270,5 +4908,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Liquid heat capacities added
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="274">
   <si>
     <t>parvariable</t>
   </si>
@@ -843,6 +843,12 @@
   </si>
   <si>
     <t>J.m-3</t>
+  </si>
+  <si>
+    <t>Sander</t>
+  </si>
+  <si>
+    <t>UnionGas</t>
   </si>
 </sst>
 </file>
@@ -917,7 +923,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -947,6 +953,12 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -957,7 +969,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="104">
+  <cellStyleXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1052,6 +1064,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1079,9 +1099,9 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="93" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="93" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="104">
+  <cellStyles count="112">
     <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
@@ -1134,6 +1154,10 @@
     <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1185,6 +1209,10 @@
     <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1499,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3535,6 +3563,9 @@
       <c r="U43" s="7" t="s">
         <v>233</v>
       </c>
+      <c r="V43" s="7" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="44" spans="1:22" ht="16">
       <c r="A44" s="1" t="s">
@@ -3564,6 +3595,9 @@
       <c r="U44" s="7" t="s">
         <v>108</v>
       </c>
+      <c r="V44" s="7" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="45" spans="1:22" ht="16">
       <c r="A45" s="1" t="s">
@@ -3572,32 +3606,35 @@
       <c r="B45" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C45" s="15">
-        <v>72</v>
+      <c r="C45" s="9">
+        <v>75.349999999999994</v>
       </c>
       <c r="D45" s="15">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="E45" s="15">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="F45" s="15">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="G45" s="15">
-        <v>72</v>
-      </c>
-      <c r="H45" s="15">
-        <v>72</v>
-      </c>
-      <c r="I45" s="15">
-        <v>72</v>
-      </c>
-      <c r="J45" s="15">
-        <v>72</v>
+        <v>0</v>
+      </c>
+      <c r="H45" s="9">
+        <v>70.63</v>
+      </c>
+      <c r="I45" s="9">
+        <v>138.9</v>
+      </c>
+      <c r="J45" s="9">
+        <v>187.49</v>
       </c>
       <c r="U45" s="7" t="s">
         <v>165</v>
+      </c>
+      <c r="V45" s="7" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="16">
@@ -3639,6 +3676,9 @@
       </c>
       <c r="T46" s="3">
         <v>1E-4</v>
+      </c>
+      <c r="V46" s="7" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3656,7 +3696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Thermal conductivity of gases
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="286">
   <si>
     <t>parvariable</t>
   </si>
@@ -849,6 +849,42 @@
   </si>
   <si>
     <t>UnionGas</t>
+  </si>
+  <si>
+    <t>Thermal conductivity at 100K</t>
+  </si>
+  <si>
+    <t>lambda100</t>
+  </si>
+  <si>
+    <t>lambda200</t>
+  </si>
+  <si>
+    <t>Thermal conductivity at 200K</t>
+  </si>
+  <si>
+    <t>Thermal conductivity at 300K</t>
+  </si>
+  <si>
+    <t>Thermal conductivity at 400K</t>
+  </si>
+  <si>
+    <t>lambda300</t>
+  </si>
+  <si>
+    <t>lambda400</t>
+  </si>
+  <si>
+    <t>lambda500</t>
+  </si>
+  <si>
+    <t>lambda600</t>
+  </si>
+  <si>
+    <t>Thermal conductivity at 500K</t>
+  </si>
+  <si>
+    <t>Thermal conductivity at 600K</t>
   </si>
 </sst>
 </file>
@@ -923,7 +959,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -959,6 +995,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -969,7 +1011,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="112">
+  <cellStyleXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1082,8 +1124,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1100,8 +1148,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="93" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="112">
+  <cellStyles count="118">
     <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
@@ -1158,6 +1208,9 @@
     <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1213,6 +1266,9 @@
     <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1517,7 +1573,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1525,10 +1581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V46"/>
+  <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="H29" workbookViewId="0">
+      <selection activeCell="T53" sqref="T53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3681,6 +3737,354 @@
         <v>273</v>
       </c>
     </row>
+    <row r="47" spans="1:22" ht="16">
+      <c r="A47" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C47" s="16">
+        <v>0</v>
+      </c>
+      <c r="D47" s="13">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1.04E-2</v>
+      </c>
+      <c r="F47" s="16">
+        <v>0</v>
+      </c>
+      <c r="G47" s="13">
+        <v>6.8199999999999997E-2</v>
+      </c>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="17">
+        <v>0</v>
+      </c>
+      <c r="M47" s="17">
+        <v>0</v>
+      </c>
+      <c r="N47" s="17">
+        <v>0</v>
+      </c>
+      <c r="O47" s="17">
+        <v>0</v>
+      </c>
+      <c r="P47" s="13"/>
+      <c r="Q47" s="17">
+        <v>0</v>
+      </c>
+      <c r="R47" s="17">
+        <v>0</v>
+      </c>
+      <c r="S47" s="17">
+        <v>0</v>
+      </c>
+      <c r="T47" s="13">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="U47" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="V47" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" ht="16">
+      <c r="A48" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C48" s="16">
+        <v>0</v>
+      </c>
+      <c r="D48" s="13">
+        <v>1.83E-2</v>
+      </c>
+      <c r="E48" s="3">
+        <v>2.18E-2</v>
+      </c>
+      <c r="F48" s="16">
+        <v>0</v>
+      </c>
+      <c r="G48" s="13">
+        <v>0.1328</v>
+      </c>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="13">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="M48" s="17">
+        <v>0</v>
+      </c>
+      <c r="N48" s="17">
+        <v>0</v>
+      </c>
+      <c r="O48" s="17">
+        <v>0</v>
+      </c>
+      <c r="P48" s="13"/>
+      <c r="Q48" s="17">
+        <v>0</v>
+      </c>
+      <c r="R48" s="17">
+        <v>0</v>
+      </c>
+      <c r="S48" s="13">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="T48" s="13">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="U48" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="V48" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="16">
+      <c r="A49" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C49" s="3">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="D49" s="13">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E49" s="3">
+        <v>3.44E-2</v>
+      </c>
+      <c r="F49" s="3">
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="G49" s="13">
+        <v>0.18659999999999999</v>
+      </c>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="13">
+        <v>2.12E-2</v>
+      </c>
+      <c r="M49" s="13">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="N49" s="13">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="O49" s="13">
+        <v>1.67E-2</v>
+      </c>
+      <c r="P49" s="13"/>
+      <c r="Q49" s="17">
+        <v>0</v>
+      </c>
+      <c r="R49" s="17">
+        <v>0</v>
+      </c>
+      <c r="S49" s="13">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="T49" s="13">
+        <v>2.6499999999999999E-2</v>
+      </c>
+      <c r="U49" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="V49" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" ht="16">
+      <c r="A50" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C50" s="3">
+        <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="D50" s="13">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="F50" s="3">
+        <v>3.7199999999999997E-2</v>
+      </c>
+      <c r="G50" s="13">
+        <v>0.23089999999999999</v>
+      </c>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="M50" s="13">
+        <v>3.1E-2</v>
+      </c>
+      <c r="N50" s="13">
+        <v>2.8899999999999999E-2</v>
+      </c>
+      <c r="O50" s="13">
+        <v>2.8299999999999999E-2</v>
+      </c>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13">
+        <v>2.4899999999999999E-2</v>
+      </c>
+      <c r="R50" s="13">
+        <v>2.3400000000000001E-2</v>
+      </c>
+      <c r="S50" s="13">
+        <v>2.52E-2</v>
+      </c>
+      <c r="T50" s="13">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="U50" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="V50" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="16">
+      <c r="A51" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="C51" s="3">
+        <v>3.56E-2</v>
+      </c>
+      <c r="D51" s="13">
+        <v>3.9E-2</v>
+      </c>
+      <c r="E51" s="3">
+        <v>6.8400000000000002E-2</v>
+      </c>
+      <c r="F51" s="3">
+        <v>5.3100000000000001E-2</v>
+      </c>
+      <c r="G51" s="13">
+        <v>0.27089999999999997</v>
+      </c>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13">
+        <v>5.3800000000000001E-2</v>
+      </c>
+      <c r="M51" s="13">
+        <v>4.6399999999999997E-2</v>
+      </c>
+      <c r="N51" s="13">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="O51" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="P51" s="13"/>
+      <c r="Q51" s="13">
+        <v>3.78E-2</v>
+      </c>
+      <c r="R51" s="13">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="S51" s="13">
+        <v>3.3500000000000002E-2</v>
+      </c>
+      <c r="T51" s="13">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="U51" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="V51" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="16">
+      <c r="A52" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C52" s="3">
+        <v>4.6199999999999998E-2</v>
+      </c>
+      <c r="D52" s="13">
+        <v>4.48E-2</v>
+      </c>
+      <c r="E52" s="3">
+        <v>8.8599999999999998E-2</v>
+      </c>
+      <c r="F52" s="3">
+        <v>6.8599999999999994E-2</v>
+      </c>
+      <c r="G52" s="13">
+        <v>0.30909999999999999</v>
+      </c>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="M52" s="13">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="N52" s="13">
+        <v>6.0199999999999997E-2</v>
+      </c>
+      <c r="O52" s="13">
+        <v>6.0900000000000003E-2</v>
+      </c>
+      <c r="P52" s="13"/>
+      <c r="Q52" s="13">
+        <v>5.2699999999999997E-2</v>
+      </c>
+      <c r="R52" s="13">
+        <v>4.87E-2</v>
+      </c>
+      <c r="S52" s="13">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="T52" s="13">
+        <v>4.7699999999999999E-2</v>
+      </c>
+      <c r="U52" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="V52" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Minor changes, Sinterkorund nach hinten geschoben
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="308">
   <si>
     <t>parvariable</t>
   </si>
@@ -815,9 +815,6 @@
     <t>entity R</t>
   </si>
   <si>
-    <t>entity S</t>
-  </si>
-  <si>
     <t>C5H12</t>
   </si>
   <si>
@@ -951,6 +948,9 @@
   </si>
   <si>
     <t>Thermal conductivity at 333.16K</t>
+  </si>
+  <si>
+    <t>W.m-1.K-1</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1077,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="118">
+  <cellStyleXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1172,6 +1172,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1218,7 +1228,7 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="118">
+  <cellStyles count="128">
     <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
@@ -1278,6 +1288,11 @@
     <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1336,6 +1351,11 @@
     <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1650,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1665,14 +1685,14 @@
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
     <col min="10" max="10" width="18.83203125" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="15" width="13.83203125" customWidth="1"/>
-    <col min="16" max="17" width="16.1640625" customWidth="1"/>
-    <col min="18" max="18" width="14.6640625" customWidth="1"/>
-    <col min="19" max="19" width="16.1640625" customWidth="1"/>
-    <col min="20" max="20" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="14" width="13.83203125" customWidth="1"/>
+    <col min="15" max="16" width="16.1640625" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.1640625" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" customWidth="1"/>
     <col min="21" max="21" width="13" customWidth="1"/>
     <col min="22" max="22" width="18.33203125" customWidth="1"/>
   </cols>
@@ -1712,31 +1732,31 @@
         <v>64</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>102</v>
@@ -1840,34 +1860,34 @@
         <v>124</v>
       </c>
       <c r="K3" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="T3" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>251</v>
       </c>
       <c r="U3" s="7"/>
     </row>
@@ -1902,21 +1922,23 @@
       <c r="J4" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="7" t="s">
+        <v>252</v>
+      </c>
       <c r="L4" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>257</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>263</v>
@@ -1927,9 +1949,7 @@
       <c r="S4" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="T4" s="7" t="s">
-        <v>266</v>
-      </c>
+      <c r="T4" s="7"/>
       <c r="U4" s="7"/>
     </row>
     <row r="5" spans="1:22" ht="16">
@@ -2275,34 +2295,34 @@
       <c r="J12" s="9">
         <v>0.13200000000000001</v>
       </c>
-      <c r="K12" s="9"/>
+      <c r="K12" s="9">
+        <v>3.0068999999999999E-2</v>
+      </c>
       <c r="L12" s="9">
-        <v>3.0068999999999999E-2</v>
+        <v>4.4096000000000003E-2</v>
       </c>
       <c r="M12" s="9">
-        <v>4.4096000000000003E-2</v>
+        <v>5.8122E-2</v>
       </c>
       <c r="N12" s="9">
         <v>5.8122E-2</v>
       </c>
       <c r="O12" s="9">
-        <v>5.8122E-2</v>
+        <v>7.2149000000000005E-2</v>
       </c>
       <c r="P12" s="9">
         <v>7.2149000000000005E-2</v>
       </c>
       <c r="Q12" s="9">
-        <v>7.2149000000000005E-2</v>
+        <v>8.6175000000000002E-2</v>
       </c>
       <c r="R12" s="9">
-        <v>8.6175000000000002E-2</v>
+        <v>4.4010000000000001E-2</v>
       </c>
       <c r="S12" s="9">
-        <v>4.4010000000000001E-2</v>
-      </c>
-      <c r="T12" s="9">
         <v>3.1997999999999999E-2</v>
       </c>
+      <c r="T12" s="9"/>
       <c r="U12" s="7" t="s">
         <v>103</v>
       </c>
@@ -2486,9 +2506,7 @@
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
-      <c r="K17" s="13">
-        <v>4.5</v>
-      </c>
+      <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
@@ -2497,7 +2515,9 @@
       <c r="Q17" s="13"/>
       <c r="R17" s="13"/>
       <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
+      <c r="T17" s="13">
+        <v>4.5</v>
+      </c>
       <c r="U17" s="8" t="s">
         <v>156</v>
       </c>
@@ -2853,34 +2873,34 @@
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
+      <c r="K25" s="13">
+        <v>305.36</v>
+      </c>
       <c r="L25" s="13">
-        <v>305.36</v>
+        <v>369.9</v>
       </c>
       <c r="M25" s="13">
-        <v>369.9</v>
+        <v>407.84</v>
       </c>
       <c r="N25" s="13">
-        <v>407.84</v>
+        <v>425.2</v>
       </c>
       <c r="O25" s="13">
-        <v>425.2</v>
+        <v>460.37</v>
       </c>
       <c r="P25" s="13">
-        <v>460.37</v>
+        <v>469.7</v>
       </c>
       <c r="Q25" s="13">
-        <v>469.7</v>
+        <v>507.5</v>
       </c>
       <c r="R25" s="13">
-        <v>507.5</v>
+        <v>304.13</v>
       </c>
       <c r="S25" s="13">
-        <v>304.13</v>
-      </c>
-      <c r="T25" s="13">
         <v>154.58000000000001</v>
       </c>
+      <c r="T25" s="13"/>
       <c r="U25" s="7" t="s">
         <v>108</v>
       </c>
@@ -2915,34 +2935,34 @@
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
+      <c r="K26" s="13">
+        <v>4880000</v>
+      </c>
       <c r="L26" s="13">
-        <v>4880000</v>
+        <v>4250000</v>
       </c>
       <c r="M26" s="13">
-        <v>4250000</v>
+        <v>3640000</v>
       </c>
       <c r="N26" s="13">
-        <v>3640000</v>
+        <v>3790000</v>
       </c>
       <c r="O26" s="13">
-        <v>3790000</v>
+        <v>3350000</v>
       </c>
       <c r="P26" s="13">
-        <v>3350000</v>
+        <v>3370000</v>
       </c>
       <c r="Q26" s="13">
-        <v>3370000</v>
+        <v>3030000</v>
       </c>
       <c r="R26" s="13">
-        <v>3030000</v>
+        <v>7380000</v>
       </c>
       <c r="S26" s="13">
-        <v>7380000</v>
-      </c>
-      <c r="T26" s="13">
         <v>5040000</v>
       </c>
+      <c r="T26" s="13"/>
       <c r="U26" s="7" t="s">
         <v>140</v>
       </c>
@@ -3021,34 +3041,34 @@
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
+      <c r="K28" s="13">
+        <v>9.9000000000000005E-2</v>
+      </c>
       <c r="L28" s="13">
-        <v>9.9000000000000005E-2</v>
+        <v>0.153</v>
       </c>
       <c r="M28" s="13">
-        <v>0.153</v>
+        <v>0.183</v>
       </c>
       <c r="N28" s="13">
-        <v>0.183</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="O28" s="13">
-        <v>0.19900000000000001</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="P28" s="13">
-        <v>0.22700000000000001</v>
+        <v>0.251</v>
       </c>
       <c r="Q28" s="13">
-        <v>0.251</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="R28" s="13">
-        <v>0.29899999999999999</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="S28" s="13">
-        <v>0.23899999999999999</v>
-      </c>
-      <c r="T28" s="13">
         <v>2.5000000000000001E-2</v>
       </c>
+      <c r="T28" s="13"/>
       <c r="V28" s="7" t="s">
         <v>238</v>
       </c>
@@ -3687,7 +3707,7 @@
         <v>233</v>
       </c>
       <c r="V43" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="16">
@@ -3719,7 +3739,7 @@
         <v>108</v>
       </c>
       <c r="V44" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="16">
@@ -3762,10 +3782,10 @@
     </row>
     <row r="46" spans="1:22" ht="16">
       <c r="A46" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>267</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>268</v>
       </c>
       <c r="D46" s="13">
         <v>0.01</v>
@@ -3773,17 +3793,20 @@
       <c r="E46">
         <v>0.93899999999999995</v>
       </c>
+      <c r="K46" s="3">
+        <v>4.2000000000000003E-2</v>
+      </c>
       <c r="L46" s="3">
-        <v>4.2000000000000003E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="M46" s="3">
-        <v>3.0000000000000001E-3</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="N46" s="3">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="O46" s="3">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="P46" s="3">
         <v>1E-4</v>
@@ -3792,24 +3815,21 @@
         <v>1E-4</v>
       </c>
       <c r="R46" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="S46" s="3">
         <v>1E-4</v>
       </c>
-      <c r="S46" s="3">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="T46" s="3">
-        <v>1E-4</v>
-      </c>
       <c r="V46" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="16">
       <c r="A47" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C47" s="16">
         <v>0</v>
@@ -3859,11 +3879,11 @@
       <c r="R47" s="17">
         <v>0</v>
       </c>
-      <c r="S47" s="17">
-        <v>0</v>
-      </c>
-      <c r="T47" s="13">
+      <c r="S47" s="13">
         <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="T47" s="17">
+        <v>0</v>
       </c>
       <c r="U47" s="8" t="s">
         <v>156</v>
@@ -3874,10 +3894,10 @@
     </row>
     <row r="48" spans="1:22" ht="16">
       <c r="A48" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C48" s="16">
         <v>0</v>
@@ -3903,12 +3923,12 @@
       <c r="J48" s="17">
         <v>0</v>
       </c>
-      <c r="K48" s="17">
-        <v>0</v>
-      </c>
-      <c r="L48" s="13">
+      <c r="K48" s="13">
         <v>1.0699999999999999E-2</v>
       </c>
+      <c r="L48" s="17">
+        <v>0</v>
+      </c>
       <c r="M48" s="17">
         <v>0</v>
       </c>
@@ -3924,14 +3944,14 @@
       <c r="Q48" s="17">
         <v>0</v>
       </c>
-      <c r="R48" s="17">
-        <v>0</v>
+      <c r="R48" s="13">
+        <v>9.5999999999999992E-3</v>
       </c>
       <c r="S48" s="13">
-        <v>9.5999999999999992E-3</v>
-      </c>
-      <c r="T48" s="13">
         <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="T48" s="17">
+        <v>0</v>
       </c>
       <c r="U48" s="8" t="s">
         <v>156</v>
@@ -3942,10 +3962,10 @@
     </row>
     <row r="49" spans="1:22" ht="16">
       <c r="A49" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C49" s="3">
         <v>1.8599999999999998E-2</v>
@@ -3971,35 +3991,35 @@
       <c r="J49" s="17">
         <v>0</v>
       </c>
-      <c r="K49" s="17">
-        <v>0</v>
+      <c r="K49" s="13">
+        <v>2.12E-2</v>
       </c>
       <c r="L49" s="13">
-        <v>2.12E-2</v>
+        <v>1.8499999999999999E-2</v>
       </c>
       <c r="M49" s="13">
-        <v>1.8499999999999999E-2</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="N49" s="13">
-        <v>1.7100000000000001E-2</v>
-      </c>
-      <c r="O49" s="13">
         <v>1.67E-2</v>
       </c>
+      <c r="O49" s="17">
+        <v>0</v>
+      </c>
       <c r="P49" s="17">
         <v>0</v>
       </c>
       <c r="Q49" s="17">
         <v>0</v>
       </c>
-      <c r="R49" s="17">
-        <v>0</v>
+      <c r="R49" s="13">
+        <v>1.6799999999999999E-2</v>
       </c>
       <c r="S49" s="13">
-        <v>1.6799999999999999E-2</v>
-      </c>
-      <c r="T49" s="13">
         <v>2.6499999999999999E-2</v>
+      </c>
+      <c r="T49" s="17">
+        <v>0</v>
       </c>
       <c r="U49" s="8" t="s">
         <v>156</v>
@@ -4010,10 +4030,10 @@
     </row>
     <row r="50" spans="1:22" ht="16">
       <c r="A50" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C50" s="3">
         <v>2.6100000000000002E-2</v>
@@ -4039,35 +4059,35 @@
       <c r="J50" s="17">
         <v>0</v>
       </c>
-      <c r="K50" s="17">
-        <v>0</v>
+      <c r="K50" s="13">
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="L50" s="13">
-        <v>3.5999999999999997E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="M50" s="13">
-        <v>3.1E-2</v>
+        <v>2.8899999999999999E-2</v>
       </c>
       <c r="N50" s="13">
-        <v>2.8899999999999999E-2</v>
-      </c>
-      <c r="O50" s="13">
         <v>2.8299999999999999E-2</v>
       </c>
-      <c r="P50" s="17">
-        <v>0</v>
+      <c r="O50" s="17">
+        <v>0</v>
+      </c>
+      <c r="P50" s="13">
+        <v>2.4899999999999999E-2</v>
       </c>
       <c r="Q50" s="13">
-        <v>2.4899999999999999E-2</v>
+        <v>2.3400000000000001E-2</v>
       </c>
       <c r="R50" s="13">
-        <v>2.3400000000000001E-2</v>
+        <v>2.52E-2</v>
       </c>
       <c r="S50" s="13">
-        <v>2.52E-2</v>
-      </c>
-      <c r="T50" s="13">
         <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="T50" s="17">
+        <v>0</v>
       </c>
       <c r="U50" s="8" t="s">
         <v>156</v>
@@ -4078,10 +4098,10 @@
     </row>
     <row r="51" spans="1:22" ht="16">
       <c r="A51" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C51" s="3">
         <v>3.56E-2</v>
@@ -4107,35 +4127,35 @@
       <c r="J51" s="17">
         <v>0</v>
       </c>
-      <c r="K51" s="17">
-        <v>0</v>
+      <c r="K51" s="13">
+        <v>5.3800000000000001E-2</v>
       </c>
       <c r="L51" s="13">
-        <v>5.3800000000000001E-2</v>
+        <v>4.6399999999999997E-2</v>
       </c>
       <c r="M51" s="13">
-        <v>4.6399999999999997E-2</v>
+        <v>4.3200000000000002E-2</v>
       </c>
       <c r="N51" s="13">
-        <v>4.3200000000000002E-2</v>
-      </c>
-      <c r="O51" s="13">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="P51" s="17">
-        <v>0</v>
+      <c r="O51" s="17">
+        <v>0</v>
+      </c>
+      <c r="P51" s="13">
+        <v>3.78E-2</v>
       </c>
       <c r="Q51" s="13">
-        <v>3.78E-2</v>
+        <v>3.5400000000000001E-2</v>
       </c>
       <c r="R51" s="13">
-        <v>3.5400000000000001E-2</v>
+        <v>3.3500000000000002E-2</v>
       </c>
       <c r="S51" s="13">
-        <v>3.3500000000000002E-2</v>
-      </c>
-      <c r="T51" s="13">
         <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="T51" s="17">
+        <v>0</v>
       </c>
       <c r="U51" s="8" t="s">
         <v>156</v>
@@ -4146,10 +4166,10 @@
     </row>
     <row r="52" spans="1:22" ht="16">
       <c r="A52" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C52" s="3">
         <v>4.6199999999999998E-2</v>
@@ -4175,35 +4195,35 @@
       <c r="J52" s="17">
         <v>0</v>
       </c>
-      <c r="K52" s="17">
-        <v>0</v>
+      <c r="K52" s="13">
+        <v>7.3300000000000004E-2</v>
       </c>
       <c r="L52" s="13">
-        <v>7.3300000000000004E-2</v>
+        <v>6.4600000000000005E-2</v>
       </c>
       <c r="M52" s="13">
-        <v>6.4600000000000005E-2</v>
+        <v>6.0199999999999997E-2</v>
       </c>
       <c r="N52" s="13">
-        <v>6.0199999999999997E-2</v>
-      </c>
-      <c r="O52" s="13">
         <v>6.0900000000000003E-2</v>
       </c>
-      <c r="P52" s="17">
-        <v>0</v>
+      <c r="O52" s="17">
+        <v>0</v>
+      </c>
+      <c r="P52" s="13">
+        <v>5.2699999999999997E-2</v>
       </c>
       <c r="Q52" s="13">
-        <v>5.2699999999999997E-2</v>
+        <v>4.87E-2</v>
       </c>
       <c r="R52" s="13">
-        <v>4.87E-2</v>
+        <v>4.1599999999999998E-2</v>
       </c>
       <c r="S52" s="13">
-        <v>4.1599999999999998E-2</v>
-      </c>
-      <c r="T52" s="13">
         <v>4.7699999999999999E-2</v>
+      </c>
+      <c r="T52" s="17">
+        <v>0</v>
       </c>
       <c r="U52" s="8" t="s">
         <v>156</v>
@@ -4214,10 +4234,10 @@
     </row>
     <row r="53" spans="1:22" ht="16">
       <c r="A53" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C53" s="18">
         <v>0</v>
@@ -4233,14 +4253,20 @@
       </c>
       <c r="G53" s="17">
         <v>0</v>
+      </c>
+      <c r="U53" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="V53" s="7" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:22" ht="16">
       <c r="A54" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C54">
         <v>0.55620000000000003</v>
@@ -4258,13 +4284,19 @@
         <v>0</v>
       </c>
       <c r="H54" s="3"/>
+      <c r="U54" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="V54" s="7" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="55" spans="1:22" ht="16">
       <c r="A55" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C55">
         <v>0.60619999999999996</v>
@@ -4281,16 +4313,22 @@
       <c r="G55" s="17">
         <v>0</v>
       </c>
-      <c r="P55">
+      <c r="O55">
         <v>0.111</v>
+      </c>
+      <c r="U55" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="V55" s="7" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:22" ht="16">
       <c r="A56" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C56">
         <v>0.64229999999999998</v>
@@ -4307,13 +4345,19 @@
       <c r="G56" s="17">
         <v>0</v>
       </c>
+      <c r="U56" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="V56" s="7" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="57" spans="1:22" ht="16">
       <c r="A57" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C57">
         <v>0.6643</v>
@@ -4330,13 +4374,19 @@
       <c r="G57" s="17">
         <v>0</v>
       </c>
+      <c r="U57" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="V57" s="7" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="58" spans="1:22" ht="16">
       <c r="A58" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C58">
         <v>0.67290000000000005</v>
@@ -4353,60 +4403,96 @@
       <c r="G58" s="17">
         <v>0</v>
       </c>
+      <c r="U58" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="V58" s="7" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="59" spans="1:22" ht="16">
       <c r="A59" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>298</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>299</v>
       </c>
       <c r="H59" s="3">
         <v>9.9000000000000008E-3</v>
       </c>
+      <c r="U59" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="V59" s="7" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="60" spans="1:22" ht="16">
       <c r="A60" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H60" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
+      <c r="U60" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="V60" s="7" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="61" spans="1:22" ht="16">
       <c r="A61" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H61" s="3">
         <v>1.21E-2</v>
       </c>
+      <c r="U61" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="V61" s="7" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="62" spans="1:22" ht="16">
       <c r="A62" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H62" s="3">
         <v>1.32E-2</v>
       </c>
+      <c r="U62" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="V62" s="7" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="63" spans="1:22" ht="16">
       <c r="A63" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H63" s="3">
         <v>1.43E-2</v>
+      </c>
+      <c r="U63" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="V63" s="7" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4653,16 +4739,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B18" t="s">
         <v>269</v>
-      </c>
-      <c r="B18" t="s">
-        <v>270</v>
       </c>
       <c r="C18" s="3">
         <v>38700000</v>
       </c>
       <c r="H18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A little nicer :)
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1025,7 +1025,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1057,12 +1057,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFA6A9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1207,7 +1201,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1223,10 +1217,13 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="93" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="128">
     <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
@@ -1670,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3717,20 +3714,20 @@
       <c r="B44" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13">
+      <c r="C44" s="18"/>
+      <c r="D44" s="18">
         <v>1300</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="18">
         <v>1600</v>
       </c>
-      <c r="F44" s="13">
+      <c r="F44" s="18">
         <v>4200</v>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="18">
         <v>500</v>
       </c>
-      <c r="H44" s="13">
+      <c r="H44" s="18">
         <v>5000</v>
       </c>
       <c r="I44" s="13"/>
@@ -3749,22 +3746,22 @@
       <c r="B45" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="19">
         <v>75.349999999999994</v>
       </c>
-      <c r="D45" s="15">
-        <v>0</v>
-      </c>
-      <c r="E45" s="15">
-        <v>0</v>
-      </c>
-      <c r="F45" s="15">
-        <v>0</v>
-      </c>
-      <c r="G45" s="15">
-        <v>0</v>
-      </c>
-      <c r="H45" s="9">
+      <c r="D45" s="20">
+        <v>0</v>
+      </c>
+      <c r="E45" s="20">
+        <v>0</v>
+      </c>
+      <c r="F45" s="20">
+        <v>0</v>
+      </c>
+      <c r="G45" s="20">
+        <v>0</v>
+      </c>
+      <c r="H45" s="19">
         <v>70.63</v>
       </c>
       <c r="I45" s="9">
@@ -3787,12 +3784,16 @@
       <c r="B46" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="D46" s="13">
+      <c r="C46" s="21"/>
+      <c r="D46" s="18">
         <v>0.01</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="21">
         <v>0.93899999999999995</v>
       </c>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
       <c r="K46" s="3">
         <v>4.2000000000000003E-2</v>
       </c>
@@ -3831,7 +3832,7 @@
       <c r="B47" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="C47" s="16">
+      <c r="C47" s="15">
         <v>0</v>
       </c>
       <c r="D47" s="13">
@@ -3840,51 +3841,49 @@
       <c r="E47" s="3">
         <v>1.04E-2</v>
       </c>
-      <c r="F47" s="16">
+      <c r="F47" s="15">
         <v>0</v>
       </c>
       <c r="G47" s="13">
         <v>6.8199999999999997E-2</v>
       </c>
-      <c r="H47" s="17">
-        <v>0</v>
-      </c>
-      <c r="I47" s="17">
-        <v>0</v>
-      </c>
-      <c r="J47" s="17">
-        <v>0</v>
-      </c>
-      <c r="K47" s="17">
-        <v>0</v>
-      </c>
-      <c r="L47" s="17">
-        <v>0</v>
-      </c>
-      <c r="M47" s="17">
-        <v>0</v>
-      </c>
-      <c r="N47" s="17">
-        <v>0</v>
-      </c>
-      <c r="O47" s="17">
-        <v>0</v>
-      </c>
-      <c r="P47" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="17">
-        <v>0</v>
-      </c>
-      <c r="R47" s="17">
+      <c r="H47" s="16">
+        <v>0</v>
+      </c>
+      <c r="I47" s="16">
+        <v>0</v>
+      </c>
+      <c r="J47" s="16">
+        <v>0</v>
+      </c>
+      <c r="K47" s="16">
+        <v>0</v>
+      </c>
+      <c r="L47" s="16">
+        <v>0</v>
+      </c>
+      <c r="M47" s="16">
+        <v>0</v>
+      </c>
+      <c r="N47" s="16">
+        <v>0</v>
+      </c>
+      <c r="O47" s="16">
+        <v>0</v>
+      </c>
+      <c r="P47" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="16">
+        <v>0</v>
+      </c>
+      <c r="R47" s="16">
         <v>0</v>
       </c>
       <c r="S47" s="13">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="T47" s="17">
-        <v>0</v>
-      </c>
+      <c r="T47" s="18"/>
       <c r="U47" s="8" t="s">
         <v>156</v>
       </c>
@@ -3899,7 +3898,7 @@
       <c r="B48" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="C48" s="16">
+      <c r="C48" s="15">
         <v>0</v>
       </c>
       <c r="D48" s="13">
@@ -3908,40 +3907,40 @@
       <c r="E48" s="3">
         <v>2.18E-2</v>
       </c>
-      <c r="F48" s="16">
+      <c r="F48" s="15">
         <v>0</v>
       </c>
       <c r="G48" s="13">
         <v>0.1328</v>
       </c>
-      <c r="H48" s="17">
-        <v>0</v>
-      </c>
-      <c r="I48" s="17">
-        <v>0</v>
-      </c>
-      <c r="J48" s="17">
+      <c r="H48" s="16">
+        <v>0</v>
+      </c>
+      <c r="I48" s="16">
+        <v>0</v>
+      </c>
+      <c r="J48" s="16">
         <v>0</v>
       </c>
       <c r="K48" s="13">
         <v>1.0699999999999999E-2</v>
       </c>
-      <c r="L48" s="17">
-        <v>0</v>
-      </c>
-      <c r="M48" s="17">
-        <v>0</v>
-      </c>
-      <c r="N48" s="17">
-        <v>0</v>
-      </c>
-      <c r="O48" s="17">
-        <v>0</v>
-      </c>
-      <c r="P48" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="17">
+      <c r="L48" s="16">
+        <v>0</v>
+      </c>
+      <c r="M48" s="16">
+        <v>0</v>
+      </c>
+      <c r="N48" s="16">
+        <v>0</v>
+      </c>
+      <c r="O48" s="16">
+        <v>0</v>
+      </c>
+      <c r="P48" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="16">
         <v>0</v>
       </c>
       <c r="R48" s="13">
@@ -3950,9 +3949,7 @@
       <c r="S48" s="13">
         <v>1.8200000000000001E-2</v>
       </c>
-      <c r="T48" s="17">
-        <v>0</v>
-      </c>
+      <c r="T48" s="18"/>
       <c r="U48" s="8" t="s">
         <v>156</v>
       </c>
@@ -3982,13 +3979,13 @@
       <c r="G49" s="13">
         <v>0.18659999999999999</v>
       </c>
-      <c r="H49" s="17">
-        <v>0</v>
-      </c>
-      <c r="I49" s="17">
-        <v>0</v>
-      </c>
-      <c r="J49" s="17">
+      <c r="H49" s="16">
+        <v>0</v>
+      </c>
+      <c r="I49" s="16">
+        <v>0</v>
+      </c>
+      <c r="J49" s="16">
         <v>0</v>
       </c>
       <c r="K49" s="13">
@@ -4003,13 +4000,13 @@
       <c r="N49" s="13">
         <v>1.67E-2</v>
       </c>
-      <c r="O49" s="17">
-        <v>0</v>
-      </c>
-      <c r="P49" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="17">
+      <c r="O49" s="16">
+        <v>0</v>
+      </c>
+      <c r="P49" s="16">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="16">
         <v>0</v>
       </c>
       <c r="R49" s="13">
@@ -4018,9 +4015,7 @@
       <c r="S49" s="13">
         <v>2.6499999999999999E-2</v>
       </c>
-      <c r="T49" s="17">
-        <v>0</v>
-      </c>
+      <c r="T49" s="18"/>
       <c r="U49" s="8" t="s">
         <v>156</v>
       </c>
@@ -4050,13 +4045,13 @@
       <c r="G50" s="13">
         <v>0.23089999999999999</v>
       </c>
-      <c r="H50" s="17">
-        <v>0</v>
-      </c>
-      <c r="I50" s="17">
-        <v>0</v>
-      </c>
-      <c r="J50" s="17">
+      <c r="H50" s="16">
+        <v>0</v>
+      </c>
+      <c r="I50" s="16">
+        <v>0</v>
+      </c>
+      <c r="J50" s="16">
         <v>0</v>
       </c>
       <c r="K50" s="13">
@@ -4071,7 +4066,7 @@
       <c r="N50" s="13">
         <v>2.8299999999999999E-2</v>
       </c>
-      <c r="O50" s="17">
+      <c r="O50" s="16">
         <v>0</v>
       </c>
       <c r="P50" s="13">
@@ -4086,9 +4081,7 @@
       <c r="S50" s="13">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="T50" s="17">
-        <v>0</v>
-      </c>
+      <c r="T50" s="18"/>
       <c r="U50" s="8" t="s">
         <v>156</v>
       </c>
@@ -4118,13 +4111,13 @@
       <c r="G51" s="13">
         <v>0.27089999999999997</v>
       </c>
-      <c r="H51" s="17">
-        <v>0</v>
-      </c>
-      <c r="I51" s="17">
-        <v>0</v>
-      </c>
-      <c r="J51" s="17">
+      <c r="H51" s="16">
+        <v>0</v>
+      </c>
+      <c r="I51" s="16">
+        <v>0</v>
+      </c>
+      <c r="J51" s="16">
         <v>0</v>
       </c>
       <c r="K51" s="13">
@@ -4139,7 +4132,7 @@
       <c r="N51" s="13">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="O51" s="17">
+      <c r="O51" s="16">
         <v>0</v>
       </c>
       <c r="P51" s="13">
@@ -4154,9 +4147,7 @@
       <c r="S51" s="13">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="T51" s="17">
-        <v>0</v>
-      </c>
+      <c r="T51" s="18"/>
       <c r="U51" s="8" t="s">
         <v>156</v>
       </c>
@@ -4186,13 +4177,13 @@
       <c r="G52" s="13">
         <v>0.30909999999999999</v>
       </c>
-      <c r="H52" s="17">
-        <v>0</v>
-      </c>
-      <c r="I52" s="17">
-        <v>0</v>
-      </c>
-      <c r="J52" s="17">
+      <c r="H52" s="16">
+        <v>0</v>
+      </c>
+      <c r="I52" s="16">
+        <v>0</v>
+      </c>
+      <c r="J52" s="16">
         <v>0</v>
       </c>
       <c r="K52" s="13">
@@ -4207,7 +4198,7 @@
       <c r="N52" s="13">
         <v>6.0900000000000003E-2</v>
       </c>
-      <c r="O52" s="17">
+      <c r="O52" s="16">
         <v>0</v>
       </c>
       <c r="P52" s="13">
@@ -4222,9 +4213,7 @@
       <c r="S52" s="13">
         <v>4.7699999999999999E-2</v>
       </c>
-      <c r="T52" s="17">
-        <v>0</v>
-      </c>
+      <c r="T52" s="18"/>
       <c r="U52" s="8" t="s">
         <v>156</v>
       </c>
@@ -4239,19 +4228,19 @@
       <c r="B53" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="C53" s="18">
-        <v>0</v>
-      </c>
-      <c r="D53" s="17">
-        <v>0</v>
-      </c>
-      <c r="E53" s="18">
-        <v>0</v>
-      </c>
-      <c r="F53" s="18">
-        <v>0</v>
-      </c>
-      <c r="G53" s="17">
+      <c r="C53" s="17">
+        <v>0</v>
+      </c>
+      <c r="D53" s="16">
+        <v>0</v>
+      </c>
+      <c r="E53" s="17">
+        <v>0</v>
+      </c>
+      <c r="F53" s="17">
+        <v>0</v>
+      </c>
+      <c r="G53" s="16">
         <v>0</v>
       </c>
       <c r="U53" s="8" t="s">
@@ -4271,16 +4260,16 @@
       <c r="C54">
         <v>0.55620000000000003</v>
       </c>
-      <c r="D54" s="17">
-        <v>0</v>
-      </c>
-      <c r="E54" s="18">
-        <v>0</v>
-      </c>
-      <c r="F54" s="18">
-        <v>0</v>
-      </c>
-      <c r="G54" s="17">
+      <c r="D54" s="16">
+        <v>0</v>
+      </c>
+      <c r="E54" s="17">
+        <v>0</v>
+      </c>
+      <c r="F54" s="17">
+        <v>0</v>
+      </c>
+      <c r="G54" s="16">
         <v>0</v>
       </c>
       <c r="H54" s="3"/>
@@ -4301,16 +4290,16 @@
       <c r="C55">
         <v>0.60619999999999996</v>
       </c>
-      <c r="D55" s="17">
-        <v>0</v>
-      </c>
-      <c r="E55" s="18">
-        <v>0</v>
-      </c>
-      <c r="F55" s="18">
-        <v>0</v>
-      </c>
-      <c r="G55" s="17">
+      <c r="D55" s="16">
+        <v>0</v>
+      </c>
+      <c r="E55" s="17">
+        <v>0</v>
+      </c>
+      <c r="F55" s="17">
+        <v>0</v>
+      </c>
+      <c r="G55" s="16">
         <v>0</v>
       </c>
       <c r="O55">
@@ -4333,16 +4322,16 @@
       <c r="C56">
         <v>0.64229999999999998</v>
       </c>
-      <c r="D56" s="17">
-        <v>0</v>
-      </c>
-      <c r="E56" s="18">
-        <v>0</v>
-      </c>
-      <c r="F56" s="18">
-        <v>0</v>
-      </c>
-      <c r="G56" s="17">
+      <c r="D56" s="16">
+        <v>0</v>
+      </c>
+      <c r="E56" s="17">
+        <v>0</v>
+      </c>
+      <c r="F56" s="17">
+        <v>0</v>
+      </c>
+      <c r="G56" s="16">
         <v>0</v>
       </c>
       <c r="U56" s="8" t="s">
@@ -4362,16 +4351,16 @@
       <c r="C57">
         <v>0.6643</v>
       </c>
-      <c r="D57" s="17">
-        <v>0</v>
-      </c>
-      <c r="E57" s="18">
-        <v>0</v>
-      </c>
-      <c r="F57" s="18">
-        <v>0</v>
-      </c>
-      <c r="G57" s="17">
+      <c r="D57" s="16">
+        <v>0</v>
+      </c>
+      <c r="E57" s="17">
+        <v>0</v>
+      </c>
+      <c r="F57" s="17">
+        <v>0</v>
+      </c>
+      <c r="G57" s="16">
         <v>0</v>
       </c>
       <c r="U57" s="8" t="s">
@@ -4391,16 +4380,16 @@
       <c r="C58">
         <v>0.67290000000000005</v>
       </c>
-      <c r="D58" s="17">
-        <v>0</v>
-      </c>
-      <c r="E58" s="18">
-        <v>0</v>
-      </c>
-      <c r="F58" s="18">
-        <v>0</v>
-      </c>
-      <c r="G58" s="17">
+      <c r="D58" s="16">
+        <v>0</v>
+      </c>
+      <c r="E58" s="17">
+        <v>0</v>
+      </c>
+      <c r="F58" s="17">
+        <v>0</v>
+      </c>
+      <c r="G58" s="16">
         <v>0</v>
       </c>
       <c r="U58" s="8" t="s">

</xml_diff>

<commit_message>
Not done yet, on the way
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="306">
   <si>
     <t>parvariable</t>
   </si>
@@ -866,9 +866,6 @@
     <t>Thermal conductivity of gas at 600K</t>
   </si>
   <si>
-    <t>Thermal conductivity of liquid at 248.16K</t>
-  </si>
-  <si>
     <t>lambdagas100</t>
   </si>
   <si>
@@ -885,9 +882,6 @@
   </si>
   <si>
     <t>lambdagas600</t>
-  </si>
-  <si>
-    <t>lambdaliq248</t>
   </si>
   <si>
     <t>lambdaliq273</t>
@@ -1071,7 +1065,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="128">
+  <cellStyleXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1166,6 +1160,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1225,7 +1223,7 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="128">
+  <cellStyles count="132">
     <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
@@ -1290,6 +1288,8 @@
     <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1353,6 +1353,8 @@
     <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1665,10 +1667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V63"/>
+  <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44:H46"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3830,7 +3832,7 @@
         <v>273</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C47" s="15">
         <v>0</v>
@@ -3896,7 +3898,7 @@
         <v>274</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C48" s="15">
         <v>0</v>
@@ -3962,7 +3964,7 @@
         <v>275</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C49" s="3">
         <v>1.8599999999999998E-2</v>
@@ -4028,7 +4030,7 @@
         <v>276</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C50" s="3">
         <v>2.6100000000000002E-2</v>
@@ -4094,7 +4096,7 @@
         <v>277</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C51" s="3">
         <v>3.56E-2</v>
@@ -4160,7 +4162,7 @@
         <v>278</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C52" s="3">
         <v>4.6199999999999998E-2</v>
@@ -4223,13 +4225,13 @@
     </row>
     <row r="53" spans="1:22" ht="16">
       <c r="A53" s="1" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="C53" s="17">
-        <v>0</v>
+        <v>285</v>
+      </c>
+      <c r="C53">
+        <v>0.55620000000000003</v>
       </c>
       <c r="D53" s="16">
         <v>0</v>
@@ -4243,8 +4245,9 @@
       <c r="G53" s="16">
         <v>0</v>
       </c>
+      <c r="H53" s="3"/>
       <c r="U53" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V53" s="7" t="s">
         <v>135</v>
@@ -4252,13 +4255,13 @@
     </row>
     <row r="54" spans="1:22" ht="16">
       <c r="A54" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C54">
-        <v>0.55620000000000003</v>
+        <v>0.60619999999999996</v>
       </c>
       <c r="D54" s="16">
         <v>0</v>
@@ -4272,9 +4275,11 @@
       <c r="G54" s="16">
         <v>0</v>
       </c>
-      <c r="H54" s="3"/>
+      <c r="O54">
+        <v>0.111</v>
+      </c>
       <c r="U54" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V54" s="7" t="s">
         <v>135</v>
@@ -4282,13 +4287,13 @@
     </row>
     <row r="55" spans="1:22" ht="16">
       <c r="A55" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C55">
-        <v>0.60619999999999996</v>
+        <v>0.64229999999999998</v>
       </c>
       <c r="D55" s="16">
         <v>0</v>
@@ -4302,11 +4307,8 @@
       <c r="G55" s="16">
         <v>0</v>
       </c>
-      <c r="O55">
-        <v>0.111</v>
-      </c>
       <c r="U55" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V55" s="7" t="s">
         <v>135</v>
@@ -4314,13 +4316,13 @@
     </row>
     <row r="56" spans="1:22" ht="16">
       <c r="A56" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C56">
-        <v>0.64229999999999998</v>
+        <v>0.6643</v>
       </c>
       <c r="D56" s="16">
         <v>0</v>
@@ -4335,7 +4337,7 @@
         <v>0</v>
       </c>
       <c r="U56" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V56" s="7" t="s">
         <v>135</v>
@@ -4343,13 +4345,13 @@
     </row>
     <row r="57" spans="1:22" ht="16">
       <c r="A57" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C57">
-        <v>0.6643</v>
+        <v>0.67290000000000005</v>
       </c>
       <c r="D57" s="16">
         <v>0</v>
@@ -4364,7 +4366,7 @@
         <v>0</v>
       </c>
       <c r="U57" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V57" s="7" t="s">
         <v>135</v>
@@ -4372,45 +4374,33 @@
     </row>
     <row r="58" spans="1:22" ht="16">
       <c r="A58" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B58" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C58">
-        <v>0.67290000000000005</v>
-      </c>
-      <c r="D58" s="16">
-        <v>0</v>
-      </c>
-      <c r="E58" s="17">
-        <v>0</v>
-      </c>
-      <c r="F58" s="17">
-        <v>0</v>
-      </c>
-      <c r="G58" s="16">
-        <v>0</v>
+      <c r="H58" s="3">
+        <v>9.9000000000000008E-3</v>
       </c>
       <c r="U58" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V58" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:22" ht="16">
       <c r="A59" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="B59" s="7" t="s">
-        <v>298</v>
-      </c>
       <c r="H59" s="3">
-        <v>9.9000000000000008E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="U59" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V59" s="7" t="s">
         <v>136</v>
@@ -4418,16 +4408,16 @@
     </row>
     <row r="60" spans="1:22" ht="16">
       <c r="A60" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H60" s="3">
-        <v>1.0999999999999999E-2</v>
+        <v>1.21E-2</v>
       </c>
       <c r="U60" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V60" s="7" t="s">
         <v>136</v>
@@ -4435,16 +4425,16 @@
     </row>
     <row r="61" spans="1:22" ht="16">
       <c r="A61" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H61" s="3">
-        <v>1.21E-2</v>
+        <v>1.32E-2</v>
       </c>
       <c r="U61" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V61" s="7" t="s">
         <v>136</v>
@@ -4452,35 +4442,18 @@
     </row>
     <row r="62" spans="1:22" ht="16">
       <c r="A62" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="H62" s="3">
+        <v>1.43E-2</v>
+      </c>
+      <c r="U62" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="H62" s="3">
-        <v>1.32E-2</v>
-      </c>
-      <c r="U62" s="8" t="s">
-        <v>307</v>
-      </c>
       <c r="V62" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="63" spans="1:22" ht="16">
-      <c r="A63" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="H63" s="3">
-        <v>1.43E-2</v>
-      </c>
-      <c r="U63" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="V63" s="7" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel and reaction update
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,33 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB04C737-D6CF-DF46-BB67-0B075175ACC7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="310">
   <si>
     <t>parvariable</t>
   </si>
@@ -945,16 +951,28 @@
   </si>
   <si>
     <t>W.m-1.K-1</t>
+  </si>
+  <si>
+    <t>SegmentArea</t>
+  </si>
+  <si>
+    <t>Aq</t>
+  </si>
+  <si>
+    <t>Surface Area</t>
+  </si>
+  <si>
+    <t>As</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1224,137 +1242,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="132">
-    <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Bad" xfId="93" builtinId="27"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1659,28 +1677,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="75" workbookViewId="0">
       <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
     <col min="10" max="10" width="18.83203125" customWidth="1"/>
@@ -1764,7 +1782,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="16">
+    <row r="2" spans="1:22">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1827,7 +1845,7 @@
       </c>
       <c r="U2" s="7"/>
     </row>
-    <row r="3" spans="1:22" ht="16">
+    <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1890,7 +1908,7 @@
       </c>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:22" ht="16">
+    <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -1951,7 +1969,7 @@
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:22" ht="16">
+    <row r="5" spans="1:22">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -1999,7 +2017,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="16">
+    <row r="6" spans="1:22">
       <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
@@ -2043,7 +2061,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="16">
+    <row r="7" spans="1:22">
       <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
@@ -2087,7 +2105,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="16">
+    <row r="8" spans="1:22">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -2131,7 +2149,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="16">
+    <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -2175,7 +2193,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="16">
+    <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -2219,7 +2237,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="16">
+    <row r="11" spans="1:22">
       <c r="A11" s="1" t="s">
         <v>127</v>
       </c>
@@ -2263,7 +2281,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="16">
+    <row r="12" spans="1:22">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -2329,7 +2347,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="16">
+    <row r="13" spans="1:22">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2356,7 +2374,7 @@
       <c r="T13" s="9"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:22" ht="16">
+    <row r="14" spans="1:22">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -2404,7 +2422,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="16">
+    <row r="15" spans="1:22">
       <c r="A15" s="1" t="s">
         <v>110</v>
       </c>
@@ -2450,7 +2468,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="16">
+    <row r="16" spans="1:22">
       <c r="A16" s="1" t="s">
         <v>143</v>
       </c>
@@ -2490,7 +2508,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="16">
+    <row r="17" spans="1:22">
       <c r="A17" s="1" t="s">
         <v>141</v>
       </c>
@@ -2521,7 +2539,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="16">
+    <row r="18" spans="1:22">
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
@@ -2569,7 +2587,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="16">
+    <row r="19" spans="1:22">
       <c r="A19" s="1" t="s">
         <v>159</v>
       </c>
@@ -2617,7 +2635,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="16">
+    <row r="20" spans="1:22">
       <c r="A20" s="1" t="s">
         <v>162</v>
       </c>
@@ -2665,7 +2683,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="16">
+    <row r="21" spans="1:22">
       <c r="A21" s="1" t="s">
         <v>168</v>
       </c>
@@ -2711,7 +2729,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="16">
+    <row r="22" spans="1:22">
       <c r="A22" s="1" t="s">
         <v>169</v>
       </c>
@@ -2757,7 +2775,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="16">
+    <row r="23" spans="1:22">
       <c r="A23" s="1" t="s">
         <v>175</v>
       </c>
@@ -2801,7 +2819,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="16">
+    <row r="24" spans="1:22">
       <c r="A24" s="1" t="s">
         <v>177</v>
       </c>
@@ -2845,7 +2863,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="16">
+    <row r="25" spans="1:22">
       <c r="A25" s="1" t="s">
         <v>186</v>
       </c>
@@ -2907,7 +2925,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="16">
+    <row r="26" spans="1:22">
       <c r="A26" s="1" t="s">
         <v>188</v>
       </c>
@@ -2969,7 +2987,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="16">
+    <row r="27" spans="1:22">
       <c r="A27" s="1" t="s">
         <v>190</v>
       </c>
@@ -3013,7 +3031,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="16">
+    <row r="28" spans="1:22">
       <c r="A28" s="1" t="s">
         <v>196</v>
       </c>
@@ -3072,7 +3090,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="16">
+    <row r="29" spans="1:22">
       <c r="A29" s="1" t="s">
         <v>210</v>
       </c>
@@ -3114,7 +3132,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="16">
+    <row r="30" spans="1:22">
       <c r="A30" s="1" t="s">
         <v>211</v>
       </c>
@@ -3158,7 +3176,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="16">
+    <row r="31" spans="1:22">
       <c r="A31" s="1" t="s">
         <v>208</v>
       </c>
@@ -3202,7 +3220,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="16">
+    <row r="32" spans="1:22">
       <c r="A32" s="1" t="s">
         <v>209</v>
       </c>
@@ -3246,7 +3264,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="16">
+    <row r="33" spans="1:22">
       <c r="A33" s="1" t="s">
         <v>212</v>
       </c>
@@ -3290,7 +3308,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="16">
+    <row r="34" spans="1:22">
       <c r="A34" s="1" t="s">
         <v>218</v>
       </c>
@@ -3334,7 +3352,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="16">
+    <row r="35" spans="1:22">
       <c r="A35" s="1" t="s">
         <v>219</v>
       </c>
@@ -3375,7 +3393,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="16">
+    <row r="36" spans="1:22">
       <c r="A36" s="1" t="s">
         <v>215</v>
       </c>
@@ -3416,7 +3434,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="16">
+    <row r="37" spans="1:22">
       <c r="A37" s="1" t="s">
         <v>216</v>
       </c>
@@ -3460,7 +3478,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="16">
+    <row r="38" spans="1:22">
       <c r="A38" s="1" t="s">
         <v>213</v>
       </c>
@@ -3504,7 +3522,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="16">
+    <row r="39" spans="1:22">
       <c r="A39" s="1" t="s">
         <v>214</v>
       </c>
@@ -3548,7 +3566,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="16">
+    <row r="40" spans="1:22">
       <c r="A40" s="1" t="s">
         <v>217</v>
       </c>
@@ -3592,7 +3610,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="16">
+    <row r="41" spans="1:22">
       <c r="A41" s="1" t="s">
         <v>222</v>
       </c>
@@ -3636,7 +3654,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="16">
+    <row r="42" spans="1:22">
       <c r="A42" s="1" t="s">
         <v>223</v>
       </c>
@@ -3677,7 +3695,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="16">
+    <row r="43" spans="1:22">
       <c r="A43" s="1" t="s">
         <v>229</v>
       </c>
@@ -3709,7 +3727,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="16">
+    <row r="44" spans="1:22">
       <c r="A44" s="1" t="s">
         <v>231</v>
       </c>
@@ -3741,7 +3759,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="16">
+    <row r="45" spans="1:22">
       <c r="A45" s="1" t="s">
         <v>240</v>
       </c>
@@ -3779,7 +3797,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="16">
+    <row r="46" spans="1:22">
       <c r="A46" s="1" t="s">
         <v>266</v>
       </c>
@@ -3827,7 +3845,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="16">
+    <row r="47" spans="1:22">
       <c r="A47" s="1" t="s">
         <v>273</v>
       </c>
@@ -3893,7 +3911,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:22" ht="16">
+    <row r="48" spans="1:22">
       <c r="A48" s="1" t="s">
         <v>274</v>
       </c>
@@ -3959,7 +3977,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="16">
+    <row r="49" spans="1:22">
       <c r="A49" s="1" t="s">
         <v>275</v>
       </c>
@@ -4025,7 +4043,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="16">
+    <row r="50" spans="1:22">
       <c r="A50" s="1" t="s">
         <v>276</v>
       </c>
@@ -4091,7 +4109,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:22" ht="16">
+    <row r="51" spans="1:22">
       <c r="A51" s="1" t="s">
         <v>277</v>
       </c>
@@ -4157,7 +4175,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:22" ht="16">
+    <row r="52" spans="1:22">
       <c r="A52" s="1" t="s">
         <v>278</v>
       </c>
@@ -4223,7 +4241,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:22" ht="16">
+    <row r="53" spans="1:22">
       <c r="A53" s="1" t="s">
         <v>290</v>
       </c>
@@ -4253,7 +4271,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:22" ht="16">
+    <row r="54" spans="1:22">
       <c r="A54" s="1" t="s">
         <v>291</v>
       </c>
@@ -4285,7 +4303,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:22" ht="16">
+    <row r="55" spans="1:22">
       <c r="A55" s="1" t="s">
         <v>292</v>
       </c>
@@ -4314,7 +4332,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:22" ht="16">
+    <row r="56" spans="1:22">
       <c r="A56" s="1" t="s">
         <v>293</v>
       </c>
@@ -4343,7 +4361,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:22" ht="16">
+    <row r="57" spans="1:22">
       <c r="A57" s="1" t="s">
         <v>294</v>
       </c>
@@ -4372,7 +4390,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:22" ht="16">
+    <row r="58" spans="1:22">
       <c r="A58" s="1" t="s">
         <v>295</v>
       </c>
@@ -4389,7 +4407,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:22" ht="16">
+    <row r="59" spans="1:22">
       <c r="A59" s="1" t="s">
         <v>301</v>
       </c>
@@ -4406,7 +4424,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:22" ht="16">
+    <row r="60" spans="1:22">
       <c r="A60" s="1" t="s">
         <v>302</v>
       </c>
@@ -4423,7 +4441,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:22" ht="16">
+    <row r="61" spans="1:22">
       <c r="A61" s="1" t="s">
         <v>303</v>
       </c>
@@ -4440,7 +4458,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:22" ht="16">
+    <row r="62" spans="1:22">
       <c r="A62" s="1" t="s">
         <v>304</v>
       </c>
@@ -4469,14 +4487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="29.1640625" style="1" customWidth="1"/>
   </cols>
@@ -4571,6 +4589,9 @@
       <c r="B5" t="s">
         <v>47</v>
       </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
@@ -4579,137 +4600,159 @@
       <c r="B6" t="s">
         <v>46</v>
       </c>
+      <c r="C6">
+        <v>1.4999999999999999E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>308</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>306</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="3"/>
+        <v>307</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>51</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <f>10*365*24*3600</f>
         <v>315360000</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H15" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" t="s">
-        <v>171</v>
-      </c>
-      <c r="C15">
-        <v>229410</v>
-      </c>
-      <c r="H15" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C16">
-        <v>91880</v>
-      </c>
-      <c r="H16" t="s">
-        <v>164</v>
+        <v>61</v>
+      </c>
+      <c r="F16">
+        <v>0.74</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>226</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
-        <v>227</v>
-      </c>
-      <c r="G17">
-        <v>8.3140000000000001</v>
+        <v>171</v>
+      </c>
+      <c r="C17">
+        <v>229410</v>
       </c>
       <c r="H17" t="s">
-        <v>129</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18">
+        <v>91880</v>
+      </c>
+      <c r="H18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B19" t="s">
+        <v>227</v>
+      </c>
+      <c r="G19">
+        <v>8.3140000000000001</v>
+      </c>
+      <c r="H19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>269</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C20" s="3">
         <v>38700000</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H20" t="s">
         <v>270</v>
       </c>
     </row>
@@ -4725,14 +4768,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Sieht noch nicht gut aus, aber sollte funktionieren
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,39 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB04C737-D6CF-DF46-BB67-0B075175ACC7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="313">
   <si>
     <t>parvariable</t>
   </si>
@@ -963,16 +957,25 @@
   </si>
   <si>
     <t>As</t>
+  </si>
+  <si>
+    <t>Thermal conductivity of liquid at 300K</t>
+  </si>
+  <si>
+    <t>lambdaliq300</t>
+  </si>
+  <si>
+    <t>EngineeringToolBox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1242,137 +1245,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="132">
-    <cellStyle name="Bad" xfId="93" builtinId="27"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1677,21 +1680,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="75" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:XFD53"/>
+    <sheetView tabSelected="1" topLeftCell="E36" zoomScale="75" workbookViewId="0">
+      <selection activeCell="V63" sqref="V63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -1782,7 +1785,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" ht="16">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1845,7 +1848,7 @@
       </c>
       <c r="U2" s="7"/>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" ht="16">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1908,7 +1911,7 @@
       </c>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" ht="16">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -1969,7 +1972,7 @@
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" ht="16">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" ht="16">
       <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" ht="16">
       <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
@@ -2105,7 +2108,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" ht="16">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -2149,7 +2152,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" ht="16">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -2193,7 +2196,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" ht="16">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" ht="16">
       <c r="A11" s="1" t="s">
         <v>127</v>
       </c>
@@ -2281,7 +2284,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" ht="16">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -2347,7 +2350,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" ht="16">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2374,7 +2377,7 @@
       <c r="T13" s="9"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" ht="16">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" ht="16">
       <c r="A15" s="1" t="s">
         <v>110</v>
       </c>
@@ -2468,7 +2471,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" ht="16">
       <c r="A16" s="1" t="s">
         <v>143</v>
       </c>
@@ -2508,7 +2511,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" ht="16">
       <c r="A17" s="1" t="s">
         <v>141</v>
       </c>
@@ -2539,7 +2542,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" ht="16">
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" ht="16">
       <c r="A19" s="1" t="s">
         <v>159</v>
       </c>
@@ -2635,7 +2638,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" ht="16">
       <c r="A20" s="1" t="s">
         <v>162</v>
       </c>
@@ -2683,7 +2686,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" ht="16">
       <c r="A21" s="1" t="s">
         <v>168</v>
       </c>
@@ -2729,7 +2732,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" ht="16">
       <c r="A22" s="1" t="s">
         <v>169</v>
       </c>
@@ -2775,7 +2778,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" ht="16">
       <c r="A23" s="1" t="s">
         <v>175</v>
       </c>
@@ -2819,7 +2822,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" ht="16">
       <c r="A24" s="1" t="s">
         <v>177</v>
       </c>
@@ -2863,7 +2866,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" ht="16">
       <c r="A25" s="1" t="s">
         <v>186</v>
       </c>
@@ -2925,7 +2928,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" ht="16">
       <c r="A26" s="1" t="s">
         <v>188</v>
       </c>
@@ -2987,7 +2990,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" ht="16">
       <c r="A27" s="1" t="s">
         <v>190</v>
       </c>
@@ -3031,7 +3034,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" ht="16">
       <c r="A28" s="1" t="s">
         <v>196</v>
       </c>
@@ -3090,7 +3093,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" ht="16">
       <c r="A29" s="1" t="s">
         <v>210</v>
       </c>
@@ -3132,7 +3135,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" ht="16">
       <c r="A30" s="1" t="s">
         <v>211</v>
       </c>
@@ -3176,7 +3179,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" ht="16">
       <c r="A31" s="1" t="s">
         <v>208</v>
       </c>
@@ -3220,7 +3223,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" ht="16">
       <c r="A32" s="1" t="s">
         <v>209</v>
       </c>
@@ -3264,7 +3267,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:22" ht="16">
       <c r="A33" s="1" t="s">
         <v>212</v>
       </c>
@@ -3308,7 +3311,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:22" ht="16">
       <c r="A34" s="1" t="s">
         <v>218</v>
       </c>
@@ -3352,7 +3355,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:22" ht="16">
       <c r="A35" s="1" t="s">
         <v>219</v>
       </c>
@@ -3393,7 +3396,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:22" ht="16">
       <c r="A36" s="1" t="s">
         <v>215</v>
       </c>
@@ -3434,7 +3437,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:22" ht="16">
       <c r="A37" s="1" t="s">
         <v>216</v>
       </c>
@@ -3478,7 +3481,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="38" spans="1:22">
+    <row r="38" spans="1:22" ht="16">
       <c r="A38" s="1" t="s">
         <v>213</v>
       </c>
@@ -3522,7 +3525,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:22">
+    <row r="39" spans="1:22" ht="16">
       <c r="A39" s="1" t="s">
         <v>214</v>
       </c>
@@ -3566,7 +3569,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:22">
+    <row r="40" spans="1:22" ht="16">
       <c r="A40" s="1" t="s">
         <v>217</v>
       </c>
@@ -3610,7 +3613,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="41" spans="1:22">
+    <row r="41" spans="1:22" ht="16">
       <c r="A41" s="1" t="s">
         <v>222</v>
       </c>
@@ -3654,7 +3657,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="1:22">
+    <row r="42" spans="1:22" ht="16">
       <c r="A42" s="1" t="s">
         <v>223</v>
       </c>
@@ -3695,7 +3698,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:22">
+    <row r="43" spans="1:22" ht="16">
       <c r="A43" s="1" t="s">
         <v>229</v>
       </c>
@@ -3727,7 +3730,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="44" spans="1:22">
+    <row r="44" spans="1:22" ht="16">
       <c r="A44" s="1" t="s">
         <v>231</v>
       </c>
@@ -3759,7 +3762,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="45" spans="1:22">
+    <row r="45" spans="1:22" ht="16">
       <c r="A45" s="1" t="s">
         <v>240</v>
       </c>
@@ -3797,7 +3800,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:22">
+    <row r="46" spans="1:22" ht="16">
       <c r="A46" s="1" t="s">
         <v>266</v>
       </c>
@@ -3845,7 +3848,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="47" spans="1:22">
+    <row r="47" spans="1:22" ht="16">
       <c r="A47" s="1" t="s">
         <v>273</v>
       </c>
@@ -3911,7 +3914,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:22">
+    <row r="48" spans="1:22" ht="16">
       <c r="A48" s="1" t="s">
         <v>274</v>
       </c>
@@ -3977,7 +3980,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:22">
+    <row r="49" spans="1:22" ht="16">
       <c r="A49" s="1" t="s">
         <v>275</v>
       </c>
@@ -4043,7 +4046,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:22">
+    <row r="50" spans="1:22" ht="16">
       <c r="A50" s="1" t="s">
         <v>276</v>
       </c>
@@ -4109,7 +4112,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:22">
+    <row r="51" spans="1:22" ht="16">
       <c r="A51" s="1" t="s">
         <v>277</v>
       </c>
@@ -4175,7 +4178,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:22">
+    <row r="52" spans="1:22" ht="16">
       <c r="A52" s="1" t="s">
         <v>278</v>
       </c>
@@ -4241,7 +4244,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:22">
+    <row r="53" spans="1:22" ht="16">
       <c r="A53" s="1" t="s">
         <v>290</v>
       </c>
@@ -4271,7 +4274,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:22">
+    <row r="54" spans="1:22" ht="16">
       <c r="A54" s="1" t="s">
         <v>291</v>
       </c>
@@ -4303,7 +4306,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:22">
+    <row r="55" spans="1:22" ht="16">
       <c r="A55" s="1" t="s">
         <v>292</v>
       </c>
@@ -4332,7 +4335,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:22">
+    <row r="56" spans="1:22" ht="16">
       <c r="A56" s="1" t="s">
         <v>293</v>
       </c>
@@ -4361,7 +4364,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:22">
+    <row r="57" spans="1:22" ht="16">
       <c r="A57" s="1" t="s">
         <v>294</v>
       </c>
@@ -4390,7 +4393,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:22">
+    <row r="58" spans="1:22" ht="16">
       <c r="A58" s="1" t="s">
         <v>295</v>
       </c>
@@ -4407,7 +4410,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:22">
+    <row r="59" spans="1:22" ht="16">
       <c r="A59" s="1" t="s">
         <v>301</v>
       </c>
@@ -4424,7 +4427,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:22">
+    <row r="60" spans="1:22" ht="16">
       <c r="A60" s="1" t="s">
         <v>302</v>
       </c>
@@ -4441,7 +4444,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:22">
+    <row r="61" spans="1:22" ht="16">
       <c r="A61" s="1" t="s">
         <v>303</v>
       </c>
@@ -4458,7 +4461,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:22">
+    <row r="62" spans="1:22" ht="16">
       <c r="A62" s="1" t="s">
         <v>304</v>
       </c>
@@ -4473,6 +4476,23 @@
       </c>
       <c r="V62" s="7" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" ht="16">
+      <c r="A63" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="I63">
+        <v>0.5</v>
+      </c>
+      <c r="U63" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="V63" s="7" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -4487,14 +4507,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.1640625" style="1" customWidth="1"/>
   </cols>
@@ -4768,14 +4788,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Dynamic viscosity of liquids
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="338">
   <si>
     <t>parvariable</t>
   </si>
@@ -1005,6 +1005,42 @@
   </si>
   <si>
     <t>Pa.s</t>
+  </si>
+  <si>
+    <t>Dynamic viscosity of liquid at 273.16 K</t>
+  </si>
+  <si>
+    <t>muliq273</t>
+  </si>
+  <si>
+    <t>Dynamic viscosity of liquid at 298.16 K</t>
+  </si>
+  <si>
+    <t>Dynamic viscosity of liquid at 323.16 K</t>
+  </si>
+  <si>
+    <t>Dynamic viscosity of liquid at 348.16 K</t>
+  </si>
+  <si>
+    <t>Dynamic viscosity of liquid at 373.16 K</t>
+  </si>
+  <si>
+    <t>muliq298</t>
+  </si>
+  <si>
+    <t>muliq323</t>
+  </si>
+  <si>
+    <t>muliq348</t>
+  </si>
+  <si>
+    <t>muliq373</t>
+  </si>
+  <si>
+    <t>Dynamic viscosity of liquid at 248.16 K</t>
+  </si>
+  <si>
+    <t>muliq248</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1172,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="144">
+  <cellStyleXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1281,8 +1317,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1308,8 +1350,9 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="144">
+  <cellStyles count="150">
     <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
@@ -1382,6 +1425,9 @@
     <cellStyle name="Lien hypertexte" xfId="138" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="140" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="148" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1453,6 +1499,9 @@
     <cellStyle name="Lien hypertexte visité" xfId="139" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="149" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1765,10 +1814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V76"/>
+  <dimension ref="A1:V75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D36" zoomScale="75" workbookViewId="0">
-      <selection activeCell="S70" sqref="S70"/>
+    <sheetView tabSelected="1" topLeftCell="E48" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76:W86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4963,7 +5012,43 @@
       </c>
     </row>
     <row r="70" spans="1:22" ht="16">
-      <c r="H70" s="3"/>
+      <c r="A70" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C70" s="24">
+        <v>0</v>
+      </c>
+      <c r="D70" s="24">
+        <v>0</v>
+      </c>
+      <c r="E70" s="24">
+        <v>0</v>
+      </c>
+      <c r="F70" s="24">
+        <v>0</v>
+      </c>
+      <c r="G70" s="24">
+        <v>0</v>
+      </c>
+      <c r="H70" s="24">
+        <v>0</v>
+      </c>
+      <c r="I70" s="25"/>
+      <c r="J70" s="25"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="25">
+        <v>3.7599999999999998E-4</v>
+      </c>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="3"/>
       <c r="U70" s="8" t="s">
         <v>325</v>
       </c>
@@ -4972,6 +5057,33 @@
       </c>
     </row>
     <row r="71" spans="1:22" ht="16">
+      <c r="A71" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C71" s="3">
+        <v>1.7930000000000001E-3</v>
+      </c>
+      <c r="D71" s="24">
+        <v>0</v>
+      </c>
+      <c r="E71" s="24">
+        <v>0</v>
+      </c>
+      <c r="F71" s="24">
+        <v>0</v>
+      </c>
+      <c r="G71" s="24">
+        <v>0</v>
+      </c>
+      <c r="H71" s="3">
+        <v>2.3499999999999999E-4</v>
+      </c>
+      <c r="O71" s="3">
+        <v>2.7700000000000001E-4</v>
+      </c>
       <c r="U71" s="8" t="s">
         <v>325</v>
       </c>
@@ -4980,6 +5092,33 @@
       </c>
     </row>
     <row r="72" spans="1:22" ht="16">
+      <c r="A72" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C72" s="3">
+        <v>8.8999999999999995E-4</v>
+      </c>
+      <c r="D72" s="24">
+        <v>0</v>
+      </c>
+      <c r="E72" s="24">
+        <v>0</v>
+      </c>
+      <c r="F72" s="24">
+        <v>0</v>
+      </c>
+      <c r="G72" s="24">
+        <v>0</v>
+      </c>
+      <c r="H72" s="3">
+        <v>1.83E-4</v>
+      </c>
+      <c r="O72" s="3">
+        <v>2.14E-4</v>
+      </c>
       <c r="U72" s="8" t="s">
         <v>325</v>
       </c>
@@ -4988,6 +5127,27 @@
       </c>
     </row>
     <row r="73" spans="1:22" ht="16">
+      <c r="A73" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C73" s="3">
+        <v>5.4699999999999996E-4</v>
+      </c>
+      <c r="D73" s="24">
+        <v>0</v>
+      </c>
+      <c r="E73" s="24">
+        <v>0</v>
+      </c>
+      <c r="F73" s="24">
+        <v>0</v>
+      </c>
+      <c r="G73" s="24">
+        <v>0</v>
+      </c>
       <c r="U73" s="8" t="s">
         <v>325</v>
       </c>
@@ -4996,6 +5156,27 @@
       </c>
     </row>
     <row r="74" spans="1:22" ht="16">
+      <c r="A74" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="C74" s="3">
+        <v>3.7800000000000003E-4</v>
+      </c>
+      <c r="D74" s="24">
+        <v>0</v>
+      </c>
+      <c r="E74" s="24">
+        <v>0</v>
+      </c>
+      <c r="F74" s="24">
+        <v>0</v>
+      </c>
+      <c r="G74" s="24">
+        <v>0</v>
+      </c>
       <c r="U74" s="8" t="s">
         <v>325</v>
       </c>
@@ -5004,18 +5185,31 @@
       </c>
     </row>
     <row r="75" spans="1:22" ht="16">
+      <c r="A75" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="C75" s="3">
+        <v>2.8200000000000002E-4</v>
+      </c>
+      <c r="D75" s="24">
+        <v>0</v>
+      </c>
+      <c r="E75" s="24">
+        <v>0</v>
+      </c>
+      <c r="F75" s="24">
+        <v>0</v>
+      </c>
+      <c r="G75" s="24">
+        <v>0</v>
+      </c>
       <c r="U75" s="8" t="s">
         <v>325</v>
       </c>
       <c r="V75" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="76" spans="1:22" ht="16">
-      <c r="U76" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="V76" s="7" t="s">
         <v>135</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dynamic viscosity function done
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1816,8 +1816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E48" zoomScale="75" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76:W86"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5036,7 +5036,9 @@
       <c r="H70" s="24">
         <v>0</v>
       </c>
-      <c r="I70" s="25"/>
+      <c r="I70" s="24">
+        <v>0</v>
+      </c>
       <c r="J70" s="25"/>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
@@ -5081,6 +5083,9 @@
       <c r="H71" s="3">
         <v>2.3499999999999999E-4</v>
       </c>
+      <c r="I71" s="24">
+        <v>0</v>
+      </c>
       <c r="O71" s="3">
         <v>2.7700000000000001E-4</v>
       </c>
@@ -5116,6 +5121,9 @@
       <c r="H72" s="3">
         <v>1.83E-4</v>
       </c>
+      <c r="I72" s="3">
+        <v>2.3800000000000002E-2</v>
+      </c>
       <c r="O72" s="3">
         <v>2.14E-4</v>
       </c>
@@ -5148,6 +5156,9 @@
       <c r="G73" s="24">
         <v>0</v>
       </c>
+      <c r="I73" s="3">
+        <v>1.17E-2</v>
+      </c>
       <c r="U73" s="8" t="s">
         <v>325</v>
       </c>
@@ -5177,6 +5188,9 @@
       <c r="G74" s="24">
         <v>0</v>
       </c>
+      <c r="I74" s="3">
+        <v>6.6E-3</v>
+      </c>
       <c r="U74" s="8" t="s">
         <v>325</v>
       </c>
@@ -5205,6 +5219,9 @@
       </c>
       <c r="G75" s="24">
         <v>0</v>
+      </c>
+      <c r="I75" s="3">
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="U75" s="8" t="s">
         <v>325</v>

</xml_diff>

<commit_message>
First implementation of energy balnce
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0120599E-C735-7743-85CB-5428A7636795}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -545,9 +551,6 @@
     <t>deltaHHCN</t>
   </si>
   <si>
-    <t>deltaHNH3</t>
-  </si>
-  <si>
     <t>Reaction enthalpy NH3</t>
   </si>
   <si>
@@ -1041,16 +1044,19 @@
   </si>
   <si>
     <t>muliq248</t>
+  </si>
+  <si>
+    <t>deltaHNH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1353,155 +1359,155 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="150">
-    <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="134" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="136" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="138" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="140" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="142" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="144" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="146" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="148" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Bad" xfId="93" builtinId="27"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1806,21 +1812,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="75" workbookViewId="0">
       <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -1884,25 +1890,25 @@
         <v>66</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="Q1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>102</v>
@@ -1911,7 +1917,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="16">
+    <row r="2" spans="1:22">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1974,7 +1980,7 @@
       </c>
       <c r="U2" s="7"/>
     </row>
-    <row r="3" spans="1:22" ht="16">
+    <row r="3" spans="1:22">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2006,38 +2012,38 @@
         <v>124</v>
       </c>
       <c r="K3" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="S3" s="8" t="s">
         <v>250</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>251</v>
       </c>
       <c r="T3" s="8" t="s">
         <v>155</v>
       </c>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:22" ht="16">
+    <row r="4" spans="1:22">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -2069,36 +2075,36 @@
         <v>125</v>
       </c>
       <c r="K4" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>253</v>
-      </c>
       <c r="M4" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O4" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q4" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="P4" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="Q4" s="7" t="s">
+      <c r="R4" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="S4" s="7" t="s">
         <v>264</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>265</v>
       </c>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
     </row>
-    <row r="5" spans="1:22" ht="16">
+    <row r="5" spans="1:22">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -2146,7 +2152,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="16">
+    <row r="6" spans="1:22">
       <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
@@ -2190,7 +2196,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="16">
+    <row r="7" spans="1:22">
       <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
@@ -2234,7 +2240,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="16">
+    <row r="8" spans="1:22">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -2278,7 +2284,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="16">
+    <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="16">
+    <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -2366,7 +2372,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="16">
+    <row r="11" spans="1:22">
       <c r="A11" s="1" t="s">
         <v>127</v>
       </c>
@@ -2410,7 +2416,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="16">
+    <row r="12" spans="1:22">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -2476,7 +2482,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="16">
+    <row r="13" spans="1:22">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2503,7 +2509,7 @@
       <c r="T13" s="9"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:22" ht="16">
+    <row r="14" spans="1:22">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -2551,7 +2557,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="16">
+    <row r="15" spans="1:22">
       <c r="A15" s="1" t="s">
         <v>110</v>
       </c>
@@ -2597,7 +2603,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="16">
+    <row r="16" spans="1:22">
       <c r="A16" s="1" t="s">
         <v>143</v>
       </c>
@@ -2637,7 +2643,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="16">
+    <row r="17" spans="1:22">
       <c r="A17" s="1" t="s">
         <v>141</v>
       </c>
@@ -2668,7 +2674,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="16">
+    <row r="18" spans="1:22">
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
@@ -2716,7 +2722,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="16">
+    <row r="19" spans="1:22">
       <c r="A19" s="1" t="s">
         <v>159</v>
       </c>
@@ -2764,7 +2770,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="16">
+    <row r="20" spans="1:22">
       <c r="A20" s="1" t="s">
         <v>162</v>
       </c>
@@ -2812,7 +2818,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="16">
+    <row r="21" spans="1:22">
       <c r="A21" s="1" t="s">
         <v>168</v>
       </c>
@@ -2858,7 +2864,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="16">
+    <row r="22" spans="1:22">
       <c r="A22" s="1" t="s">
         <v>169</v>
       </c>
@@ -2904,12 +2910,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="16">
+    <row r="23" spans="1:22">
       <c r="A23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>176</v>
       </c>
       <c r="C23" s="13">
         <v>0.55369999999999997</v>
@@ -2942,18 +2948,18 @@
       <c r="S23" s="13"/>
       <c r="T23" s="13"/>
       <c r="U23" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="V23" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="16">
+    <row r="24" spans="1:22">
       <c r="A24" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="C24" s="13">
         <v>3.0519999999999998E-8</v>
@@ -2986,18 +2992,18 @@
       <c r="S24" s="13"/>
       <c r="T24" s="13"/>
       <c r="U24" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="V24" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="16">
+    <row r="25" spans="1:22">
       <c r="A25" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>187</v>
       </c>
       <c r="C25" s="13">
         <v>647.1</v>
@@ -3051,15 +3057,15 @@
         <v>108</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" ht="16">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="C26" s="13">
         <v>22060000</v>
@@ -3113,15 +3119,15 @@
         <v>140</v>
       </c>
       <c r="V26" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" ht="16">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22">
       <c r="A27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>190</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>191</v>
       </c>
       <c r="C27" s="13">
         <v>5.5999999999999999E-5</v>
@@ -3154,18 +3160,18 @@
       <c r="S27" s="13"/>
       <c r="T27" s="13"/>
       <c r="U27" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="V27" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="V27" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" ht="16">
+    </row>
+    <row r="28" spans="1:22">
       <c r="A28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="C28" s="13">
         <v>0.34399999999999997</v>
@@ -3216,15 +3222,15 @@
       </c>
       <c r="T28" s="13"/>
       <c r="V28" s="7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" ht="16">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C29" s="13">
         <v>2.677</v>
@@ -3258,15 +3264,15 @@
       <c r="T29" s="13"/>
       <c r="U29" s="7"/>
       <c r="V29" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C30" s="14">
         <v>2.9732000000000001E-3</v>
@@ -3299,18 +3305,18 @@
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
       <c r="U30" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V30" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
       <c r="A31" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C31" s="14">
         <v>-7.7377000000000003E-7</v>
@@ -3343,18 +3349,18 @@
       <c r="S31" s="13"/>
       <c r="T31" s="13"/>
       <c r="U31" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
       <c r="A32" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C32" s="14">
         <v>9.4433999999999999E-11</v>
@@ -3387,18 +3393,18 @@
       <c r="S32" s="13"/>
       <c r="T32" s="13"/>
       <c r="U32" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V32" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" s="14">
         <v>-4.2689999999999998E-15</v>
@@ -3431,18 +3437,18 @@
       <c r="S33" s="13"/>
       <c r="T33" s="13"/>
       <c r="U33" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="V33" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="V33" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22" ht="16">
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C34" s="14">
         <v>-29886</v>
@@ -3478,15 +3484,15 @@
         <v>108</v>
       </c>
       <c r="V34" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C35" s="13">
         <v>6.8826000000000001</v>
@@ -3519,15 +3525,15 @@
       <c r="S35" s="13"/>
       <c r="T35" s="13"/>
       <c r="V35" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C36" s="13">
         <v>4.1985999999999999</v>
@@ -3560,15 +3566,15 @@
       <c r="S36" s="13"/>
       <c r="T36" s="13"/>
       <c r="V36" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C37" s="14">
         <v>-2.0363999999999998E-3</v>
@@ -3601,18 +3607,18 @@
       <c r="S37" s="13"/>
       <c r="T37" s="13"/>
       <c r="U37" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V37" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
       <c r="A38" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C38" s="13">
         <v>6.5204000000000003E-6</v>
@@ -3645,18 +3651,18 @@
       <c r="S38" s="13"/>
       <c r="T38" s="13"/>
       <c r="U38" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="V38" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22">
       <c r="A39" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C39" s="14">
         <v>-5.4880000000000001E-9</v>
@@ -3689,18 +3695,18 @@
       <c r="S39" s="13"/>
       <c r="T39" s="13"/>
       <c r="U39" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V39" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C40" s="13">
         <v>1.7719999999999999E-12</v>
@@ -3733,18 +3739,18 @@
       <c r="S40" s="13"/>
       <c r="T40" s="13"/>
       <c r="U40" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="V40" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="V40" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22" ht="16">
+    </row>
+    <row r="41" spans="1:22">
       <c r="A41" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C41" s="14">
         <v>-30294</v>
@@ -3780,15 +3786,15 @@
         <v>108</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
       <c r="A42" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C42" s="14">
         <v>-0.84902999999999995</v>
@@ -3821,15 +3827,15 @@
       <c r="S42" s="13"/>
       <c r="T42" s="13"/>
       <c r="V42" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22" ht="16">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22">
       <c r="A43" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="13">
@@ -3850,18 +3856,18 @@
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
       <c r="U43" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="V43" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22" ht="16">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
       <c r="A44" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>232</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18">
@@ -3885,15 +3891,15 @@
         <v>108</v>
       </c>
       <c r="V44" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" ht="16">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C45" s="19">
         <v>75.349999999999994</v>
@@ -3926,12 +3932,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="16">
+    <row r="46" spans="1:22">
       <c r="A46" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>266</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>267</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="18">
@@ -3971,15 +3977,15 @@
         <v>1E-4</v>
       </c>
       <c r="V46" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
+      <c r="A47" s="1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" ht="16">
-      <c r="A47" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="B47" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C47" s="15">
         <v>0</v>
@@ -4040,12 +4046,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:22" ht="16">
+    <row r="48" spans="1:22">
       <c r="A48" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C48" s="15">
         <v>0</v>
@@ -4106,12 +4112,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="16">
+    <row r="49" spans="1:22">
       <c r="A49" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C49" s="3">
         <v>1.8599999999999998E-2</v>
@@ -4172,12 +4178,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="16">
+    <row r="50" spans="1:22">
       <c r="A50" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C50" s="3">
         <v>2.6100000000000002E-2</v>
@@ -4238,12 +4244,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:22" ht="16">
+    <row r="51" spans="1:22">
       <c r="A51" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C51" s="3">
         <v>3.56E-2</v>
@@ -4304,12 +4310,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:22" ht="16">
+    <row r="52" spans="1:22">
       <c r="A52" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C52" s="3">
         <v>4.6199999999999998E-2</v>
@@ -4370,12 +4376,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:22" ht="16">
+    <row r="53" spans="1:22">
       <c r="A53" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C53">
         <v>0.55620000000000003</v>
@@ -4394,18 +4400,18 @@
       </c>
       <c r="H53" s="3"/>
       <c r="U53" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V53" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:22" ht="16">
+    <row r="54" spans="1:22">
       <c r="A54" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C54">
         <v>0.60619999999999996</v>
@@ -4426,18 +4432,18 @@
         <v>0.111</v>
       </c>
       <c r="U54" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V54" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:22" ht="16">
+    <row r="55" spans="1:22">
       <c r="A55" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C55">
         <v>0.64229999999999998</v>
@@ -4455,18 +4461,18 @@
         <v>0</v>
       </c>
       <c r="U55" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V55" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:22" ht="16">
+    <row r="56" spans="1:22">
       <c r="A56" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C56">
         <v>0.6643</v>
@@ -4484,18 +4490,18 @@
         <v>0</v>
       </c>
       <c r="U56" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V56" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:22" ht="16">
+    <row r="57" spans="1:22">
       <c r="A57" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C57">
         <v>0.67290000000000005</v>
@@ -4513,120 +4519,120 @@
         <v>0</v>
       </c>
       <c r="U57" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V57" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:22" ht="16">
+    <row r="58" spans="1:22">
       <c r="A58" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>295</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>296</v>
       </c>
       <c r="H58" s="3">
         <v>9.9000000000000008E-3</v>
       </c>
       <c r="U58" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V58" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:22" ht="16">
+    <row r="59" spans="1:22">
       <c r="A59" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H59" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="U59" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V59" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:22" ht="16">
+    <row r="60" spans="1:22">
       <c r="A60" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H60" s="3">
         <v>1.21E-2</v>
       </c>
       <c r="U60" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V60" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:22" ht="16">
+    <row r="61" spans="1:22">
       <c r="A61" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H61" s="3">
         <v>1.32E-2</v>
       </c>
       <c r="U61" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V61" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:22" ht="16">
+    <row r="62" spans="1:22">
       <c r="A62" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H62" s="3">
         <v>1.43E-2</v>
       </c>
       <c r="U62" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V62" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:22" ht="16">
+    <row r="63" spans="1:22">
       <c r="A63" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>310</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>311</v>
       </c>
       <c r="I63">
         <v>0.5</v>
       </c>
       <c r="U63" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V63" s="7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22">
+      <c r="A64" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="64" spans="1:22" ht="16">
-      <c r="A64" s="1" t="s">
+      <c r="B64" s="7" t="s">
         <v>313</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>314</v>
       </c>
       <c r="C64" s="22">
         <v>0</v>
@@ -4680,18 +4686,18 @@
         <v>7.7000000000000008E-6</v>
       </c>
       <c r="U64" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V64" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:22" ht="16">
+    <row r="65" spans="1:22">
       <c r="A65" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C65" s="22">
         <v>0</v>
@@ -4745,18 +4751,18 @@
         <v>1.47E-5</v>
       </c>
       <c r="U65" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V65" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="16">
+    <row r="66" spans="1:22">
       <c r="A66" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C66" s="3">
         <v>9.7999999999999993E-6</v>
@@ -4810,18 +4816,18 @@
         <v>2.0699999999999998E-5</v>
       </c>
       <c r="U66" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V66" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="67" spans="1:22" ht="16">
+    <row r="67" spans="1:22">
       <c r="A67" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C67" s="3">
         <v>1.34E-5</v>
@@ -4875,18 +4881,18 @@
         <v>2.58E-5</v>
       </c>
       <c r="U67" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V67" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:22" ht="16">
+    <row r="68" spans="1:22">
       <c r="A68" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C68" s="3">
         <v>1.73E-5</v>
@@ -4940,18 +4946,18 @@
         <v>3.0499999999999999E-5</v>
       </c>
       <c r="U68" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V68" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="16">
+    <row r="69" spans="1:22">
       <c r="A69" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C69" s="3">
         <v>2.1399999999999998E-5</v>
@@ -5005,18 +5011,18 @@
         <v>3.4700000000000003E-5</v>
       </c>
       <c r="U69" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V69" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="16">
+    <row r="70" spans="1:22">
       <c r="A70" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B70" s="7" t="s">
         <v>336</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>337</v>
       </c>
       <c r="C70" s="24">
         <v>0</v>
@@ -5052,18 +5058,18 @@
       <c r="R70" s="3"/>
       <c r="S70" s="3"/>
       <c r="U70" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V70" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="16">
+    <row r="71" spans="1:22">
       <c r="A71" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B71" s="7" t="s">
         <v>326</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>327</v>
       </c>
       <c r="C71" s="3">
         <v>1.7930000000000001E-3</v>
@@ -5090,18 +5096,18 @@
         <v>2.7700000000000001E-4</v>
       </c>
       <c r="U71" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V71" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="16">
+    <row r="72" spans="1:22">
       <c r="A72" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C72" s="3">
         <v>8.8999999999999995E-4</v>
@@ -5128,18 +5134,18 @@
         <v>2.14E-4</v>
       </c>
       <c r="U72" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V72" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="16">
+    <row r="73" spans="1:22">
       <c r="A73" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C73" s="3">
         <v>5.4699999999999996E-4</v>
@@ -5160,18 +5166,18 @@
         <v>1.17E-2</v>
       </c>
       <c r="U73" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V73" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="74" spans="1:22" ht="16">
+    <row r="74" spans="1:22">
       <c r="A74" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C74" s="3">
         <v>3.7800000000000003E-4</v>
@@ -5192,18 +5198,18 @@
         <v>6.6E-3</v>
       </c>
       <c r="U74" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V74" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:22" ht="16">
+    <row r="75" spans="1:22">
       <c r="A75" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C75" s="3">
         <v>2.8200000000000002E-4</v>
@@ -5224,7 +5230,7 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="U75" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V75" s="7" t="s">
         <v>135</v>
@@ -5242,14 +5248,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="29.1640625" style="1" customWidth="1"/>
   </cols>
@@ -5361,18 +5367,18 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7" t="s">
         <v>308</v>
-      </c>
-      <c r="B7" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B8" t="s">
         <v>306</v>
-      </c>
-      <c r="B8" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -5441,7 +5447,7 @@
         <v>315360000</v>
       </c>
       <c r="H15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -5471,10 +5477,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18" t="s">
-        <v>172</v>
+        <v>337</v>
       </c>
       <c r="C18">
         <v>91880</v>
@@ -5485,10 +5491,10 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B19" t="s">
         <v>226</v>
-      </c>
-      <c r="B19" t="s">
-        <v>227</v>
       </c>
       <c r="G19">
         <v>8.3140000000000001</v>
@@ -5499,16 +5505,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B20" t="s">
         <v>268</v>
-      </c>
-      <c r="B20" t="s">
-        <v>269</v>
       </c>
       <c r="C20" s="3">
         <v>38700000</v>
       </c>
       <c r="H20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -5523,14 +5529,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>
@@ -5579,7 +5585,7 @@
         <v>138</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -6129,10 +6135,10 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B15" t="s">
         <v>234</v>
-      </c>
-      <c r="B15" t="s">
-        <v>235</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -6170,10 +6176,10 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B16" t="s">
         <v>241</v>
-      </c>
-      <c r="B16" t="s">
-        <v>242</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -6498,10 +6504,10 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B24" t="s">
         <v>194</v>
-      </c>
-      <c r="B24" t="s">
-        <v>195</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -6539,10 +6545,10 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B25" t="s">
         <v>236</v>
-      </c>
-      <c r="B25" t="s">
-        <v>237</v>
       </c>
       <c r="C25">
         <v>0</v>

</xml_diff>

<commit_message>
Bug Fix EB Enthalpy load
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0120599E-C735-7743-85CB-5428A7636795}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98B5137-C511-0748-8BAA-0BE61533B54A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="339">
   <si>
     <t>parvariable</t>
   </si>
@@ -1047,6 +1047,9 @@
   </si>
   <si>
     <t>deltaHNH</t>
+  </si>
+  <si>
+    <t>foo</t>
   </si>
 </sst>
 </file>
@@ -1566,7 +1569,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1618,7 +1621,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5249,10 +5252,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5515,6 +5518,17 @@
       </c>
       <c r="H20" t="s">
         <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B21" t="s">
+        <v>338</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stuff from natural gas in trash, consider natural gas as methane
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,39 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98B5137-C511-0748-8BAA-0BE61533B54A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="319">
   <si>
     <t>parvariable</t>
   </si>
@@ -761,75 +755,12 @@
     <t>xN2</t>
   </si>
   <si>
-    <t>Ethane</t>
-  </si>
-  <si>
-    <t>Propane</t>
-  </si>
-  <si>
-    <t>Isobutane</t>
-  </si>
-  <si>
-    <t>Butane</t>
-  </si>
-  <si>
-    <t>Isopentane</t>
-  </si>
-  <si>
-    <t>Pentane</t>
-  </si>
-  <si>
-    <t>Hexane</t>
-  </si>
-  <si>
     <t>Carbon dioxide</t>
   </si>
   <si>
-    <t>Oxygen</t>
-  </si>
-  <si>
-    <t>C2H6</t>
-  </si>
-  <si>
-    <t>C3H8</t>
-  </si>
-  <si>
-    <t>entity L</t>
-  </si>
-  <si>
-    <t>entity M</t>
-  </si>
-  <si>
-    <t>entity N</t>
-  </si>
-  <si>
-    <t>C4H10</t>
-  </si>
-  <si>
-    <t>entity O</t>
-  </si>
-  <si>
-    <t>entity P</t>
-  </si>
-  <si>
-    <t>entity Q</t>
-  </si>
-  <si>
-    <t>entity R</t>
-  </si>
-  <si>
-    <t>C5H12</t>
-  </si>
-  <si>
-    <t>C6H14</t>
-  </si>
-  <si>
     <t>CO2</t>
   </si>
   <si>
-    <t>O2</t>
-  </si>
-  <si>
     <t>Mole fraction in the natural gas</t>
   </si>
   <si>
@@ -1050,16 +981,19 @@
   </si>
   <si>
     <t>foo</t>
+  </si>
+  <si>
+    <t>entity PI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1362,155 +1296,155 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="150">
-    <cellStyle name="Bad" xfId="93" builtinId="27"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="149" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1569,7 +1503,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1621,7 +1555,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1815,21 +1749,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J72" sqref="J72"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -1840,19 +1774,13 @@
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
     <col min="10" max="10" width="18.83203125" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="14" width="13.83203125" customWidth="1"/>
-    <col min="15" max="16" width="16.1640625" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" customWidth="1"/>
-    <col min="19" max="19" width="16.6640625" customWidth="1"/>
-    <col min="20" max="20" width="13.83203125" customWidth="1"/>
-    <col min="21" max="21" width="13" customWidth="1"/>
-    <col min="22" max="22" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1884,43 +1812,19 @@
         <v>63</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>64</v>
+        <v>318</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="V1" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:14" ht="16">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1957,33 +1861,9 @@
       <c r="L2" s="7">
         <v>10</v>
       </c>
-      <c r="M2" s="7">
-        <v>11</v>
-      </c>
-      <c r="N2" s="7">
-        <v>12</v>
-      </c>
-      <c r="O2" s="7">
-        <v>13</v>
-      </c>
-      <c r="P2" s="7">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="7">
-        <v>15</v>
-      </c>
-      <c r="R2" s="7">
-        <v>16</v>
-      </c>
-      <c r="S2" s="7">
-        <v>17</v>
-      </c>
-      <c r="T2" s="7">
-        <v>18</v>
-      </c>
-      <c r="U2" s="7"/>
-    </row>
-    <row r="3" spans="1:22">
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:14" ht="16">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2018,35 +1898,11 @@
         <v>242</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="T3" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="U3" s="7"/>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" ht="16">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -2078,36 +1934,12 @@
         <v>125</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-    </row>
-    <row r="5" spans="1:22">
+        <v>243</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" ht="16">
       <c r="A5" s="1" t="s">
         <v>133</v>
       </c>
@@ -2140,22 +1972,14 @@
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="V5" t="s">
+      <c r="N5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:14" ht="16">
       <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
@@ -2186,20 +2010,12 @@
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="7"/>
-      <c r="V6" t="s">
+      <c r="M6" s="7"/>
+      <c r="N6" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:14" ht="16">
       <c r="A7" s="1" t="s">
         <v>112</v>
       </c>
@@ -2230,20 +2046,12 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="7"/>
-      <c r="V7" t="s">
+      <c r="M7" s="7"/>
+      <c r="N7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:14" ht="16">
       <c r="A8" s="1" t="s">
         <v>120</v>
       </c>
@@ -2274,20 +2082,12 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="7"/>
-      <c r="V8" t="s">
+      <c r="M8" s="7"/>
+      <c r="N8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:14" ht="16">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -2318,20 +2118,12 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="7"/>
-      <c r="V9" t="s">
+      <c r="M9" s="7"/>
+      <c r="N9" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:14" ht="16">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -2362,20 +2154,12 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="7"/>
-      <c r="V10" t="s">
+      <c r="M10" s="7"/>
+      <c r="N10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:14" ht="16">
       <c r="A11" s="1" t="s">
         <v>127</v>
       </c>
@@ -2406,20 +2190,12 @@
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="7"/>
-      <c r="V11" t="s">
+      <c r="M11" s="7"/>
+      <c r="N11" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:14" ht="16">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -2451,41 +2227,17 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="K12" s="9">
-        <v>3.0068999999999999E-2</v>
-      </c>
-      <c r="L12" s="9">
-        <v>4.4096000000000003E-2</v>
-      </c>
-      <c r="M12" s="9">
-        <v>5.8122E-2</v>
-      </c>
-      <c r="N12" s="9">
-        <v>5.8122E-2</v>
-      </c>
-      <c r="O12" s="9">
-        <v>7.2149000000000005E-2</v>
-      </c>
-      <c r="P12" s="9">
-        <v>7.2149000000000005E-2</v>
-      </c>
-      <c r="Q12" s="9">
-        <v>8.6175000000000002E-2</v>
-      </c>
-      <c r="R12" s="9">
         <v>4.4010000000000001E-2</v>
       </c>
-      <c r="S12" s="9">
-        <v>3.1997999999999999E-2</v>
-      </c>
-      <c r="T12" s="9"/>
-      <c r="U12" s="7" t="s">
+      <c r="L12" s="9"/>
+      <c r="M12" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="V12" s="7" t="s">
+      <c r="N12" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:14" ht="16">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2502,17 +2254,9 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="7"/>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" ht="16">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -2545,22 +2289,14 @@
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="7" t="s">
+      <c r="M14" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="V14" s="7" t="s">
+      <c r="N14" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:14" ht="16">
       <c r="A15" s="1" t="s">
         <v>110</v>
       </c>
@@ -2591,22 +2327,14 @@
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="7" t="s">
+      <c r="M15" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="V15" s="7" t="s">
+      <c r="N15" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:14" ht="16">
       <c r="A16" s="1" t="s">
         <v>143</v>
       </c>
@@ -2631,22 +2359,14 @@
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="7" t="s">
+      <c r="M16" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="V16" s="7" t="s">
+      <c r="N16" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:14" ht="16">
       <c r="A17" s="1" t="s">
         <v>141</v>
       </c>
@@ -2662,22 +2382,14 @@
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13">
+      <c r="L17" s="13">
         <v>4.5</v>
       </c>
-      <c r="U17" s="8" t="s">
+      <c r="M17" s="8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:14" ht="16">
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
@@ -2710,22 +2422,14 @@
       </c>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="7" t="s">
+      <c r="M18" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="V18" s="7" t="s">
+      <c r="N18" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:14" ht="16">
       <c r="A19" s="1" t="s">
         <v>159</v>
       </c>
@@ -2758,22 +2462,14 @@
       </c>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="7" t="s">
+      <c r="M19" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="V19" s="7" t="s">
+      <c r="N19" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:14" ht="16">
       <c r="A20" s="1" t="s">
         <v>162</v>
       </c>
@@ -2806,22 +2502,14 @@
       </c>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="7" t="s">
+      <c r="M20" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="V20" s="7" t="s">
+      <c r="N20" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:14" ht="16">
       <c r="A21" s="1" t="s">
         <v>168</v>
       </c>
@@ -2852,22 +2540,14 @@
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="7" t="s">
+      <c r="M21" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="V21" s="7" t="s">
+      <c r="N21" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:14" ht="16">
       <c r="A22" s="1" t="s">
         <v>169</v>
       </c>
@@ -2898,22 +2578,14 @@
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="7" t="s">
+      <c r="M22" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="V22" s="7" t="s">
+      <c r="N22" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:14" ht="16">
       <c r="A23" s="1" t="s">
         <v>174</v>
       </c>
@@ -2942,22 +2614,14 @@
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="7" t="s">
+      <c r="M23" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="V23" s="7" t="s">
+      <c r="N23" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:14" ht="16">
       <c r="A24" s="1" t="s">
         <v>176</v>
       </c>
@@ -2986,22 +2650,14 @@
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="7" t="s">
+      <c r="M24" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="V24" s="7" t="s">
+      <c r="N24" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:14" ht="16">
       <c r="A25" s="1" t="s">
         <v>185</v>
       </c>
@@ -3029,41 +2685,17 @@
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13">
-        <v>305.36</v>
-      </c>
-      <c r="L25" s="13">
-        <v>369.9</v>
-      </c>
-      <c r="M25" s="13">
-        <v>407.84</v>
-      </c>
-      <c r="N25" s="13">
-        <v>425.2</v>
-      </c>
-      <c r="O25" s="13">
-        <v>460.37</v>
-      </c>
-      <c r="P25" s="13">
-        <v>469.7</v>
-      </c>
-      <c r="Q25" s="13">
-        <v>507.5</v>
-      </c>
-      <c r="R25" s="13">
         <v>304.13</v>
       </c>
-      <c r="S25" s="13">
-        <v>154.58000000000001</v>
-      </c>
-      <c r="T25" s="13"/>
-      <c r="U25" s="7" t="s">
+      <c r="L25" s="13"/>
+      <c r="M25" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="V25" s="7" t="s">
+      <c r="N25" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:14" ht="16">
       <c r="A26" s="1" t="s">
         <v>187</v>
       </c>
@@ -3091,41 +2723,17 @@
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13">
-        <v>4880000</v>
-      </c>
-      <c r="L26" s="13">
-        <v>4250000</v>
-      </c>
-      <c r="M26" s="13">
-        <v>3640000</v>
-      </c>
-      <c r="N26" s="13">
-        <v>3790000</v>
-      </c>
-      <c r="O26" s="13">
-        <v>3350000</v>
-      </c>
-      <c r="P26" s="13">
-        <v>3370000</v>
-      </c>
-      <c r="Q26" s="13">
-        <v>3030000</v>
-      </c>
-      <c r="R26" s="13">
         <v>7380000</v>
       </c>
-      <c r="S26" s="13">
-        <v>5040000</v>
-      </c>
-      <c r="T26" s="13"/>
-      <c r="U26" s="7" t="s">
+      <c r="L26" s="13"/>
+      <c r="M26" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="V26" s="7" t="s">
+      <c r="N26" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:14" ht="16">
       <c r="A27" s="1" t="s">
         <v>189</v>
       </c>
@@ -3154,22 +2762,14 @@
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="7" t="s">
+      <c r="M27" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="V27" s="7" t="s">
+      <c r="N27" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:14" ht="16">
       <c r="A28" s="1" t="s">
         <v>195</v>
       </c>
@@ -3197,38 +2797,14 @@
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="L28" s="13">
-        <v>0.153</v>
-      </c>
-      <c r="M28" s="13">
-        <v>0.183</v>
-      </c>
-      <c r="N28" s="13">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="O28" s="13">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="P28" s="13">
-        <v>0.251</v>
-      </c>
-      <c r="Q28" s="13">
-        <v>0.29899999999999999</v>
-      </c>
-      <c r="R28" s="13">
         <v>0.23899999999999999</v>
       </c>
-      <c r="S28" s="13">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="T28" s="13"/>
-      <c r="V28" s="7" t="s">
+      <c r="L28" s="13"/>
+      <c r="N28" s="7" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:14" ht="16">
       <c r="A29" s="1" t="s">
         <v>209</v>
       </c>
@@ -3257,20 +2833,12 @@
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="7" t="s">
+      <c r="M29" s="7"/>
+      <c r="N29" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:14" ht="16">
       <c r="A30" s="1" t="s">
         <v>210</v>
       </c>
@@ -3299,22 +2867,14 @@
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
-      <c r="U30" s="7" t="s">
+      <c r="M30" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="V30" s="7" t="s">
+      <c r="N30" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:14" ht="16">
       <c r="A31" s="1" t="s">
         <v>207</v>
       </c>
@@ -3343,22 +2903,14 @@
       <c r="J31" s="13"/>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13"/>
-      <c r="U31" s="7" t="s">
+      <c r="M31" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="V31" s="7" t="s">
+      <c r="N31" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:14" ht="16">
       <c r="A32" s="1" t="s">
         <v>208</v>
       </c>
@@ -3387,22 +2939,14 @@
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13"/>
-      <c r="T32" s="13"/>
-      <c r="U32" s="7" t="s">
+      <c r="M32" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="V32" s="7" t="s">
+      <c r="N32" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:14" ht="16">
       <c r="A33" s="1" t="s">
         <v>211</v>
       </c>
@@ -3431,22 +2975,14 @@
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="13"/>
-      <c r="S33" s="13"/>
-      <c r="T33" s="13"/>
-      <c r="U33" s="7" t="s">
+      <c r="M33" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="V33" s="7" t="s">
+      <c r="N33" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:14" ht="16">
       <c r="A34" s="1" t="s">
         <v>217</v>
       </c>
@@ -3475,22 +3011,14 @@
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="13"/>
-      <c r="T34" s="13"/>
-      <c r="U34" s="7" t="s">
+      <c r="M34" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="V34" s="7" t="s">
+      <c r="N34" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:14" ht="16">
       <c r="A35" s="1" t="s">
         <v>218</v>
       </c>
@@ -3519,19 +3047,11 @@
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13"/>
-      <c r="T35" s="13"/>
-      <c r="V35" s="7" t="s">
+      <c r="N35" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:14" ht="16">
       <c r="A36" s="1" t="s">
         <v>214</v>
       </c>
@@ -3560,19 +3080,11 @@
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="13"/>
-      <c r="T36" s="13"/>
-      <c r="V36" s="7" t="s">
+      <c r="N36" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:14" ht="16">
       <c r="A37" s="1" t="s">
         <v>215</v>
       </c>
@@ -3601,22 +3113,14 @@
       <c r="J37" s="13"/>
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="13"/>
-      <c r="P37" s="13"/>
-      <c r="Q37" s="13"/>
-      <c r="R37" s="13"/>
-      <c r="S37" s="13"/>
-      <c r="T37" s="13"/>
-      <c r="U37" s="7" t="s">
+      <c r="M37" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="V37" s="7" t="s">
+      <c r="N37" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:22">
+    <row r="38" spans="1:14" ht="16">
       <c r="A38" s="1" t="s">
         <v>212</v>
       </c>
@@ -3645,22 +3149,14 @@
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13"/>
-      <c r="Q38" s="13"/>
-      <c r="R38" s="13"/>
-      <c r="S38" s="13"/>
-      <c r="T38" s="13"/>
-      <c r="U38" s="7" t="s">
+      <c r="M38" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="V38" s="7" t="s">
+      <c r="N38" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:22">
+    <row r="39" spans="1:14" ht="16">
       <c r="A39" s="1" t="s">
         <v>213</v>
       </c>
@@ -3689,22 +3185,14 @@
       <c r="J39" s="13"/>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="13"/>
-      <c r="P39" s="13"/>
-      <c r="Q39" s="13"/>
-      <c r="R39" s="13"/>
-      <c r="S39" s="13"/>
-      <c r="T39" s="13"/>
-      <c r="U39" s="7" t="s">
+      <c r="M39" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="V39" s="7" t="s">
+      <c r="N39" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="40" spans="1:22">
+    <row r="40" spans="1:14" ht="16">
       <c r="A40" s="1" t="s">
         <v>216</v>
       </c>
@@ -3733,22 +3221,14 @@
       <c r="J40" s="13"/>
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="13"/>
-      <c r="Q40" s="13"/>
-      <c r="R40" s="13"/>
-      <c r="S40" s="13"/>
-      <c r="T40" s="13"/>
-      <c r="U40" s="7" t="s">
+      <c r="M40" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="V40" s="7" t="s">
+      <c r="N40" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="41" spans="1:22">
+    <row r="41" spans="1:14" ht="16">
       <c r="A41" s="1" t="s">
         <v>221</v>
       </c>
@@ -3777,22 +3257,14 @@
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="13"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="13"/>
-      <c r="S41" s="13"/>
-      <c r="T41" s="13"/>
-      <c r="U41" s="7" t="s">
+      <c r="M41" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="V41" s="7" t="s">
+      <c r="N41" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:22">
+    <row r="42" spans="1:14" ht="16">
       <c r="A42" s="1" t="s">
         <v>222</v>
       </c>
@@ -3821,19 +3293,11 @@
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
       <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="13"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="13"/>
-      <c r="R42" s="13"/>
-      <c r="S42" s="13"/>
-      <c r="T42" s="13"/>
-      <c r="V42" s="7" t="s">
+      <c r="N42" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="43" spans="1:22">
+    <row r="43" spans="1:14" ht="16">
       <c r="A43" s="1" t="s">
         <v>228</v>
       </c>
@@ -3858,14 +3322,14 @@
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
-      <c r="U43" s="7" t="s">
+      <c r="M43" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="V43" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22">
+      <c r="N43" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="16">
       <c r="A44" s="1" t="s">
         <v>230</v>
       </c>
@@ -3890,14 +3354,14 @@
       </c>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
-      <c r="U44" s="7" t="s">
+      <c r="M44" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="V44" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22">
+      <c r="N44" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="16">
       <c r="A45" s="1" t="s">
         <v>239</v>
       </c>
@@ -3928,19 +3392,19 @@
       <c r="J45" s="9">
         <v>187.49</v>
       </c>
-      <c r="U45" s="7" t="s">
+      <c r="M45" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="V45" s="7" t="s">
+      <c r="N45" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:22">
+    <row r="46" spans="1:14" ht="16">
       <c r="A46" s="1" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="18">
@@ -3953,42 +3417,18 @@
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
       <c r="K46" s="3">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="L46" s="3">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="M46" s="3">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="N46" s="3">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="O46" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="P46" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="Q46" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="R46" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="S46" s="3">
-        <v>1E-4</v>
-      </c>
-      <c r="V46" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22">
+      <c r="N46" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="16">
       <c r="A47" s="1" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="C47" s="15">
         <v>0</v>
@@ -4017,44 +3457,20 @@
       <c r="K47" s="16">
         <v>0</v>
       </c>
-      <c r="L47" s="16">
-        <v>0</v>
-      </c>
-      <c r="M47" s="16">
-        <v>0</v>
-      </c>
-      <c r="N47" s="16">
-        <v>0</v>
-      </c>
-      <c r="O47" s="16">
-        <v>0</v>
-      </c>
-      <c r="P47" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="16">
-        <v>0</v>
-      </c>
-      <c r="R47" s="16">
-        <v>0</v>
-      </c>
-      <c r="S47" s="13">
-        <v>9.1000000000000004E-3</v>
-      </c>
-      <c r="T47" s="18"/>
-      <c r="U47" s="8" t="s">
+      <c r="L47" s="18"/>
+      <c r="M47" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="V47" s="7" t="s">
+      <c r="N47" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="48" spans="1:22">
+    <row r="48" spans="1:14" ht="16">
       <c r="A48" s="1" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="C48" s="15">
         <v>0</v>
@@ -4081,46 +3497,22 @@
         <v>0</v>
       </c>
       <c r="K48" s="13">
-        <v>1.0699999999999999E-2</v>
-      </c>
-      <c r="L48" s="16">
-        <v>0</v>
-      </c>
-      <c r="M48" s="16">
-        <v>0</v>
-      </c>
-      <c r="N48" s="16">
-        <v>0</v>
-      </c>
-      <c r="O48" s="16">
-        <v>0</v>
-      </c>
-      <c r="P48" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="16">
-        <v>0</v>
-      </c>
-      <c r="R48" s="13">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="S48" s="13">
-        <v>1.8200000000000001E-2</v>
-      </c>
-      <c r="T48" s="18"/>
-      <c r="U48" s="8" t="s">
+      <c r="L48" s="18"/>
+      <c r="M48" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="V48" s="7" t="s">
+      <c r="N48" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:22">
+    <row r="49" spans="1:14" ht="16">
       <c r="A49" s="1" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="C49" s="3">
         <v>1.8599999999999998E-2</v>
@@ -4147,46 +3539,22 @@
         <v>0</v>
       </c>
       <c r="K49" s="13">
-        <v>2.12E-2</v>
-      </c>
-      <c r="L49" s="13">
-        <v>1.8499999999999999E-2</v>
-      </c>
-      <c r="M49" s="13">
-        <v>1.7100000000000001E-2</v>
-      </c>
-      <c r="N49" s="13">
-        <v>1.67E-2</v>
-      </c>
-      <c r="O49" s="16">
-        <v>0</v>
-      </c>
-      <c r="P49" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="16">
-        <v>0</v>
-      </c>
-      <c r="R49" s="13">
         <v>1.6799999999999999E-2</v>
       </c>
-      <c r="S49" s="13">
-        <v>2.6499999999999999E-2</v>
-      </c>
-      <c r="T49" s="18"/>
-      <c r="U49" s="8" t="s">
+      <c r="L49" s="18"/>
+      <c r="M49" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="V49" s="7" t="s">
+      <c r="N49" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:22">
+    <row r="50" spans="1:14" ht="16">
       <c r="A50" s="1" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="C50" s="3">
         <v>2.6100000000000002E-2</v>
@@ -4213,46 +3581,22 @@
         <v>0</v>
       </c>
       <c r="K50" s="13">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="L50" s="13">
-        <v>3.1E-2</v>
-      </c>
-      <c r="M50" s="13">
-        <v>2.8899999999999999E-2</v>
-      </c>
-      <c r="N50" s="13">
-        <v>2.8299999999999999E-2</v>
-      </c>
-      <c r="O50" s="16">
-        <v>0</v>
-      </c>
-      <c r="P50" s="13">
-        <v>2.4899999999999999E-2</v>
-      </c>
-      <c r="Q50" s="13">
-        <v>2.3400000000000001E-2</v>
-      </c>
-      <c r="R50" s="13">
         <v>2.52E-2</v>
       </c>
-      <c r="S50" s="13">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="T50" s="18"/>
-      <c r="U50" s="8" t="s">
+      <c r="L50" s="18"/>
+      <c r="M50" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="V50" s="7" t="s">
+      <c r="N50" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:22">
+    <row r="51" spans="1:14" ht="16">
       <c r="A51" s="1" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
       <c r="C51" s="3">
         <v>3.56E-2</v>
@@ -4279,46 +3623,22 @@
         <v>0</v>
       </c>
       <c r="K51" s="13">
-        <v>5.3800000000000001E-2</v>
-      </c>
-      <c r="L51" s="13">
-        <v>4.6399999999999997E-2</v>
-      </c>
-      <c r="M51" s="13">
-        <v>4.3200000000000002E-2</v>
-      </c>
-      <c r="N51" s="13">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="O51" s="16">
-        <v>0</v>
-      </c>
-      <c r="P51" s="13">
-        <v>3.78E-2</v>
-      </c>
-      <c r="Q51" s="13">
-        <v>3.5400000000000001E-2</v>
-      </c>
-      <c r="R51" s="13">
         <v>3.3500000000000002E-2</v>
       </c>
-      <c r="S51" s="13">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="T51" s="18"/>
-      <c r="U51" s="8" t="s">
+      <c r="L51" s="18"/>
+      <c r="M51" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="V51" s="7" t="s">
+      <c r="N51" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="52" spans="1:22">
+    <row r="52" spans="1:14" ht="16">
       <c r="A52" s="1" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="C52" s="3">
         <v>4.6199999999999998E-2</v>
@@ -4345,46 +3665,22 @@
         <v>0</v>
       </c>
       <c r="K52" s="13">
-        <v>7.3300000000000004E-2</v>
-      </c>
-      <c r="L52" s="13">
-        <v>6.4600000000000005E-2</v>
-      </c>
-      <c r="M52" s="13">
-        <v>6.0199999999999997E-2</v>
-      </c>
-      <c r="N52" s="13">
-        <v>6.0900000000000003E-2</v>
-      </c>
-      <c r="O52" s="16">
-        <v>0</v>
-      </c>
-      <c r="P52" s="13">
-        <v>5.2699999999999997E-2</v>
-      </c>
-      <c r="Q52" s="13">
-        <v>4.87E-2</v>
-      </c>
-      <c r="R52" s="13">
         <v>4.1599999999999998E-2</v>
       </c>
-      <c r="S52" s="13">
-        <v>4.7699999999999999E-2</v>
-      </c>
-      <c r="T52" s="18"/>
-      <c r="U52" s="8" t="s">
+      <c r="L52" s="18"/>
+      <c r="M52" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="V52" s="7" t="s">
+      <c r="N52" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:22">
+    <row r="53" spans="1:14" ht="16">
       <c r="A53" s="1" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="C53">
         <v>0.55620000000000003</v>
@@ -4402,19 +3698,19 @@
         <v>0</v>
       </c>
       <c r="H53" s="3"/>
-      <c r="U53" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="V53" s="7" t="s">
+      <c r="M53" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="N53" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:22">
+    <row r="54" spans="1:14" ht="16">
       <c r="A54" s="1" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="C54">
         <v>0.60619999999999996</v>
@@ -4431,22 +3727,19 @@
       <c r="G54" s="16">
         <v>0</v>
       </c>
-      <c r="O54">
-        <v>0.111</v>
-      </c>
-      <c r="U54" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="V54" s="7" t="s">
+      <c r="M54" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="N54" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:22">
+    <row r="55" spans="1:14" ht="16">
       <c r="A55" s="1" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="C55">
         <v>0.64229999999999998</v>
@@ -4463,19 +3756,19 @@
       <c r="G55" s="16">
         <v>0</v>
       </c>
-      <c r="U55" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="V55" s="7" t="s">
+      <c r="M55" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="N55" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:22">
+    <row r="56" spans="1:14" ht="16">
       <c r="A56" s="1" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="C56">
         <v>0.6643</v>
@@ -4492,19 +3785,19 @@
       <c r="G56" s="16">
         <v>0</v>
       </c>
-      <c r="U56" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="V56" s="7" t="s">
+      <c r="M56" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="N56" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:22">
+    <row r="57" spans="1:14" ht="16">
       <c r="A57" s="1" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="C57">
         <v>0.67290000000000005</v>
@@ -4521,121 +3814,121 @@
       <c r="G57" s="16">
         <v>0</v>
       </c>
-      <c r="U57" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="V57" s="7" t="s">
+      <c r="M57" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="N57" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:22">
+    <row r="58" spans="1:14" ht="16">
       <c r="A58" s="1" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="H58" s="3">
         <v>9.9000000000000008E-3</v>
       </c>
-      <c r="U58" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="V58" s="7" t="s">
+      <c r="M58" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="N58" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:22">
+    <row r="59" spans="1:14" ht="16">
       <c r="A59" s="1" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>296</v>
+        <v>275</v>
       </c>
       <c r="H59" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="U59" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="V59" s="7" t="s">
+      <c r="M59" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="N59" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:22">
+    <row r="60" spans="1:14" ht="16">
       <c r="A60" s="1" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
       <c r="H60" s="3">
         <v>1.21E-2</v>
       </c>
-      <c r="U60" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="V60" s="7" t="s">
+      <c r="M60" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="N60" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:22">
+    <row r="61" spans="1:14" ht="16">
       <c r="A61" s="1" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
       <c r="H61" s="3">
         <v>1.32E-2</v>
       </c>
-      <c r="U61" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="V61" s="7" t="s">
+      <c r="M61" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="N61" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:22">
+    <row r="62" spans="1:14" ht="16">
       <c r="A62" s="1" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="H62" s="3">
         <v>1.43E-2</v>
       </c>
-      <c r="U62" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="V62" s="7" t="s">
+      <c r="M62" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="N62" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:22">
+    <row r="63" spans="1:14" ht="16">
       <c r="A63" s="1" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="I63">
         <v>0.5</v>
       </c>
-      <c r="U63" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="V63" s="7" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="64" spans="1:22">
+      <c r="M63" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="N63" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="16">
       <c r="A64" s="1" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="C64" s="22">
         <v>0</v>
@@ -4664,43 +3957,19 @@
       <c r="K64" s="24">
         <v>0</v>
       </c>
-      <c r="L64" s="24">
-        <v>0</v>
-      </c>
-      <c r="M64" s="24">
-        <v>0</v>
-      </c>
-      <c r="N64" s="24">
-        <v>0</v>
-      </c>
-      <c r="O64" s="24">
-        <v>0</v>
-      </c>
-      <c r="P64" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q64" s="24">
-        <v>0</v>
-      </c>
-      <c r="R64" s="24">
-        <v>0</v>
-      </c>
-      <c r="S64" s="3">
-        <v>7.7000000000000008E-6</v>
-      </c>
-      <c r="U64" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V64" s="7" t="s">
+      <c r="M64" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N64" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:22">
+    <row r="65" spans="1:14" ht="16">
       <c r="A65" s="1" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="C65" s="22">
         <v>0</v>
@@ -4727,45 +3996,21 @@
         <v>0</v>
       </c>
       <c r="K65" s="3">
-        <v>6.3999999999999997E-6</v>
-      </c>
-      <c r="L65" s="24">
-        <v>0</v>
-      </c>
-      <c r="M65" s="24">
-        <v>0</v>
-      </c>
-      <c r="N65" s="24">
-        <v>0</v>
-      </c>
-      <c r="O65" s="24">
-        <v>0</v>
-      </c>
-      <c r="P65" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q65" s="24">
-        <v>0</v>
-      </c>
-      <c r="R65" s="3">
         <v>1.01E-5</v>
       </c>
-      <c r="S65" s="3">
-        <v>1.47E-5</v>
-      </c>
-      <c r="U65" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V65" s="7" t="s">
+      <c r="M65" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N65" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:22">
+    <row r="66" spans="1:14" ht="16">
       <c r="A66" s="1" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
       <c r="C66" s="3">
         <v>9.7999999999999993E-6</v>
@@ -4792,45 +4037,21 @@
         <v>0</v>
       </c>
       <c r="K66" s="3">
-        <v>9.3999999999999998E-6</v>
-      </c>
-      <c r="L66" s="3">
-        <v>8.1999999999999994E-6</v>
-      </c>
-      <c r="M66" s="3">
-        <v>7.5000000000000002E-6</v>
-      </c>
-      <c r="N66" s="3">
-        <v>7.5000000000000002E-6</v>
-      </c>
-      <c r="O66" s="24">
-        <v>0</v>
-      </c>
-      <c r="P66" s="3">
-        <v>6.7000000000000002E-6</v>
-      </c>
-      <c r="Q66" s="24">
-        <v>0</v>
-      </c>
-      <c r="R66" s="3">
         <v>1.5E-5</v>
       </c>
-      <c r="S66" s="3">
-        <v>2.0699999999999998E-5</v>
-      </c>
-      <c r="U66" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V66" s="7" t="s">
+      <c r="M66" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N66" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="67" spans="1:22">
+    <row r="67" spans="1:14" ht="16">
       <c r="A67" s="1" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="C67" s="3">
         <v>1.34E-5</v>
@@ -4857,45 +4078,21 @@
         <v>0</v>
       </c>
       <c r="K67" s="3">
-        <v>1.22E-5</v>
-      </c>
-      <c r="L67" s="3">
-        <v>1.08E-5</v>
-      </c>
-      <c r="M67" s="3">
-        <v>9.9000000000000001E-6</v>
-      </c>
-      <c r="N67" s="3">
-        <v>9.9000000000000001E-6</v>
-      </c>
-      <c r="O67" s="24">
-        <v>0</v>
-      </c>
-      <c r="P67" s="3">
-        <v>9.2E-5</v>
-      </c>
-      <c r="Q67" s="3">
-        <v>8.6000000000000007E-6</v>
-      </c>
-      <c r="R67" s="3">
         <v>1.9700000000000001E-5</v>
       </c>
-      <c r="S67" s="3">
-        <v>2.58E-5</v>
-      </c>
-      <c r="U67" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V67" s="7" t="s">
+      <c r="M67" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N67" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:22">
+    <row r="68" spans="1:14" ht="16">
       <c r="A68" s="1" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="C68" s="3">
         <v>1.73E-5</v>
@@ -4922,45 +4119,21 @@
         <v>0</v>
       </c>
       <c r="K68" s="3">
-        <v>1.4800000000000001E-5</v>
-      </c>
-      <c r="L68" s="3">
-        <v>1.33E-5</v>
-      </c>
-      <c r="M68" s="3">
-        <v>1.22E-5</v>
-      </c>
-      <c r="N68" s="3">
-        <v>1.22E-5</v>
-      </c>
-      <c r="O68" s="24">
-        <v>0</v>
-      </c>
-      <c r="P68" s="3">
-        <v>1.1399999999999999E-5</v>
-      </c>
-      <c r="Q68" s="3">
-        <v>1.08E-5</v>
-      </c>
-      <c r="R68" s="3">
         <v>2.4000000000000001E-5</v>
       </c>
-      <c r="S68" s="3">
-        <v>3.0499999999999999E-5</v>
-      </c>
-      <c r="U68" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V68" s="7" t="s">
+      <c r="M68" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N68" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:22">
+    <row r="69" spans="1:14" ht="16">
       <c r="A69" s="1" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>323</v>
+        <v>302</v>
       </c>
       <c r="C69" s="3">
         <v>2.1399999999999998E-5</v>
@@ -4987,45 +4160,21 @@
         <v>0</v>
       </c>
       <c r="K69" s="3">
-        <v>1.7099999999999999E-5</v>
-      </c>
-      <c r="L69" s="3">
-        <v>1.56E-5</v>
-      </c>
-      <c r="M69" s="3">
-        <v>1.4399999999999999E-5</v>
-      </c>
-      <c r="N69" s="3">
-        <v>1.45E-5</v>
-      </c>
-      <c r="O69" s="24">
-        <v>0</v>
-      </c>
-      <c r="P69" s="3">
-        <v>1.34E-5</v>
-      </c>
-      <c r="Q69" s="3">
-        <v>1.2799999999999999E-5</v>
-      </c>
-      <c r="R69" s="3">
         <v>2.8E-5</v>
       </c>
-      <c r="S69" s="3">
-        <v>3.4700000000000003E-5</v>
-      </c>
-      <c r="U69" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V69" s="7" t="s">
+      <c r="M69" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N69" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:22">
+    <row r="70" spans="1:14" ht="16">
       <c r="A70" s="1" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>336</v>
+        <v>315</v>
       </c>
       <c r="C70" s="24">
         <v>0</v>
@@ -5050,29 +4199,19 @@
       </c>
       <c r="J70" s="25"/>
       <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
-      <c r="M70" s="3"/>
-      <c r="N70" s="3"/>
-      <c r="O70" s="25">
-        <v>3.7599999999999998E-4</v>
-      </c>
-      <c r="P70" s="3"/>
-      <c r="Q70" s="3"/>
-      <c r="R70" s="3"/>
-      <c r="S70" s="3"/>
-      <c r="U70" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V70" s="7" t="s">
+      <c r="M70" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N70" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="1:22">
+    <row r="71" spans="1:14" ht="16">
       <c r="A71" s="1" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="C71" s="3">
         <v>1.7930000000000001E-3</v>
@@ -5095,22 +4234,19 @@
       <c r="I71" s="24">
         <v>0</v>
       </c>
-      <c r="O71" s="3">
-        <v>2.7700000000000001E-4</v>
-      </c>
-      <c r="U71" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V71" s="7" t="s">
+      <c r="M71" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N71" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="72" spans="1:22">
+    <row r="72" spans="1:14" ht="16">
       <c r="A72" s="1" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="C72" s="3">
         <v>8.8999999999999995E-4</v>
@@ -5133,22 +4269,19 @@
       <c r="I72" s="3">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="O72" s="3">
-        <v>2.14E-4</v>
-      </c>
-      <c r="U72" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V72" s="7" t="s">
+      <c r="M72" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N72" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="73" spans="1:22">
+    <row r="73" spans="1:14" ht="16">
       <c r="A73" s="1" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
       <c r="C73" s="3">
         <v>5.4699999999999996E-4</v>
@@ -5168,19 +4301,19 @@
       <c r="I73" s="3">
         <v>1.17E-2</v>
       </c>
-      <c r="U73" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V73" s="7" t="s">
+      <c r="M73" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N73" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="74" spans="1:22">
+    <row r="74" spans="1:14" ht="16">
       <c r="A74" s="1" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="C74" s="3">
         <v>3.7800000000000003E-4</v>
@@ -5200,19 +4333,19 @@
       <c r="I74" s="3">
         <v>6.6E-3</v>
       </c>
-      <c r="U74" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V74" s="7" t="s">
+      <c r="M74" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N74" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:22">
+    <row r="75" spans="1:14" ht="16">
       <c r="A75" s="1" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="C75" s="3">
         <v>2.8200000000000002E-4</v>
@@ -5232,10 +4365,10 @@
       <c r="I75" s="3">
         <v>4.1000000000000003E-3</v>
       </c>
-      <c r="U75" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="V75" s="7" t="s">
+      <c r="M75" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="N75" s="7" t="s">
         <v>135</v>
       </c>
     </row>
@@ -5251,14 +4384,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.1640625" style="1" customWidth="1"/>
   </cols>
@@ -5370,18 +4503,18 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="B7" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
       <c r="B8" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -5483,7 +4616,7 @@
         <v>172</v>
       </c>
       <c r="B18" t="s">
-        <v>337</v>
+        <v>316</v>
       </c>
       <c r="C18">
         <v>91880</v>
@@ -5508,24 +4641,24 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="B20" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="C20" s="3">
         <v>38700000</v>
       </c>
       <c r="H20" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
       <c r="B21" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -5543,14 +4676,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Heat capacity parameters for CO2
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,39 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5EC943-47E1-424E-823E-27F3F73BEAB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="322">
   <si>
     <t>parvariable</t>
   </si>
@@ -999,25 +993,16 @@
   </si>
   <si>
     <t>deltaWall</t>
-  </si>
-  <si>
-    <t>mol s</t>
-  </si>
-  <si>
-    <t>Needed Output HCN</t>
-  </si>
-  <si>
-    <t>noutned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1139,7 +1124,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="150">
+  <cellStyleXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1234,6 +1219,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1319,156 +1308,160 @@
     <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="150">
-    <cellStyle name="Bad" xfId="93" builtinId="27"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+  <cellStyles count="154">
+    <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="153" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1527,7 +1520,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1579,7 +1572,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1773,21 +1766,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -1848,7 +1841,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" ht="16">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1887,7 +1880,7 @@
       </c>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" ht="16">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1926,7 +1919,7 @@
       </c>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" ht="16">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -1963,7 +1956,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" ht="16">
       <c r="A5" s="1" t="s">
         <v>132</v>
       </c>
@@ -2003,7 +1996,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" ht="16">
       <c r="A6" s="1" t="s">
         <v>118</v>
       </c>
@@ -2039,7 +2032,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" ht="16">
       <c r="A7" s="1" t="s">
         <v>111</v>
       </c>
@@ -2075,7 +2068,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" ht="16">
       <c r="A8" s="1" t="s">
         <v>119</v>
       </c>
@@ -2111,7 +2104,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" ht="16">
       <c r="A9" s="1" t="s">
         <v>125</v>
       </c>
@@ -2147,7 +2140,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" ht="16">
       <c r="A10" s="1" t="s">
         <v>120</v>
       </c>
@@ -2183,7 +2176,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" ht="16">
       <c r="A11" s="1" t="s">
         <v>126</v>
       </c>
@@ -2219,7 +2212,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" ht="16">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -2261,7 +2254,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" ht="16">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2280,7 +2273,7 @@
       <c r="L13" s="9"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" ht="16">
       <c r="A14" s="1" t="s">
         <v>103</v>
       </c>
@@ -2320,7 +2313,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" ht="16">
       <c r="A15" s="1" t="s">
         <v>109</v>
       </c>
@@ -2358,7 +2351,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" ht="16">
       <c r="A16" s="1" t="s">
         <v>142</v>
       </c>
@@ -2390,7 +2383,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" ht="16">
       <c r="A17" s="1" t="s">
         <v>140</v>
       </c>
@@ -2413,7 +2406,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" ht="16">
       <c r="A18" s="1" t="s">
         <v>157</v>
       </c>
@@ -2453,7 +2446,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" ht="16">
       <c r="A19" s="1" t="s">
         <v>158</v>
       </c>
@@ -2493,7 +2486,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" ht="16">
       <c r="A20" s="1" t="s">
         <v>161</v>
       </c>
@@ -2533,7 +2526,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" ht="16">
       <c r="A21" s="1" t="s">
         <v>167</v>
       </c>
@@ -2571,7 +2564,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" ht="16">
       <c r="A22" s="1" t="s">
         <v>168</v>
       </c>
@@ -2609,7 +2602,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" ht="16">
       <c r="A23" s="1" t="s">
         <v>173</v>
       </c>
@@ -2645,7 +2638,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" ht="16">
       <c r="A24" s="1" t="s">
         <v>175</v>
       </c>
@@ -2681,7 +2674,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" ht="16">
       <c r="A25" s="1" t="s">
         <v>184</v>
       </c>
@@ -2719,7 +2712,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" ht="16">
       <c r="A26" s="1" t="s">
         <v>186</v>
       </c>
@@ -2757,7 +2750,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" ht="16">
       <c r="A27" s="1" t="s">
         <v>188</v>
       </c>
@@ -2793,7 +2786,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" ht="16">
       <c r="A28" s="1" t="s">
         <v>194</v>
       </c>
@@ -2828,7 +2821,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" ht="16">
       <c r="A29" s="1" t="s">
         <v>208</v>
       </c>
@@ -2855,14 +2848,16 @@
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
+      <c r="K29" s="13">
+        <v>4.63659</v>
+      </c>
       <c r="L29" s="13"/>
       <c r="M29" s="7"/>
       <c r="N29" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" ht="16">
       <c r="A30" s="1" t="s">
         <v>209</v>
       </c>
@@ -2889,7 +2884,9 @@
       </c>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
+      <c r="K30" s="13">
+        <v>2.7413200000000002E-3</v>
+      </c>
       <c r="L30" s="13"/>
       <c r="M30" s="7" t="s">
         <v>179</v>
@@ -2898,7 +2895,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" ht="16">
       <c r="A31" s="1" t="s">
         <v>206</v>
       </c>
@@ -2925,7 +2922,9 @@
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
+      <c r="K31" s="13">
+        <v>-9.9582900000000002E-7</v>
+      </c>
       <c r="L31" s="13"/>
       <c r="M31" s="7" t="s">
         <v>180</v>
@@ -2934,7 +2933,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" ht="16">
       <c r="A32" s="1" t="s">
         <v>207</v>
       </c>
@@ -2961,7 +2960,9 @@
       </c>
       <c r="I32" s="13"/>
       <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
+      <c r="K32" s="13">
+        <v>1.6037300000000001E-10</v>
+      </c>
       <c r="L32" s="13"/>
       <c r="M32" s="7" t="s">
         <v>181</v>
@@ -2970,7 +2971,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" ht="16">
       <c r="A33" s="1" t="s">
         <v>210</v>
       </c>
@@ -2997,7 +2998,9 @@
       </c>
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
+      <c r="K33" s="13">
+        <v>-9.1610299999999997E-15</v>
+      </c>
       <c r="L33" s="13"/>
       <c r="M33" s="7" t="s">
         <v>182</v>
@@ -3006,7 +3009,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" ht="16">
       <c r="A34" s="1" t="s">
         <v>216</v>
       </c>
@@ -3033,7 +3036,9 @@
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
+      <c r="K34" s="13">
+        <v>-49024.9</v>
+      </c>
       <c r="L34" s="13"/>
       <c r="M34" s="7" t="s">
         <v>107</v>
@@ -3042,7 +3047,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" ht="16">
       <c r="A35" s="1" t="s">
         <v>217</v>
       </c>
@@ -3069,13 +3074,15 @@
       </c>
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
+      <c r="K35" s="13">
+        <v>-1.9353499999999999</v>
+      </c>
       <c r="L35" s="13"/>
       <c r="N35" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" ht="16">
       <c r="A36" s="1" t="s">
         <v>213</v>
       </c>
@@ -3102,13 +3109,15 @@
       </c>
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
+      <c r="K36" s="13">
+        <v>2.35677</v>
+      </c>
       <c r="L36" s="13"/>
       <c r="N36" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" ht="16">
       <c r="A37" s="1" t="s">
         <v>214</v>
       </c>
@@ -3135,7 +3144,9 @@
       </c>
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
+      <c r="K37" s="13">
+        <v>8.9847999999999994E-3</v>
+      </c>
       <c r="L37" s="13"/>
       <c r="M37" s="7" t="s">
         <v>179</v>
@@ -3144,7 +3155,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" ht="16">
       <c r="A38" s="1" t="s">
         <v>211</v>
       </c>
@@ -3171,7 +3182,9 @@
       </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
+      <c r="K38" s="13">
+        <v>-7.1235599999999996E-6</v>
+      </c>
       <c r="L38" s="13"/>
       <c r="M38" s="7" t="s">
         <v>180</v>
@@ -3180,7 +3193,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" ht="16">
       <c r="A39" s="1" t="s">
         <v>212</v>
       </c>
@@ -3207,7 +3220,9 @@
       </c>
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
+      <c r="K39" s="13">
+        <v>2.4591900000000001E-9</v>
+      </c>
       <c r="L39" s="13"/>
       <c r="M39" s="7" t="s">
         <v>181</v>
@@ -3216,7 +3231,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" ht="16">
       <c r="A40" s="1" t="s">
         <v>215</v>
       </c>
@@ -3243,7 +3258,9 @@
       </c>
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
+      <c r="K40" s="13">
+        <v>1.4370000000000001E-13</v>
+      </c>
       <c r="L40" s="13"/>
       <c r="M40" s="7" t="s">
         <v>182</v>
@@ -3252,7 +3269,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" ht="16">
       <c r="A41" s="1" t="s">
         <v>220</v>
       </c>
@@ -3279,7 +3296,9 @@
       </c>
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
+      <c r="K41" s="13">
+        <v>-48372</v>
+      </c>
       <c r="L41" s="13"/>
       <c r="M41" s="7" t="s">
         <v>107</v>
@@ -3288,7 +3307,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" ht="16">
       <c r="A42" s="1" t="s">
         <v>221</v>
       </c>
@@ -3315,13 +3334,15 @@
       </c>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
+      <c r="K42" s="13">
+        <v>9.9010499999999997</v>
+      </c>
       <c r="L42" s="13"/>
       <c r="N42" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" ht="16">
       <c r="A43" s="1" t="s">
         <v>227</v>
       </c>
@@ -3353,7 +3374,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" ht="16">
       <c r="A44" s="1" t="s">
         <v>229</v>
       </c>
@@ -3385,7 +3406,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" ht="16">
       <c r="A45" s="1" t="s">
         <v>238</v>
       </c>
@@ -3423,7 +3444,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" ht="16">
       <c r="A46" s="1" t="s">
         <v>243</v>
       </c>
@@ -3447,7 +3468,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" ht="16">
       <c r="A47" s="1" t="s">
         <v>250</v>
       </c>
@@ -3489,7 +3510,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" ht="16">
       <c r="A48" s="1" t="s">
         <v>251</v>
       </c>
@@ -3531,7 +3552,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" ht="16">
       <c r="A49" s="1" t="s">
         <v>252</v>
       </c>
@@ -3573,7 +3594,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" ht="16">
       <c r="A50" s="1" t="s">
         <v>253</v>
       </c>
@@ -3615,7 +3636,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" ht="16">
       <c r="A51" s="1" t="s">
         <v>254</v>
       </c>
@@ -3657,7 +3678,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" ht="16">
       <c r="A52" s="1" t="s">
         <v>255</v>
       </c>
@@ -3699,7 +3720,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" ht="16">
       <c r="A53" s="1" t="s">
         <v>267</v>
       </c>
@@ -3729,7 +3750,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" ht="16">
       <c r="A54" s="1" t="s">
         <v>268</v>
       </c>
@@ -3758,7 +3779,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" ht="16">
       <c r="A55" s="1" t="s">
         <v>269</v>
       </c>
@@ -3787,7 +3808,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" ht="16">
       <c r="A56" s="1" t="s">
         <v>270</v>
       </c>
@@ -3816,7 +3837,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" ht="16">
       <c r="A57" s="1" t="s">
         <v>271</v>
       </c>
@@ -3845,7 +3866,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" ht="16">
       <c r="A58" s="1" t="s">
         <v>272</v>
       </c>
@@ -3862,7 +3883,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" ht="16">
       <c r="A59" s="1" t="s">
         <v>278</v>
       </c>
@@ -3879,7 +3900,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" ht="16">
       <c r="A60" s="1" t="s">
         <v>279</v>
       </c>
@@ -3896,7 +3917,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" ht="16">
       <c r="A61" s="1" t="s">
         <v>280</v>
       </c>
@@ -3913,7 +3934,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" ht="16">
       <c r="A62" s="1" t="s">
         <v>281</v>
       </c>
@@ -3930,7 +3951,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" ht="16">
       <c r="A63" s="1" t="s">
         <v>287</v>
       </c>
@@ -3947,7 +3968,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" ht="16">
       <c r="A64" s="1" t="s">
         <v>290</v>
       </c>
@@ -3988,7 +4009,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" ht="16">
       <c r="A65" s="1" t="s">
         <v>292</v>
       </c>
@@ -4029,7 +4050,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" ht="16">
       <c r="A66" s="1" t="s">
         <v>293</v>
       </c>
@@ -4070,7 +4091,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" ht="16">
       <c r="A67" s="1" t="s">
         <v>294</v>
       </c>
@@ -4111,7 +4132,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" ht="16">
       <c r="A68" s="1" t="s">
         <v>295</v>
       </c>
@@ -4152,7 +4173,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" ht="16">
       <c r="A69" s="1" t="s">
         <v>296</v>
       </c>
@@ -4193,7 +4214,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" ht="16">
       <c r="A70" s="1" t="s">
         <v>313</v>
       </c>
@@ -4230,7 +4251,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" ht="16">
       <c r="A71" s="1" t="s">
         <v>303</v>
       </c>
@@ -4265,7 +4286,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" ht="16">
       <c r="A72" s="1" t="s">
         <v>305</v>
       </c>
@@ -4300,7 +4321,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" ht="16">
       <c r="A73" s="1" t="s">
         <v>306</v>
       </c>
@@ -4332,7 +4353,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" ht="16">
       <c r="A74" s="1" t="s">
         <v>307</v>
       </c>
@@ -4364,7 +4385,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" ht="16">
       <c r="A75" s="1" t="s">
         <v>308</v>
       </c>
@@ -4408,14 +4429,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.1640625" style="1" customWidth="1"/>
   </cols>
@@ -4703,20 +4724,6 @@
       </c>
       <c r="H22" t="s">
         <v>320</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B23" t="s">
-        <v>324</v>
-      </c>
-      <c r="G23">
-        <v>12.86</v>
-      </c>
-      <c r="H23" t="s">
-        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -4731,14 +4738,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Henry's constant parameters for CO2
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1776,8 +1776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3367,6 +3367,9 @@
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
+      <c r="K43" s="3">
+        <v>3.5000000000000003E-2</v>
+      </c>
       <c r="M43" s="7" t="s">
         <v>231</v>
       </c>
@@ -3399,6 +3402,9 @@
       </c>
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
+      <c r="K44" s="13">
+        <v>2400</v>
+      </c>
       <c r="M44" s="7" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
Reynolds number for outer stream added
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="324">
   <si>
     <t>parvariable</t>
   </si>
@@ -993,6 +993,12 @@
   </si>
   <si>
     <t>deltaWall</t>
+  </si>
+  <si>
+    <t>Reynolds number natural gas stream</t>
+  </si>
+  <si>
+    <t>Reout</t>
   </si>
 </sst>
 </file>
@@ -1766,7 +1772,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1776,7 +1782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="75" workbookViewId="0">
       <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
@@ -4436,15 +4442,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
@@ -4730,6 +4736,17 @@
       </c>
       <c r="H22" t="s">
         <v>320</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B23" t="s">
+        <v>323</v>
+      </c>
+      <c r="C23">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reynolds out auf 10'000
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,32 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638E2E2D-B82F-7D41-AFD8-14C2DE80C62C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -1046,11 +1040,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1379,171 +1373,171 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="166">
-    <cellStyle name="Bad" xfId="93" builtinId="27"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="165" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1848,21 +1842,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N81"/>
   <sheetViews>
     <sheetView topLeftCell="A59" zoomScale="75" workbookViewId="0">
       <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -1923,7 +1917,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" ht="16">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1962,7 +1956,7 @@
       </c>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" ht="16">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2001,7 +1995,7 @@
       </c>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" ht="16">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -2038,7 +2032,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" ht="16">
       <c r="A5" s="1" t="s">
         <v>132</v>
       </c>
@@ -2078,7 +2072,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" ht="16">
       <c r="A6" s="1" t="s">
         <v>118</v>
       </c>
@@ -2114,7 +2108,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" ht="16">
       <c r="A7" s="1" t="s">
         <v>111</v>
       </c>
@@ -2150,7 +2144,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" ht="16">
       <c r="A8" s="1" t="s">
         <v>119</v>
       </c>
@@ -2186,7 +2180,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" ht="16">
       <c r="A9" s="1" t="s">
         <v>125</v>
       </c>
@@ -2222,7 +2216,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" ht="16">
       <c r="A10" s="1" t="s">
         <v>120</v>
       </c>
@@ -2258,7 +2252,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" ht="16">
       <c r="A11" s="1" t="s">
         <v>126</v>
       </c>
@@ -2294,7 +2288,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" ht="16">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -2336,7 +2330,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" ht="16">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2355,7 +2349,7 @@
       <c r="L13" s="9"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" ht="16">
       <c r="A14" s="1" t="s">
         <v>103</v>
       </c>
@@ -2395,7 +2389,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" ht="16">
       <c r="A15" s="1" t="s">
         <v>109</v>
       </c>
@@ -2433,7 +2427,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" ht="16">
       <c r="A16" s="1" t="s">
         <v>142</v>
       </c>
@@ -2465,7 +2459,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" ht="16">
       <c r="A17" s="1" t="s">
         <v>140</v>
       </c>
@@ -2488,7 +2482,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" ht="16">
       <c r="A18" s="1" t="s">
         <v>157</v>
       </c>
@@ -2528,7 +2522,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" ht="16">
       <c r="A19" s="1" t="s">
         <v>158</v>
       </c>
@@ -2568,7 +2562,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" ht="16">
       <c r="A20" s="1" t="s">
         <v>161</v>
       </c>
@@ -2608,7 +2602,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" ht="16">
       <c r="A21" s="1" t="s">
         <v>167</v>
       </c>
@@ -2646,7 +2640,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" ht="16">
       <c r="A22" s="1" t="s">
         <v>168</v>
       </c>
@@ -2684,7 +2678,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" ht="16">
       <c r="A23" s="1" t="s">
         <v>173</v>
       </c>
@@ -2720,7 +2714,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" ht="16">
       <c r="A24" s="1" t="s">
         <v>175</v>
       </c>
@@ -2756,7 +2750,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" ht="16">
       <c r="A25" s="1" t="s">
         <v>184</v>
       </c>
@@ -2794,7 +2788,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" ht="16">
       <c r="A26" s="1" t="s">
         <v>186</v>
       </c>
@@ -2832,7 +2826,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" ht="16">
       <c r="A27" s="1" t="s">
         <v>188</v>
       </c>
@@ -2868,7 +2862,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" ht="16">
       <c r="A28" s="1" t="s">
         <v>194</v>
       </c>
@@ -2903,7 +2897,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" ht="16">
       <c r="A29" s="1" t="s">
         <v>208</v>
       </c>
@@ -2939,7 +2933,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" ht="16">
       <c r="A30" s="1" t="s">
         <v>209</v>
       </c>
@@ -2977,7 +2971,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" ht="16">
       <c r="A31" s="1" t="s">
         <v>206</v>
       </c>
@@ -3015,7 +3009,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" ht="16">
       <c r="A32" s="1" t="s">
         <v>207</v>
       </c>
@@ -3053,7 +3047,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" ht="16">
       <c r="A33" s="1" t="s">
         <v>210</v>
       </c>
@@ -3091,7 +3085,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" ht="16">
       <c r="A34" s="1" t="s">
         <v>216</v>
       </c>
@@ -3129,7 +3123,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" ht="16">
       <c r="A35" s="1" t="s">
         <v>217</v>
       </c>
@@ -3164,7 +3158,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" ht="16">
       <c r="A36" s="1" t="s">
         <v>213</v>
       </c>
@@ -3199,7 +3193,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" ht="16">
       <c r="A37" s="1" t="s">
         <v>214</v>
       </c>
@@ -3237,7 +3231,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" ht="16">
       <c r="A38" s="1" t="s">
         <v>211</v>
       </c>
@@ -3275,7 +3269,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" ht="16">
       <c r="A39" s="1" t="s">
         <v>212</v>
       </c>
@@ -3313,7 +3307,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" ht="16">
       <c r="A40" s="1" t="s">
         <v>215</v>
       </c>
@@ -3351,7 +3345,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" ht="16">
       <c r="A41" s="1" t="s">
         <v>220</v>
       </c>
@@ -3389,7 +3383,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" ht="16">
       <c r="A42" s="1" t="s">
         <v>221</v>
       </c>
@@ -3424,7 +3418,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" ht="16">
       <c r="A43" s="1" t="s">
         <v>227</v>
       </c>
@@ -3459,7 +3453,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" ht="16">
       <c r="A44" s="1" t="s">
         <v>229</v>
       </c>
@@ -3494,7 +3488,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" ht="16">
       <c r="A45" s="1" t="s">
         <v>238</v>
       </c>
@@ -3532,7 +3526,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" ht="16">
       <c r="A46" s="1" t="s">
         <v>243</v>
       </c>
@@ -3556,7 +3550,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" ht="16">
       <c r="A47" s="1" t="s">
         <v>250</v>
       </c>
@@ -3598,7 +3592,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" ht="16">
       <c r="A48" s="1" t="s">
         <v>251</v>
       </c>
@@ -3640,7 +3634,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" ht="16">
       <c r="A49" s="1" t="s">
         <v>252</v>
       </c>
@@ -3682,7 +3676,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" ht="16">
       <c r="A50" s="1" t="s">
         <v>253</v>
       </c>
@@ -3724,7 +3718,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" ht="16">
       <c r="A51" s="1" t="s">
         <v>254</v>
       </c>
@@ -3766,7 +3760,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" ht="16">
       <c r="A52" s="1" t="s">
         <v>255</v>
       </c>
@@ -3808,7 +3802,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" ht="16">
       <c r="A53" s="1" t="s">
         <v>267</v>
       </c>
@@ -3838,7 +3832,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" ht="16">
       <c r="A54" s="1" t="s">
         <v>268</v>
       </c>
@@ -3867,7 +3861,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" ht="16">
       <c r="A55" s="1" t="s">
         <v>269</v>
       </c>
@@ -3896,7 +3890,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" ht="16">
       <c r="A56" s="1" t="s">
         <v>270</v>
       </c>
@@ -3925,7 +3919,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" ht="16">
       <c r="A57" s="1" t="s">
         <v>271</v>
       </c>
@@ -3954,7 +3948,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" ht="16">
       <c r="A58" s="1" t="s">
         <v>272</v>
       </c>
@@ -3971,7 +3965,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" ht="16">
       <c r="A59" s="1" t="s">
         <v>278</v>
       </c>
@@ -3988,7 +3982,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" ht="16">
       <c r="A60" s="1" t="s">
         <v>279</v>
       </c>
@@ -4005,7 +3999,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" ht="16">
       <c r="A61" s="1" t="s">
         <v>280</v>
       </c>
@@ -4022,7 +4016,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" ht="16">
       <c r="A62" s="1" t="s">
         <v>281</v>
       </c>
@@ -4039,7 +4033,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" ht="16">
       <c r="A63" s="1" t="s">
         <v>287</v>
       </c>
@@ -4056,7 +4050,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" ht="16">
       <c r="A64" s="1" t="s">
         <v>290</v>
       </c>
@@ -4097,7 +4091,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" ht="16">
       <c r="A65" s="1" t="s">
         <v>292</v>
       </c>
@@ -4138,7 +4132,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" ht="16">
       <c r="A66" s="1" t="s">
         <v>293</v>
       </c>
@@ -4179,7 +4173,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" ht="16">
       <c r="A67" s="1" t="s">
         <v>294</v>
       </c>
@@ -4220,7 +4214,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" ht="16">
       <c r="A68" s="1" t="s">
         <v>295</v>
       </c>
@@ -4261,7 +4255,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" ht="16">
       <c r="A69" s="1" t="s">
         <v>296</v>
       </c>
@@ -4302,7 +4296,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" ht="16">
       <c r="A70" s="1" t="s">
         <v>313</v>
       </c>
@@ -4339,7 +4333,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" ht="16">
       <c r="A71" s="1" t="s">
         <v>303</v>
       </c>
@@ -4374,7 +4368,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" ht="16">
       <c r="A72" s="1" t="s">
         <v>305</v>
       </c>
@@ -4409,7 +4403,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" ht="16">
       <c r="A73" s="1" t="s">
         <v>306</v>
       </c>
@@ -4441,7 +4435,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" ht="16">
       <c r="A74" s="1" t="s">
         <v>307</v>
       </c>
@@ -4473,7 +4467,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" ht="16">
       <c r="A75" s="1" t="s">
         <v>308</v>
       </c>
@@ -4505,7 +4499,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" ht="16">
       <c r="A76" s="1" t="s">
         <v>324</v>
       </c>
@@ -4534,7 +4528,7 @@
         <v>18.811</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" ht="16">
       <c r="A77" s="1" t="s">
         <v>325</v>
       </c>
@@ -4563,7 +4557,7 @@
         <v>0.49837999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" ht="16">
       <c r="A78" s="1" t="s">
         <v>326</v>
       </c>
@@ -4592,7 +4586,7 @@
         <v>-1.0851E-4</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" ht="16">
       <c r="A79" s="1" t="s">
         <v>330</v>
       </c>
@@ -4621,7 +4615,7 @@
         <v>-1.2E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" ht="16">
       <c r="A80" s="1" t="s">
         <v>333</v>
       </c>
@@ -4650,7 +4644,7 @@
         <v>1.0208E-4</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" ht="16">
       <c r="A81" s="1" t="s">
         <v>332</v>
       </c>
@@ -4691,14 +4685,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32" style="1" customWidth="1"/>
   </cols>
@@ -4997,7 +4991,7 @@
         <v>323</v>
       </c>
       <c r="C23" s="26">
-        <v>2000</v>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -5012,14 +5006,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Part trashed for clarity (but local copy on my computer if needed)
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="275">
   <si>
     <t>parvariable</t>
   </si>
@@ -779,105 +779,6 @@
     <t>UnionGas</t>
   </si>
   <si>
-    <t>Thermal conductivity of gas at 100K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity of gas at 200K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity of gas at 300K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity of gas at 400K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity of gas at 500K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity of gas at 600K</t>
-  </si>
-  <si>
-    <t>lambdagas100</t>
-  </si>
-  <si>
-    <t>lambdagas200</t>
-  </si>
-  <si>
-    <t>lambdagas300</t>
-  </si>
-  <si>
-    <t>lambdagas400</t>
-  </si>
-  <si>
-    <t>lambdagas500</t>
-  </si>
-  <si>
-    <t>lambdagas600</t>
-  </si>
-  <si>
-    <t>lambdaliq273</t>
-  </si>
-  <si>
-    <t>lambdaliq298</t>
-  </si>
-  <si>
-    <t>lambdaliq323</t>
-  </si>
-  <si>
-    <t>lambdaliq348</t>
-  </si>
-  <si>
-    <t>lambdaliq373</t>
-  </si>
-  <si>
-    <t>Thermal conductivity of liquid at 273.16K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity of liquid at 298.16K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity of liquid at 323.16K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity of liquid at 348.16K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity of liquid at 373.16K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity at 253.16K</t>
-  </si>
-  <si>
-    <t>lambda253</t>
-  </si>
-  <si>
-    <t>lambda273</t>
-  </si>
-  <si>
-    <t>lambda293</t>
-  </si>
-  <si>
-    <t>lambda313</t>
-  </si>
-  <si>
-    <t>lambda333</t>
-  </si>
-  <si>
-    <t>Thermal conductivity at 273.16K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity at 293.16K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity at 313.16K</t>
-  </si>
-  <si>
-    <t>Thermal conductivity at 333.16K</t>
-  </si>
-  <si>
-    <t>W.m-1.K-1</t>
-  </si>
-  <si>
     <t>SegmentArea</t>
   </si>
   <si>
@@ -888,90 +789,6 @@
   </si>
   <si>
     <t>As</t>
-  </si>
-  <si>
-    <t>Thermal conductivity of liquid at 300K</t>
-  </si>
-  <si>
-    <t>lambdaliq300</t>
-  </si>
-  <si>
-    <t>EngineeringToolBox</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of gases at 100 K</t>
-  </si>
-  <si>
-    <t>mugas100</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of gases at 200 K</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of gases at 300 K</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of gases at 400 K</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of gases at 500 K</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of gases at 600 K</t>
-  </si>
-  <si>
-    <t>mugas200</t>
-  </si>
-  <si>
-    <t>mugas300</t>
-  </si>
-  <si>
-    <t>mugas400</t>
-  </si>
-  <si>
-    <t>mugas500</t>
-  </si>
-  <si>
-    <t>mugas600</t>
-  </si>
-  <si>
-    <t>Pa.s</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of liquid at 273.16 K</t>
-  </si>
-  <si>
-    <t>muliq273</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of liquid at 298.16 K</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of liquid at 323.16 K</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of liquid at 348.16 K</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of liquid at 373.16 K</t>
-  </si>
-  <si>
-    <t>muliq298</t>
-  </si>
-  <si>
-    <t>muliq323</t>
-  </si>
-  <si>
-    <t>muliq348</t>
-  </si>
-  <si>
-    <t>muliq373</t>
-  </si>
-  <si>
-    <t>Dynamic viscosity of liquid at 248.16 K</t>
-  </si>
-  <si>
-    <t>muliq248</t>
   </si>
   <si>
     <t>deltaHNH</t>
@@ -1044,7 +861,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1108,13 +925,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1146,18 +958,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFA6A9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9CB1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1340,7 +1140,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1356,18 +1156,12 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="93" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1842,7 +1636,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1850,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N81"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1905,7 +1699,7 @@
         <v>62</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>317</v>
+        <v>256</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>64</v>
@@ -3460,20 +3254,20 @@
       <c r="B44" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15">
         <v>1300</v>
       </c>
-      <c r="E44" s="18">
+      <c r="E44" s="15">
         <v>1600</v>
       </c>
-      <c r="F44" s="18">
+      <c r="F44" s="15">
         <v>4200</v>
       </c>
-      <c r="G44" s="18">
+      <c r="G44" s="15">
         <v>500</v>
       </c>
-      <c r="H44" s="18">
+      <c r="H44" s="15">
         <v>5000</v>
       </c>
       <c r="I44" s="13"/>
@@ -3495,22 +3289,22 @@
       <c r="B45" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="C45" s="19">
+      <c r="C45" s="16">
         <v>75.349999999999994</v>
       </c>
-      <c r="D45" s="20">
-        <v>0</v>
-      </c>
-      <c r="E45" s="20">
-        <v>0</v>
-      </c>
-      <c r="F45" s="20">
-        <v>0</v>
-      </c>
-      <c r="G45" s="20">
-        <v>0</v>
-      </c>
-      <c r="H45" s="19">
+      <c r="D45" s="17">
+        <v>0</v>
+      </c>
+      <c r="E45" s="17">
+        <v>0</v>
+      </c>
+      <c r="F45" s="17">
+        <v>0</v>
+      </c>
+      <c r="G45" s="17">
+        <v>0</v>
+      </c>
+      <c r="H45" s="16">
         <v>70.63</v>
       </c>
       <c r="I45" s="9">
@@ -3533,16 +3327,16 @@
       <c r="B46" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="18">
+      <c r="C46" s="18"/>
+      <c r="D46" s="15">
         <v>0.01</v>
       </c>
-      <c r="E46" s="21">
+      <c r="E46" s="18">
         <v>0.93899999999999995</v>
       </c>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
       <c r="K46" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -3552,1124 +3346,175 @@
     </row>
     <row r="47" spans="1:14" ht="16">
       <c r="A47" s="1" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="C47" s="15">
-        <v>0</v>
-      </c>
-      <c r="D47" s="13">
-        <v>9.4000000000000004E-3</v>
-      </c>
-      <c r="E47" s="3">
-        <v>1.04E-2</v>
-      </c>
-      <c r="F47" s="15">
-        <v>0</v>
-      </c>
-      <c r="G47" s="13">
-        <v>6.8199999999999997E-2</v>
-      </c>
-      <c r="H47" s="16">
-        <v>0</v>
-      </c>
-      <c r="I47" s="16">
-        <v>0</v>
-      </c>
-      <c r="J47" s="16">
-        <v>0</v>
-      </c>
-      <c r="K47" s="16">
-        <v>0</v>
-      </c>
-      <c r="L47" s="18"/>
-      <c r="M47" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N47" s="7" t="s">
-        <v>134</v>
+        <v>266</v>
+      </c>
+      <c r="C47" s="3">
+        <v>-36.826000000000001</v>
+      </c>
+      <c r="D47" s="19">
+        <v>42.606000000000002</v>
+      </c>
+      <c r="E47" s="22">
+        <v>3.8439999999999999</v>
+      </c>
+      <c r="F47" s="22">
+        <v>-7.8739999999999997</v>
+      </c>
+      <c r="G47" s="22">
+        <v>27.757999999999999</v>
+      </c>
+      <c r="H47" s="21">
+        <v>-8.4860000000000007</v>
+      </c>
+      <c r="K47">
+        <v>18.811</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="16">
       <c r="A48" s="1" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="C48" s="15">
-        <v>0</v>
-      </c>
-      <c r="D48" s="13">
-        <v>1.83E-2</v>
-      </c>
-      <c r="E48" s="3">
-        <v>2.18E-2</v>
-      </c>
-      <c r="F48" s="15">
-        <v>0</v>
-      </c>
-      <c r="G48" s="13">
-        <v>0.1328</v>
-      </c>
-      <c r="H48" s="16">
-        <v>0</v>
-      </c>
-      <c r="I48" s="16">
-        <v>0</v>
-      </c>
-      <c r="J48" s="16">
-        <v>0</v>
-      </c>
-      <c r="K48" s="13">
-        <v>9.5999999999999992E-3</v>
-      </c>
-      <c r="L48" s="18"/>
-      <c r="M48" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N48" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" ht="16">
+        <v>267</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="E48" s="23">
+        <v>0.40111999999999998</v>
+      </c>
+      <c r="F48" s="23">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="G48" s="23">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="H48" s="23">
+        <v>9.0368000000000004E-2</v>
+      </c>
+      <c r="K48" s="3">
+        <v>0.49837999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="16">
       <c r="A49" s="1" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="C49" s="3">
-        <v>1.8599999999999998E-2</v>
-      </c>
-      <c r="D49" s="13">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="E49" s="3">
-        <v>3.44E-2</v>
-      </c>
-      <c r="F49" s="3">
-        <v>2.5100000000000001E-2</v>
-      </c>
-      <c r="G49" s="13">
-        <v>0.18659999999999999</v>
-      </c>
-      <c r="H49" s="16">
-        <v>0</v>
-      </c>
-      <c r="I49" s="16">
-        <v>0</v>
-      </c>
-      <c r="J49" s="16">
-        <v>0</v>
-      </c>
-      <c r="K49" s="13">
-        <v>1.6799999999999999E-2</v>
-      </c>
-      <c r="L49" s="18"/>
-      <c r="M49" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N49" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="16">
+        <v>-1.6200000000000001E-5</v>
+      </c>
+      <c r="D49" s="3">
+        <v>-9.8800000000000003E-5</v>
+      </c>
+      <c r="E49" s="23">
+        <v>-1.4302999999999999E-4</v>
+      </c>
+      <c r="F49" s="23">
+        <v>-4.4700000000000004E-6</v>
+      </c>
+      <c r="G49" s="23">
+        <v>-3.2799999999999998E-5</v>
+      </c>
+      <c r="H49" s="23">
+        <v>7.9146000000000004E-5</v>
+      </c>
+      <c r="K49" s="3">
+        <v>-1.0851E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="16">
       <c r="A50" s="1" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="C50" s="3">
-        <v>2.6100000000000002E-2</v>
-      </c>
-      <c r="D50" s="13">
-        <v>3.2800000000000003E-2</v>
-      </c>
-      <c r="E50" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="F50" s="3">
-        <v>3.7199999999999997E-2</v>
-      </c>
-      <c r="G50" s="13">
-        <v>0.23089999999999999</v>
-      </c>
-      <c r="H50" s="16">
-        <v>0</v>
-      </c>
-      <c r="I50" s="16">
-        <v>0</v>
-      </c>
-      <c r="J50" s="16">
-        <v>0</v>
-      </c>
-      <c r="K50" s="13">
-        <v>2.52E-2</v>
-      </c>
-      <c r="L50" s="18"/>
-      <c r="M50" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N50" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" ht="16">
+        <v>5.2999999999999998E-4</v>
+      </c>
+      <c r="D50" s="3">
+        <v>3.0899999999999999E-3</v>
+      </c>
+      <c r="E50" s="23">
+        <v>-9.3500000000000007E-3</v>
+      </c>
+      <c r="F50" s="23">
+        <v>4.5700000000000003E-3</v>
+      </c>
+      <c r="G50" s="23">
+        <v>3.9510000000000003E-2</v>
+      </c>
+      <c r="H50" s="21">
+        <v>-1.3600000000000001E-3</v>
+      </c>
+      <c r="K50">
+        <v>-1.2E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="16">
       <c r="A51" s="1" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="C51" s="3">
-        <v>3.56E-2</v>
-      </c>
-      <c r="D51" s="13">
-        <v>3.9E-2</v>
+        <v>4.7092999999999998E-5</v>
+      </c>
+      <c r="D51" s="3">
+        <v>7.593E-5</v>
       </c>
       <c r="E51" s="3">
-        <v>6.8400000000000002E-2</v>
+        <v>1.4028000000000001E-4</v>
       </c>
       <c r="F51" s="3">
-        <v>5.3100000000000001E-2</v>
-      </c>
-      <c r="G51" s="13">
-        <v>0.27089999999999997</v>
-      </c>
-      <c r="H51" s="16">
-        <v>0</v>
-      </c>
-      <c r="I51" s="16">
-        <v>0</v>
-      </c>
-      <c r="J51" s="16">
-        <v>0</v>
-      </c>
-      <c r="K51" s="13">
-        <v>3.3500000000000002E-2</v>
-      </c>
-      <c r="L51" s="18"/>
-      <c r="M51" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N51" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="16">
+        <v>2.3238999999999999E-5</v>
+      </c>
+      <c r="G51" s="3">
+        <v>4.5918E-4</v>
+      </c>
+      <c r="H51" s="3">
+        <v>3.7886000000000003E-5</v>
+      </c>
+      <c r="K51" s="3">
+        <v>1.0208E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="16">
       <c r="A52" s="1" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>261</v>
+        <v>274</v>
       </c>
       <c r="C52" s="3">
-        <v>4.6199999999999998E-2</v>
-      </c>
-      <c r="D52" s="13">
-        <v>4.48E-2</v>
+        <v>4.9550999999999998E-8</v>
+      </c>
+      <c r="D52" s="3">
+        <v>-1.1014E-8</v>
       </c>
       <c r="E52" s="3">
-        <v>8.8599999999999998E-2</v>
+        <v>3.3180000000000003E-8</v>
       </c>
       <c r="F52" s="3">
-        <v>6.8599999999999994E-2</v>
-      </c>
-      <c r="G52" s="13">
-        <v>0.30909999999999999</v>
-      </c>
-      <c r="H52" s="16">
-        <v>0</v>
-      </c>
-      <c r="I52" s="16">
-        <v>0</v>
-      </c>
-      <c r="J52" s="16">
-        <v>0</v>
-      </c>
-      <c r="K52" s="13">
-        <v>4.1599999999999998E-2</v>
-      </c>
-      <c r="L52" s="18"/>
-      <c r="M52" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N52" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" ht="16">
-      <c r="A53" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="C53">
-        <v>0.55620000000000003</v>
-      </c>
-      <c r="D53" s="16">
-        <v>0</v>
-      </c>
-      <c r="E53" s="17">
-        <v>0</v>
-      </c>
-      <c r="F53" s="17">
-        <v>0</v>
-      </c>
-      <c r="G53" s="16">
-        <v>0</v>
-      </c>
-      <c r="H53" s="3"/>
-      <c r="M53" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="N53" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" ht="16">
-      <c r="A54" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="C54">
-        <v>0.60619999999999996</v>
-      </c>
-      <c r="D54" s="16">
-        <v>0</v>
-      </c>
-      <c r="E54" s="17">
-        <v>0</v>
-      </c>
-      <c r="F54" s="17">
-        <v>0</v>
-      </c>
-      <c r="G54" s="16">
-        <v>0</v>
-      </c>
-      <c r="M54" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="N54" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" ht="16">
-      <c r="A55" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="C55">
-        <v>0.64229999999999998</v>
-      </c>
-      <c r="D55" s="16">
-        <v>0</v>
-      </c>
-      <c r="E55" s="17">
-        <v>0</v>
-      </c>
-      <c r="F55" s="17">
-        <v>0</v>
-      </c>
-      <c r="G55" s="16">
-        <v>0</v>
-      </c>
-      <c r="M55" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="N55" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" ht="16">
-      <c r="A56" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="C56">
-        <v>0.6643</v>
-      </c>
-      <c r="D56" s="16">
-        <v>0</v>
-      </c>
-      <c r="E56" s="17">
-        <v>0</v>
-      </c>
-      <c r="F56" s="17">
-        <v>0</v>
-      </c>
-      <c r="G56" s="16">
-        <v>0</v>
-      </c>
-      <c r="M56" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="N56" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" ht="16">
-      <c r="A57" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="C57">
-        <v>0.67290000000000005</v>
-      </c>
-      <c r="D57" s="16">
-        <v>0</v>
-      </c>
-      <c r="E57" s="17">
-        <v>0</v>
-      </c>
-      <c r="F57" s="17">
-        <v>0</v>
-      </c>
-      <c r="G57" s="16">
-        <v>0</v>
-      </c>
-      <c r="M57" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="N57" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="16">
-      <c r="A58" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="H58" s="3">
-        <v>9.9000000000000008E-3</v>
-      </c>
-      <c r="M58" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="N58" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" ht="16">
-      <c r="A59" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="H59" s="3">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="M59" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="N59" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" ht="16">
-      <c r="A60" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="H60" s="3">
-        <v>1.21E-2</v>
-      </c>
-      <c r="M60" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="N60" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" ht="16">
-      <c r="A61" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="H61" s="3">
-        <v>1.32E-2</v>
-      </c>
-      <c r="M61" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="N61" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="16">
-      <c r="A62" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="H62" s="3">
-        <v>1.43E-2</v>
-      </c>
-      <c r="M62" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="N62" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" ht="16">
-      <c r="A63" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="I63">
-        <v>0.5</v>
-      </c>
-      <c r="M63" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="N63" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" ht="16">
-      <c r="A64" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C64" s="22">
-        <v>0</v>
-      </c>
-      <c r="D64" s="3">
-        <v>6.9999999999999999E-6</v>
-      </c>
-      <c r="E64" s="3">
-        <v>3.8999999999999999E-6</v>
-      </c>
-      <c r="F64" s="23">
-        <v>0</v>
-      </c>
-      <c r="G64" s="3">
-        <v>4.0999999999999997E-6</v>
-      </c>
-      <c r="H64" s="24">
-        <v>0</v>
-      </c>
-      <c r="I64" s="24">
-        <v>0</v>
-      </c>
-      <c r="J64" s="24">
-        <v>0</v>
-      </c>
-      <c r="K64" s="24">
-        <v>0</v>
-      </c>
-      <c r="M64" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N64" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" ht="16">
-      <c r="A65" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="C65" s="22">
-        <v>0</v>
-      </c>
-      <c r="D65" s="3">
-        <v>1.29E-5</v>
-      </c>
-      <c r="E65" s="3">
-        <v>7.7000000000000008E-6</v>
-      </c>
-      <c r="F65" s="23">
-        <v>0</v>
-      </c>
-      <c r="G65" s="3">
-        <v>6.8000000000000001E-6</v>
-      </c>
-      <c r="H65" s="24">
-        <v>0</v>
-      </c>
-      <c r="I65" s="24">
-        <v>0</v>
-      </c>
-      <c r="J65" s="24">
-        <v>0</v>
-      </c>
-      <c r="K65" s="3">
-        <v>1.01E-5</v>
-      </c>
-      <c r="M65" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N65" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" ht="16">
-      <c r="A66" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="C66" s="3">
-        <v>9.7999999999999993E-6</v>
-      </c>
-      <c r="D66" s="3">
-        <v>1.7900000000000001E-5</v>
-      </c>
-      <c r="E66" s="3">
-        <v>1.11E-5</v>
-      </c>
-      <c r="F66" s="3">
-        <v>1.0200000000000001E-5</v>
-      </c>
-      <c r="G66" s="3">
-        <v>8.8999999999999995E-6</v>
-      </c>
-      <c r="H66" s="24">
-        <v>0</v>
-      </c>
-      <c r="I66" s="24">
-        <v>0</v>
-      </c>
-      <c r="J66" s="24">
-        <v>0</v>
-      </c>
-      <c r="K66" s="3">
-        <v>1.5E-5</v>
-      </c>
-      <c r="M66" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N66" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" ht="16">
-      <c r="A67" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C67" s="3">
-        <v>1.34E-5</v>
-      </c>
-      <c r="D67" s="3">
-        <v>2.2200000000000001E-5</v>
-      </c>
-      <c r="E67" s="3">
-        <v>1.42E-5</v>
-      </c>
-      <c r="F67" s="3">
-        <v>1.4E-5</v>
-      </c>
-      <c r="G67" s="3">
-        <v>1.0900000000000001E-5</v>
-      </c>
-      <c r="H67" s="24">
-        <v>0</v>
-      </c>
-      <c r="I67" s="24">
-        <v>0</v>
-      </c>
-      <c r="J67" s="24">
-        <v>0</v>
-      </c>
-      <c r="K67" s="3">
-        <v>1.9700000000000001E-5</v>
-      </c>
-      <c r="M67" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N67" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="16">
-      <c r="A68" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="C68" s="3">
-        <v>1.73E-5</v>
-      </c>
-      <c r="D68" s="3">
-        <v>2.6100000000000001E-5</v>
-      </c>
-      <c r="E68" s="3">
-        <v>1.7E-5</v>
-      </c>
-      <c r="F68" s="3">
-        <v>1.7900000000000001E-5</v>
-      </c>
-      <c r="G68" s="3">
-        <v>1.2799999999999999E-5</v>
-      </c>
-      <c r="H68" s="24">
-        <v>0</v>
-      </c>
-      <c r="I68" s="24">
-        <v>0</v>
-      </c>
-      <c r="J68" s="24">
-        <v>0</v>
-      </c>
-      <c r="K68" s="3">
-        <v>2.4000000000000001E-5</v>
-      </c>
-      <c r="M68" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N68" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" ht="16">
-      <c r="A69" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="C69" s="3">
-        <v>2.1399999999999998E-5</v>
-      </c>
-      <c r="D69" s="3">
-        <v>2.9600000000000001E-5</v>
-      </c>
-      <c r="E69" s="3">
-        <v>1.95E-5</v>
-      </c>
-      <c r="F69" s="3">
-        <v>2.1699999999999999E-5</v>
-      </c>
-      <c r="G69" s="3">
-        <v>1.45E-5</v>
-      </c>
-      <c r="H69" s="24">
-        <v>0</v>
-      </c>
-      <c r="I69" s="24">
-        <v>0</v>
-      </c>
-      <c r="J69" s="24">
-        <v>0</v>
-      </c>
-      <c r="K69" s="3">
-        <v>2.8E-5</v>
-      </c>
-      <c r="M69" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N69" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" ht="16">
-      <c r="A70" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="C70" s="24">
-        <v>0</v>
-      </c>
-      <c r="D70" s="24">
-        <v>0</v>
-      </c>
-      <c r="E70" s="24">
-        <v>0</v>
-      </c>
-      <c r="F70" s="24">
-        <v>0</v>
-      </c>
-      <c r="G70" s="24">
-        <v>0</v>
-      </c>
-      <c r="H70" s="24">
-        <v>0</v>
-      </c>
-      <c r="I70" s="24">
-        <v>0</v>
-      </c>
-      <c r="J70" s="25"/>
-      <c r="K70" s="3"/>
-      <c r="M70" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N70" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" ht="16">
-      <c r="A71" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="C71" s="3">
-        <v>1.7930000000000001E-3</v>
-      </c>
-      <c r="D71" s="24">
-        <v>0</v>
-      </c>
-      <c r="E71" s="24">
-        <v>0</v>
-      </c>
-      <c r="F71" s="24">
-        <v>0</v>
-      </c>
-      <c r="G71" s="24">
-        <v>0</v>
-      </c>
-      <c r="H71" s="3">
-        <v>2.3499999999999999E-4</v>
-      </c>
-      <c r="I71" s="24">
-        <v>0</v>
-      </c>
-      <c r="M71" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N71" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" ht="16">
-      <c r="A72" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="C72" s="3">
-        <v>8.8999999999999995E-4</v>
-      </c>
-      <c r="D72" s="24">
-        <v>0</v>
-      </c>
-      <c r="E72" s="24">
-        <v>0</v>
-      </c>
-      <c r="F72" s="24">
-        <v>0</v>
-      </c>
-      <c r="G72" s="24">
-        <v>0</v>
-      </c>
-      <c r="H72" s="3">
-        <v>1.83E-4</v>
-      </c>
-      <c r="I72" s="3">
-        <v>2.3800000000000002E-2</v>
-      </c>
-      <c r="M72" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N72" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" ht="16">
-      <c r="A73" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="C73" s="3">
-        <v>5.4699999999999996E-4</v>
-      </c>
-      <c r="D73" s="24">
-        <v>0</v>
-      </c>
-      <c r="E73" s="24">
-        <v>0</v>
-      </c>
-      <c r="F73" s="24">
-        <v>0</v>
-      </c>
-      <c r="G73" s="24">
-        <v>0</v>
-      </c>
-      <c r="I73" s="3">
-        <v>1.17E-2</v>
-      </c>
-      <c r="M73" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N73" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" ht="16">
-      <c r="A74" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="C74" s="3">
-        <v>3.7800000000000003E-4</v>
-      </c>
-      <c r="D74" s="24">
-        <v>0</v>
-      </c>
-      <c r="E74" s="24">
-        <v>0</v>
-      </c>
-      <c r="F74" s="24">
-        <v>0</v>
-      </c>
-      <c r="G74" s="24">
-        <v>0</v>
-      </c>
-      <c r="I74" s="3">
-        <v>6.6E-3</v>
-      </c>
-      <c r="M74" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N74" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" ht="16">
-      <c r="A75" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="C75" s="3">
-        <v>2.8200000000000002E-4</v>
-      </c>
-      <c r="D75" s="24">
-        <v>0</v>
-      </c>
-      <c r="E75" s="24">
-        <v>0</v>
-      </c>
-      <c r="F75" s="24">
-        <v>0</v>
-      </c>
-      <c r="G75" s="24">
-        <v>0</v>
-      </c>
-      <c r="I75" s="3">
-        <v>4.1000000000000003E-3</v>
-      </c>
-      <c r="M75" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="N75" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" ht="16">
-      <c r="A76" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="C76" s="3">
-        <v>-36.826000000000001</v>
-      </c>
-      <c r="D76" s="25">
-        <v>42.606000000000002</v>
-      </c>
-      <c r="E76" s="28">
-        <v>3.8439999999999999</v>
-      </c>
-      <c r="F76" s="28">
-        <v>-7.8739999999999997</v>
-      </c>
-      <c r="G76" s="28">
-        <v>27.757999999999999</v>
-      </c>
-      <c r="H76" s="27">
-        <v>-8.4860000000000007</v>
-      </c>
-      <c r="K76">
-        <v>18.811</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" ht="16">
-      <c r="A77" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="C77" s="3">
-        <v>0.42899999999999999</v>
-      </c>
-      <c r="D77" s="3">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="E77" s="29">
-        <v>0.40111999999999998</v>
-      </c>
-      <c r="F77" s="29">
-        <v>0.36699999999999999</v>
-      </c>
-      <c r="G77" s="29">
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="H77" s="29">
-        <v>9.0368000000000004E-2</v>
-      </c>
-      <c r="K77" s="3">
-        <v>0.49837999999999999</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" ht="16">
-      <c r="A78" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="C78" s="3">
-        <v>-1.6200000000000001E-5</v>
-      </c>
-      <c r="D78" s="3">
-        <v>-9.8800000000000003E-5</v>
-      </c>
-      <c r="E78" s="29">
-        <v>-1.4302999999999999E-4</v>
-      </c>
-      <c r="F78" s="29">
-        <v>-4.4700000000000004E-6</v>
-      </c>
-      <c r="G78" s="29">
-        <v>-3.2799999999999998E-5</v>
-      </c>
-      <c r="H78" s="29">
-        <v>7.9146000000000004E-5</v>
-      </c>
-      <c r="K78" s="3">
-        <v>-1.0851E-4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" ht="16">
-      <c r="A79" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="C79" s="3">
-        <v>5.2999999999999998E-4</v>
-      </c>
-      <c r="D79" s="3">
-        <v>3.0899999999999999E-3</v>
-      </c>
-      <c r="E79" s="29">
-        <v>-9.3500000000000007E-3</v>
-      </c>
-      <c r="F79" s="29">
-        <v>4.5700000000000003E-3</v>
-      </c>
-      <c r="G79" s="29">
-        <v>3.9510000000000003E-2</v>
-      </c>
-      <c r="H79" s="27">
-        <v>-1.3600000000000001E-3</v>
-      </c>
-      <c r="K79">
-        <v>-1.2E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" ht="16">
-      <c r="A80" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="C80" s="3">
-        <v>4.7092999999999998E-5</v>
-      </c>
-      <c r="D80" s="3">
-        <v>7.593E-5</v>
-      </c>
-      <c r="E80" s="3">
-        <v>1.4028000000000001E-4</v>
-      </c>
-      <c r="F80" s="3">
-        <v>2.3238999999999999E-5</v>
-      </c>
-      <c r="G80" s="3">
-        <v>4.5918E-4</v>
-      </c>
-      <c r="H80" s="3">
-        <v>3.7886000000000003E-5</v>
-      </c>
-      <c r="K80" s="3">
-        <v>1.0208E-4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" ht="16">
-      <c r="A81" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="C81" s="3">
-        <v>4.9550999999999998E-8</v>
-      </c>
-      <c r="D81" s="3">
-        <v>-1.1014E-8</v>
-      </c>
-      <c r="E81" s="3">
-        <v>3.3180000000000003E-8</v>
-      </c>
-      <c r="F81" s="3">
         <v>1.4810000000000001E-7</v>
       </c>
-      <c r="G81" s="3">
+      <c r="G52" s="3">
         <v>-6.4933000000000003E-8</v>
       </c>
-      <c r="H81" s="3">
+      <c r="H52" s="3">
         <v>2.6807E-8</v>
       </c>
-      <c r="K81" s="3">
+      <c r="K52" s="3">
         <v>-2.2402999999999999E-8</v>
       </c>
     </row>
@@ -4688,7 +3533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -4793,7 +3638,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>319</v>
+        <v>258</v>
       </c>
       <c r="B6" t="s">
         <v>45</v>
@@ -4803,23 +3648,23 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="H6" t="s">
-        <v>320</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>285</v>
+        <v>252</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>283</v>
+        <v>250</v>
       </c>
       <c r="B8" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4921,7 +3766,7 @@
         <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>315</v>
+        <v>254</v>
       </c>
       <c r="C18">
         <v>91880</v>
@@ -4960,10 +3805,10 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>316</v>
+        <v>255</v>
       </c>
       <c r="B21" t="s">
-        <v>316</v>
+        <v>255</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -4971,26 +3816,26 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>318</v>
+        <v>257</v>
       </c>
       <c r="B22" t="s">
-        <v>321</v>
+        <v>260</v>
       </c>
       <c r="C22" s="3">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="H22" t="s">
-        <v>320</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>322</v>
+        <v>261</v>
       </c>
       <c r="B23" t="s">
-        <v>323</v>
-      </c>
-      <c r="C23" s="26">
+        <v>262</v>
+      </c>
+      <c r="C23" s="20">
         <v>10000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Heat of combustion of methane and hydrogen added
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9560" yWindow="0" windowWidth="17780" windowHeight="14820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="290">
   <si>
     <t>parvariable</t>
   </si>
@@ -888,6 +888,15 @@
   </si>
   <si>
     <t>price_H2SO4</t>
+  </si>
+  <si>
+    <t>Heat of combustion</t>
+  </si>
+  <si>
+    <t>deltaHc</t>
+  </si>
+  <si>
+    <t>Pittam(CH4),  The Hydrogen Economy: Opportunities, Costs, Barriers, and R&amp;D Needs(H2)</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1017,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="166">
+  <cellStyleXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1103,6 +1112,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1201,7 +1220,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="166">
+  <cellStyles count="176">
     <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
@@ -1285,6 +1304,11 @@
     <cellStyle name="Lien hypertexte" xfId="160" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="162" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="174" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1367,6 +1391,11 @@
     <cellStyle name="Lien hypertexte visité" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="163" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="175" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1671,7 +1700,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1679,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="75" workbookViewId="0">
-      <selection activeCell="Q53" sqref="Q53"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="75" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3547,6 +3576,26 @@
         <v>272</v>
       </c>
     </row>
+    <row r="52" spans="1:14" ht="16">
+      <c r="A52" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E52" s="3">
+        <v>-890710</v>
+      </c>
+      <c r="G52" s="3">
+        <v>-286000</v>
+      </c>
+      <c r="M52" t="s">
+        <v>163</v>
+      </c>
+      <c r="N52" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3562,7 +3611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sinnvollere values for stream 1
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1722,7 +1722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1732,7 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="75" workbookViewId="0">
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
@@ -4055,7 +4055,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4376,7 +4376,7 @@
         <v>76</v>
       </c>
       <c r="C8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0.1</v>
@@ -4417,7 +4417,7 @@
         <v>77</v>
       </c>
       <c r="C9">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0.2</v>
@@ -4458,7 +4458,7 @@
         <v>79</v>
       </c>
       <c r="C10">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0.4</v>
@@ -4704,7 +4704,7 @@
         <v>91</v>
       </c>
       <c r="C16">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="D16">
         <v>0.1</v>
@@ -4745,7 +4745,7 @@
         <v>92</v>
       </c>
       <c r="C17">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D17">
         <v>0.2</v>
@@ -4786,7 +4786,7 @@
         <v>93</v>
       </c>
       <c r="C18">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0.4</v>

</xml_diff>

<commit_message>
HTU & NTU added
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,33 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mithu/CS/MatlabWD/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3690AB-0960-8C46-8786-4BC4ACD031ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="291">
   <si>
     <t>parvariable</t>
   </si>
@@ -888,16 +894,28 @@
   </si>
   <si>
     <t>Aufgabenstellung+Bericht2017</t>
+  </si>
+  <si>
+    <t>Height of theoretical units</t>
+  </si>
+  <si>
+    <t>htu</t>
+  </si>
+  <si>
+    <t>Number of theoretical units</t>
+  </si>
+  <si>
+    <t>ntu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1231,194 +1249,194 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="188">
-    <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="134" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="136" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="138" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="140" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="142" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="144" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="146" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="148" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="150" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="152" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="154" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="156" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="158" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="160" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="162" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="164" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="166" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="168" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="170" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="172" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="174" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="176" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="178" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="180" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="182" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="184" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="186" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="187" builtinId="9" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Schlecht" xfId="93" builtinId="27"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1722,21 +1740,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScale="75" workbookViewId="0">
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -1797,7 +1815,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1836,7 +1854,7 @@
       </c>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="16">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1875,7 +1893,7 @@
       </c>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:14" ht="16">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -1912,7 +1930,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:14" ht="16">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>128</v>
       </c>
@@ -1952,7 +1970,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>114</v>
       </c>
@@ -1988,7 +2006,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -2024,7 +2042,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>115</v>
       </c>
@@ -2060,7 +2078,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16">
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>121</v>
       </c>
@@ -2096,7 +2114,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16">
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>116</v>
       </c>
@@ -2132,7 +2150,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16">
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>122</v>
       </c>
@@ -2168,7 +2186,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16">
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -2210,7 +2228,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16">
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2229,7 +2247,7 @@
       <c r="L13" s="9"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:14" ht="16">
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>99</v>
       </c>
@@ -2269,7 +2287,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16">
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>105</v>
       </c>
@@ -2307,7 +2325,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16">
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>138</v>
       </c>
@@ -2339,7 +2357,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16">
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>136</v>
       </c>
@@ -2362,7 +2380,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>153</v>
       </c>
@@ -2402,7 +2420,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>154</v>
       </c>
@@ -2442,7 +2460,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>157</v>
       </c>
@@ -2482,7 +2500,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>163</v>
       </c>
@@ -2520,7 +2538,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>164</v>
       </c>
@@ -2558,7 +2576,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>169</v>
       </c>
@@ -2594,7 +2612,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>171</v>
       </c>
@@ -2630,7 +2648,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>180</v>
       </c>
@@ -2668,7 +2686,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>182</v>
       </c>
@@ -2706,7 +2724,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>184</v>
       </c>
@@ -2742,7 +2760,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>190</v>
       </c>
@@ -2777,7 +2795,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
         <v>204</v>
       </c>
@@ -2813,7 +2831,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>205</v>
       </c>
@@ -2851,7 +2869,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>202</v>
       </c>
@@ -2889,7 +2907,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>203</v>
       </c>
@@ -2927,7 +2945,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>206</v>
       </c>
@@ -2965,7 +2983,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>212</v>
       </c>
@@ -3003,7 +3021,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16">
+    <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
         <v>213</v>
       </c>
@@ -3038,7 +3056,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16">
+    <row r="36" spans="1:14">
       <c r="A36" s="1" t="s">
         <v>209</v>
       </c>
@@ -3073,7 +3091,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16">
+    <row r="37" spans="1:14">
       <c r="A37" s="1" t="s">
         <v>210</v>
       </c>
@@ -3111,7 +3129,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16">
+    <row r="38" spans="1:14">
       <c r="A38" s="1" t="s">
         <v>207</v>
       </c>
@@ -3149,7 +3167,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16">
+    <row r="39" spans="1:14">
       <c r="A39" s="1" t="s">
         <v>208</v>
       </c>
@@ -3187,7 +3205,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16">
+    <row r="40" spans="1:14">
       <c r="A40" s="1" t="s">
         <v>211</v>
       </c>
@@ -3225,7 +3243,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16">
+    <row r="41" spans="1:14">
       <c r="A41" s="1" t="s">
         <v>216</v>
       </c>
@@ -3263,7 +3281,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16">
+    <row r="42" spans="1:14">
       <c r="A42" s="1" t="s">
         <v>217</v>
       </c>
@@ -3298,7 +3316,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16">
+    <row r="43" spans="1:14">
       <c r="A43" s="1" t="s">
         <v>223</v>
       </c>
@@ -3333,7 +3351,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16">
+    <row r="44" spans="1:14">
       <c r="A44" s="1" t="s">
         <v>225</v>
       </c>
@@ -3368,7 +3386,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="16">
+    <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
         <v>234</v>
       </c>
@@ -3406,7 +3424,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="16">
+    <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
         <v>256</v>
       </c>
@@ -3438,7 +3456,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="16">
+    <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
         <v>257</v>
       </c>
@@ -3470,7 +3488,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="16">
+    <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
         <v>258</v>
       </c>
@@ -3502,7 +3520,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="16">
+    <row r="49" spans="1:14">
       <c r="A49" s="1" t="s">
         <v>262</v>
       </c>
@@ -3534,7 +3552,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="16">
+    <row r="50" spans="1:14">
       <c r="A50" s="1" t="s">
         <v>265</v>
       </c>
@@ -3566,7 +3584,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="16">
+    <row r="51" spans="1:14">
       <c r="A51" s="1" t="s">
         <v>264</v>
       </c>
@@ -3598,7 +3616,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="16">
+    <row r="52" spans="1:14">
       <c r="A52" s="1" t="s">
         <v>281</v>
       </c>
@@ -3618,7 +3636,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="16">
+    <row r="53" spans="1:14">
       <c r="A53" s="1" t="s">
         <v>284</v>
       </c>
@@ -3653,14 +3671,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="32" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
@@ -4037,6 +4055,25 @@
       </c>
       <c r="H28" t="s">
         <v>274</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B29" t="s">
+        <v>288</v>
+      </c>
+      <c r="H29" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B30" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -4051,14 +4088,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
in out paras absorber
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mithu/CS/MatlabWD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3690AB-0960-8C46-8786-4BC4ACD031ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055F5E43-E92A-C649-B7F1-09086CA6070B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -1249,99 +1249,100 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="188">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Bad" xfId="93" builtinId="27"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1435,8 +1436,7 @@
     <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
-    <cellStyle name="Schlecht" xfId="93" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3674,7 +3674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -4091,8 +4091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4236,39 +4236,6 @@
       <c r="B4" t="s">
         <v>68</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="J4">
-        <v>5</v>
-      </c>
-      <c r="K4">
-        <v>5</v>
-      </c>
-      <c r="L4">
-        <v>5</v>
-      </c>
-      <c r="M4">
-        <v>5</v>
-      </c>
       <c r="N4" t="s">
         <v>134</v>
       </c>
@@ -4280,39 +4247,6 @@
       <c r="B5" t="s">
         <v>70</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
-      <c r="K5">
-        <v>5</v>
-      </c>
-      <c r="L5">
-        <v>5</v>
-      </c>
-      <c r="M5">
-        <v>5</v>
-      </c>
       <c r="N5" t="s">
         <v>134</v>
       </c>
@@ -4324,39 +4258,8 @@
       <c r="B6" t="s">
         <v>72</v>
       </c>
-      <c r="C6">
-        <v>500000</v>
-      </c>
-      <c r="D6">
-        <v>500000</v>
-      </c>
-      <c r="E6">
-        <v>500000</v>
-      </c>
-      <c r="F6">
-        <v>500000</v>
-      </c>
-      <c r="G6">
-        <v>500000</v>
-      </c>
-      <c r="H6">
-        <v>500000</v>
-      </c>
-      <c r="I6">
-        <v>500000</v>
-      </c>
-      <c r="J6">
-        <v>500000</v>
-      </c>
-      <c r="K6" s="3">
-        <v>100000</v>
-      </c>
-      <c r="L6" s="3">
-        <v>100000</v>
-      </c>
-      <c r="M6">
-        <v>500000</v>
-      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
       <c r="N6" t="s">
         <v>135</v>
       </c>
@@ -4368,39 +4271,6 @@
       <c r="B7" t="s">
         <v>74</v>
       </c>
-      <c r="C7">
-        <v>298</v>
-      </c>
-      <c r="D7">
-        <v>370</v>
-      </c>
-      <c r="E7">
-        <v>370</v>
-      </c>
-      <c r="F7">
-        <v>370</v>
-      </c>
-      <c r="G7">
-        <v>370</v>
-      </c>
-      <c r="H7">
-        <v>370</v>
-      </c>
-      <c r="I7">
-        <v>370</v>
-      </c>
-      <c r="J7">
-        <v>370</v>
-      </c>
-      <c r="K7">
-        <v>370</v>
-      </c>
-      <c r="L7">
-        <v>370</v>
-      </c>
-      <c r="M7">
-        <v>370</v>
-      </c>
       <c r="N7" t="s">
         <v>103</v>
       </c>
@@ -4412,39 +4282,6 @@
       <c r="B8" t="s">
         <v>76</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0.1</v>
-      </c>
-      <c r="E8">
-        <v>0.1</v>
-      </c>
-      <c r="F8">
-        <v>0.1</v>
-      </c>
-      <c r="G8">
-        <v>0.1</v>
-      </c>
-      <c r="H8">
-        <v>0.1</v>
-      </c>
-      <c r="I8">
-        <v>0.1</v>
-      </c>
-      <c r="J8">
-        <v>0.1</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0.1</v>
-      </c>
-      <c r="M8">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
@@ -4453,39 +4290,6 @@
       <c r="B9" t="s">
         <v>77</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0.2</v>
-      </c>
-      <c r="E9">
-        <v>0.2</v>
-      </c>
-      <c r="F9">
-        <v>0.2</v>
-      </c>
-      <c r="G9">
-        <v>0.2</v>
-      </c>
-      <c r="H9">
-        <v>0.2</v>
-      </c>
-      <c r="I9">
-        <v>0.2</v>
-      </c>
-      <c r="J9">
-        <v>0.2</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0.2</v>
-      </c>
-      <c r="M9">
-        <v>0.2</v>
-      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
@@ -4494,39 +4298,6 @@
       <c r="B10" t="s">
         <v>79</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0.4</v>
-      </c>
-      <c r="E10">
-        <v>0.4</v>
-      </c>
-      <c r="F10">
-        <v>0.4</v>
-      </c>
-      <c r="G10">
-        <v>0.4</v>
-      </c>
-      <c r="H10">
-        <v>0.4</v>
-      </c>
-      <c r="I10">
-        <v>0.4</v>
-      </c>
-      <c r="J10">
-        <v>0.4</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0.4</v>
-      </c>
-      <c r="M10">
-        <v>0.4</v>
-      </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="5" t="s">
@@ -4535,39 +4306,6 @@
       <c r="B11" t="s">
         <v>81</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0.5</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="5" t="s">
@@ -4576,39 +4314,6 @@
       <c r="B12" t="s">
         <v>83</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="5" t="s">
@@ -4617,39 +4322,6 @@
       <c r="B13" t="s">
         <v>85</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="5" t="s">
@@ -4658,39 +4330,6 @@
       <c r="B14" t="s">
         <v>229</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0.5</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="5" t="s">
@@ -4699,39 +4338,6 @@
       <c r="B15" t="s">
         <v>236</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
@@ -4740,325 +4346,61 @@
       <c r="B16" t="s">
         <v>91</v>
       </c>
-      <c r="C16">
-        <v>0.6</v>
-      </c>
-      <c r="D16">
-        <v>0.1</v>
-      </c>
-      <c r="E16">
-        <v>0.1</v>
-      </c>
-      <c r="F16">
-        <v>0.1</v>
-      </c>
-      <c r="G16">
-        <v>0.1</v>
-      </c>
-      <c r="H16">
-        <v>0.1</v>
-      </c>
-      <c r="I16">
-        <v>0.1</v>
-      </c>
-      <c r="J16">
-        <v>0.1</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0.1</v>
-      </c>
-      <c r="M16">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B17" t="s">
         <v>92</v>
       </c>
-      <c r="C17">
-        <v>0.4</v>
-      </c>
-      <c r="D17">
-        <v>0.2</v>
-      </c>
-      <c r="E17">
-        <v>0.2</v>
-      </c>
-      <c r="F17">
-        <v>0.2</v>
-      </c>
-      <c r="G17">
-        <v>0.2</v>
-      </c>
-      <c r="H17">
-        <v>0.2</v>
-      </c>
-      <c r="I17">
-        <v>0.2</v>
-      </c>
-      <c r="J17">
-        <v>0.2</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0.2</v>
-      </c>
-      <c r="M17">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B18" t="s">
         <v>93</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0.4</v>
-      </c>
-      <c r="E18">
-        <v>0.4</v>
-      </c>
-      <c r="F18">
-        <v>0.4</v>
-      </c>
-      <c r="G18">
-        <v>0.4</v>
-      </c>
-      <c r="H18">
-        <v>0.4</v>
-      </c>
-      <c r="I18">
-        <v>0.4</v>
-      </c>
-      <c r="J18">
-        <v>0.4</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0.4</v>
-      </c>
-      <c r="M18">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B19" t="s">
         <v>94</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B20" t="s">
         <v>95</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B21" t="s">
         <v>96</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="5" t="s">
         <v>188</v>
       </c>
       <c r="B22" t="s">
         <v>189</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>230</v>
       </c>
       <c r="B23" t="s">
         <v>231</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some clean ups, system ready for  overall  optimization Velocity profile added
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3458DA0-CB7D-D143-A28C-A2F7CBB38AF1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCECC168-5373-7F42-8298-62E3933896B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26960" windowHeight="16040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="305">
   <si>
     <t>parvariable</t>
   </si>
@@ -779,9 +779,6 @@
     <t>deltaHNH</t>
   </si>
   <si>
-    <t>foo</t>
-  </si>
-  <si>
     <t>entity PI</t>
   </si>
   <si>
@@ -906,6 +903,51 @@
   </si>
   <si>
     <t>ntu</t>
+  </si>
+  <si>
+    <t>Number of reactor segments in row</t>
+  </si>
+  <si>
+    <t>nrow</t>
+  </si>
+  <si>
+    <t>N_tubes</t>
+  </si>
+  <si>
+    <t>Number of Tubes total</t>
+  </si>
+  <si>
+    <t>Number of Tubes aside</t>
+  </si>
+  <si>
+    <t>N_tubes_aside</t>
+  </si>
+  <si>
+    <t>Abolute Feed CH4 per single tube</t>
+  </si>
+  <si>
+    <t>FCH4</t>
+  </si>
+  <si>
+    <t>Peng Ribinson (1) or ideal Gas law (0)</t>
+  </si>
+  <si>
+    <t>ideal_real</t>
+  </si>
+  <si>
+    <t>% NH3 rel CH4</t>
+  </si>
+  <si>
+    <t>ubsch</t>
+  </si>
+  <si>
+    <t>yield in terms of CH4</t>
+  </si>
+  <si>
+    <t>yield</t>
+  </si>
+  <si>
+    <t>source</t>
   </si>
 </sst>
 </file>
@@ -915,7 +957,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -979,6 +1021,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1222,7 +1270,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1247,6 +1295,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="188">
     <cellStyle name="Bad" xfId="93" builtinId="27"/>
@@ -1494,7 +1543,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1546,7 +1595,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1750,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView topLeftCell="A28" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1803,7 +1852,7 @@
         <v>62</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>64</v>
@@ -1891,7 +1940,12 @@
       <c r="L3" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="M3" s="7"/>
+      <c r="M3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
@@ -3426,10 +3480,10 @@
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C46" s="3">
         <v>-36.826000000000001</v>
@@ -3453,15 +3507,15 @@
         <v>18.811</v>
       </c>
       <c r="N46" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C47" s="3">
         <v>0.42899999999999999</v>
@@ -3485,15 +3539,15 @@
         <v>0.49837999999999999</v>
       </c>
       <c r="N47" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C48" s="3">
         <v>-1.6200000000000001E-5</v>
@@ -3517,15 +3571,15 @@
         <v>-1.0851E-4</v>
       </c>
       <c r="N48" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="49" spans="1:14">
       <c r="A49" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>262</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>263</v>
       </c>
       <c r="C49" s="3">
         <v>5.2999999999999998E-4</v>
@@ -3549,15 +3603,15 @@
         <v>-1.2E-2</v>
       </c>
       <c r="N49" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B50" s="7" t="s">
         <v>265</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>266</v>
       </c>
       <c r="C50" s="3">
         <v>4.7092999999999998E-5</v>
@@ -3581,15 +3635,15 @@
         <v>1.0208E-4</v>
       </c>
       <c r="N50" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:14">
       <c r="A51" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C51" s="3">
         <v>4.9550999999999998E-8</v>
@@ -3613,15 +3667,15 @@
         <v>-2.2402999999999999E-8</v>
       </c>
       <c r="N51" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B52" s="7" t="s">
         <v>281</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>282</v>
       </c>
       <c r="E52" s="3">
         <v>-890710</v>
@@ -3633,15 +3687,15 @@
         <v>159</v>
       </c>
       <c r="N52" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="53" spans="1:14">
       <c r="A53" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B53" s="7" t="s">
         <v>284</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>285</v>
       </c>
       <c r="E53">
         <v>250</v>
@@ -3653,10 +3707,10 @@
         <v>100</v>
       </c>
       <c r="M53" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N53" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3672,10 +3726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3758,6 +3812,9 @@
       <c r="G3" t="s">
         <v>33</v>
       </c>
+      <c r="H3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
@@ -3780,7 +3837,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B6" t="s">
         <v>45</v>
@@ -3790,7 +3847,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="H6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3953,127 +4010,162 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B21" t="s">
-        <v>248</v>
-      </c>
-      <c r="C21">
-        <v>666</v>
+        <v>252</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="H21" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B22" t="s">
-        <v>253</v>
-      </c>
-      <c r="C22" s="3">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="H22" t="s">
-        <v>252</v>
+        <v>254</v>
+      </c>
+      <c r="C22" s="19">
+        <v>10000</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="B23" t="s">
-        <v>255</v>
-      </c>
-      <c r="C23" s="19">
-        <v>10000</v>
+        <v>269</v>
+      </c>
+      <c r="C23">
+        <v>500</v>
+      </c>
+      <c r="H23" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B24" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C24">
-        <v>500</v>
+        <v>0.15</v>
       </c>
       <c r="H24" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B25" t="s">
+        <v>275</v>
+      </c>
+      <c r="C25">
+        <v>0.1</v>
+      </c>
+      <c r="H25" t="s">
         <v>273</v>
-      </c>
-      <c r="C25">
-        <v>0.15</v>
-      </c>
-      <c r="H25" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B26" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C26">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="H26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B27" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C27">
-        <v>20</v>
+        <v>250</v>
       </c>
       <c r="H27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="B28" t="s">
-        <v>280</v>
-      </c>
-      <c r="C28">
-        <v>250</v>
+        <v>287</v>
       </c>
       <c r="H28" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B29" t="s">
-        <v>288</v>
-      </c>
-      <c r="H29" t="s">
-        <v>252</v>
+        <v>289</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B30" t="s">
-        <v>290</v>
+        <v>291</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B32" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B33" t="s">
+        <v>299</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B34" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -4089,10 +4181,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:M23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4228,6 +4320,9 @@
       <c r="M3" s="6" t="s">
         <v>149</v>
       </c>
+      <c r="N3" s="6" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
@@ -4325,7 +4420,7 @@
         <v>72</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>101325</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -4369,10 +4464,10 @@
         <v>74</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -4774,7 +4869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>127</v>
       </c>
@@ -4815,7 +4910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:14">
       <c r="A18" s="5" t="s">
         <v>90</v>
       </c>
@@ -4856,7 +4951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:14">
       <c r="A19" s="5" t="s">
         <v>87</v>
       </c>
@@ -4897,7 +4992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:14">
       <c r="A20" s="5" t="s">
         <v>88</v>
       </c>
@@ -4938,7 +5033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:14">
       <c r="A21" s="5" t="s">
         <v>89</v>
       </c>
@@ -4979,7 +5074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:14">
       <c r="A22" s="5" t="s">
         <v>188</v>
       </c>
@@ -5020,7 +5115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:14">
       <c r="A23" s="5" t="s">
         <v>230</v>
       </c>
@@ -5059,6 +5154,31 @@
       </c>
       <c r="M23">
         <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B24" t="s">
+        <v>297</v>
+      </c>
+      <c r="C24">
+        <v>1E-3</v>
+      </c>
+      <c r="N24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B25" t="s">
+        <v>301</v>
+      </c>
+      <c r="C25">
+        <v>1.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reactor opex now dependent from set inlet variable for mass stream of heating medium
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCECC168-5373-7F42-8298-62E3933896B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DF340F-2360-DF4D-9B68-D189D8F6ED6B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26960" windowHeight="16040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26340" windowHeight="15920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="307">
   <si>
     <t>parvariable</t>
   </si>
@@ -948,6 +948,12 @@
   </si>
   <si>
     <t>source</t>
+  </si>
+  <si>
+    <t>Gas molar fraction CO2</t>
+  </si>
+  <si>
+    <t>yCO2</t>
   </si>
 </sst>
 </file>
@@ -1799,7 +1805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="75" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -3728,8 +3734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4181,15 +4187,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -5090,9 +5097,6 @@
       <c r="E22">
         <v>0</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
       <c r="G22">
         <v>0</v>
       </c>
@@ -5132,7 +5136,7 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.66659999999999997</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -5158,26 +5162,37 @@
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="5" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="B24" t="s">
-        <v>297</v>
-      </c>
-      <c r="C24">
-        <v>1E-3</v>
-      </c>
-      <c r="N24" t="s">
-        <v>134</v>
+        <v>306</v>
+      </c>
+      <c r="F24">
+        <v>0.33329999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B25" t="s">
+        <v>297</v>
+      </c>
+      <c r="C25">
+        <v>1E-3</v>
+      </c>
+      <c r="N25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>301</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>1.05</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reactor moved commented out some outputs to move them to evaluator
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DF340F-2360-DF4D-9B68-D189D8F6ED6B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C95D34E-B1F0-BA44-9B4F-56269FDE30ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26340" windowHeight="15920" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26340" windowHeight="15920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="309">
   <si>
     <t>parvariable</t>
   </si>
@@ -954,6 +954,12 @@
   </si>
   <si>
     <t>yCO2</t>
+  </si>
+  <si>
+    <t>cocross</t>
+  </si>
+  <si>
+    <t>Co(1) or cross(0) current reactor heting</t>
   </si>
 </sst>
 </file>
@@ -3732,10 +3738,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4168,9 +4174,20 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B34" t="s">
+        <v>307</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>303</v>
       </c>
     </row>
@@ -4189,7 +4206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Priitive Overall Optimization Fucntion Included
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C95D34E-B1F0-BA44-9B4F-56269FDE30ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB461D70-D2D4-1540-9851-C7FAA7D072B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26340" windowHeight="15920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1811,7 +1811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -3740,8 +3740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3906,6 +3906,18 @@
         <v>37</v>
       </c>
       <c r="C11" s="3"/>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
@@ -3914,6 +3926,18 @@
       <c r="B12" t="s">
         <v>38</v>
       </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
@@ -3922,7 +3946,18 @@
       <c r="B13" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">

</xml_diff>

<commit_message>
nasty parameter bug fixed
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2CF9A0-8063-E644-B417-D78335455CBF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116492E9-93DD-E94D-8B95-541966AD78D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26340" windowHeight="15920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3746,8 +3746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4221,7 +4221,7 @@
         <v>307</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -4256,7 +4256,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4537,7 +4537,7 @@
         <v>74</v>
       </c>
       <c r="C7">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D7">
         <v>1600</v>

</xml_diff>

<commit_message>
Main Now takes Paramters for calculation at the very top; Main now generates an exel output file for the optimized run;
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/main/Desktop/CS/MatlabWD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BBA2B8-14A2-E840-8206-76C0BE2E82F9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0425503-EC5F-9141-B7D3-7B75F2C31C78}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26340" windowHeight="15920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="315">
   <si>
     <t>parvariable</t>
   </si>
@@ -966,6 +966,18 @@
   </si>
   <si>
     <t>mol s-1</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>$/y</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>$/kg</t>
   </si>
 </sst>
 </file>
@@ -3744,10 +3756,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3841,6 +3853,9 @@
       <c r="B4" t="s">
         <v>26</v>
       </c>
+      <c r="H4" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
@@ -3852,6 +3867,9 @@
       <c r="C5">
         <v>2</v>
       </c>
+      <c r="H5" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
@@ -3924,6 +3942,9 @@
       <c r="G11">
         <v>0</v>
       </c>
+      <c r="H11" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
@@ -3944,6 +3965,9 @@
       <c r="G12">
         <v>0</v>
       </c>
+      <c r="H12" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
@@ -4241,6 +4265,14 @@
       </c>
       <c r="H36" t="s">
         <v>310</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="B37" t="s">
+        <v>313</v>
+      </c>
+      <c r="H37" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data for CO2 added (minor change)
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1824,7 +1824,7 @@
   <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2489,7 +2489,9 @@
       <c r="J18" s="13">
         <v>-1180900</v>
       </c>
-      <c r="K18" s="13"/>
+      <c r="K18" s="13">
+        <v>-393510</v>
+      </c>
       <c r="L18" s="13"/>
       <c r="M18" s="7" t="s">
         <v>159</v>
@@ -2529,7 +2531,9 @@
       <c r="J19" s="13">
         <v>-901700</v>
       </c>
-      <c r="K19" s="13"/>
+      <c r="K19" s="13">
+        <v>394390</v>
+      </c>
       <c r="L19" s="13"/>
       <c r="M19" s="7" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
diameter and L/G ratio added in unit table
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,33 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Selina\Desktop\selinsch6\MatlabWD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE3B844-94E6-4E33-A37F-39BAAC5F0D6F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="319">
   <si>
     <t>parvariable</t>
   </si>
@@ -972,16 +978,28 @@
   </si>
   <si>
     <t>$/kg</t>
+  </si>
+  <si>
+    <t>Diameter of column</t>
+  </si>
+  <si>
+    <t>dia</t>
+  </si>
+  <si>
+    <t>L/G ratio</t>
+  </si>
+  <si>
+    <t>ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1322,194 +1340,194 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="188">
-    <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="134" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="136" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="138" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="140" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="142" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="144" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="146" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="148" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="150" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="152" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="154" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="156" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="158" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="160" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="162" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="164" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="166" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="168" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="170" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="172" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="174" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="176" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="178" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="180" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="182" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="184" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="186" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="187" builtinId="9" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Schlecht" xfId="93" builtinId="27"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1813,21 +1831,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -1888,7 +1906,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1927,7 +1945,7 @@
       </c>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="16">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1971,7 +1989,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -2008,7 +2026,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:14" ht="16">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>128</v>
       </c>
@@ -2048,7 +2066,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>114</v>
       </c>
@@ -2084,7 +2102,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>107</v>
       </c>
@@ -2120,7 +2138,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>115</v>
       </c>
@@ -2156,7 +2174,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16">
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>121</v>
       </c>
@@ -2192,7 +2210,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16">
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>116</v>
       </c>
@@ -2228,7 +2246,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="16">
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>122</v>
       </c>
@@ -2264,7 +2282,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16">
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -2306,7 +2324,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16">
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2325,7 +2343,7 @@
       <c r="L13" s="9"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:14" ht="16">
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>99</v>
       </c>
@@ -2365,7 +2383,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16">
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>105</v>
       </c>
@@ -2403,7 +2421,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16">
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>138</v>
       </c>
@@ -2435,7 +2453,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16">
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>136</v>
       </c>
@@ -2458,7 +2476,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>153</v>
       </c>
@@ -2500,7 +2518,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>154</v>
       </c>
@@ -2542,7 +2560,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>157</v>
       </c>
@@ -2582,7 +2600,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>163</v>
       </c>
@@ -2620,7 +2638,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>164</v>
       </c>
@@ -2658,7 +2676,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>169</v>
       </c>
@@ -2694,7 +2712,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>171</v>
       </c>
@@ -2730,7 +2748,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>180</v>
       </c>
@@ -2768,7 +2786,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>182</v>
       </c>
@@ -2806,7 +2824,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>184</v>
       </c>
@@ -2842,7 +2860,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>190</v>
       </c>
@@ -2877,7 +2895,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
         <v>204</v>
       </c>
@@ -2913,7 +2931,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>205</v>
       </c>
@@ -2951,7 +2969,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>202</v>
       </c>
@@ -2989,7 +3007,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>203</v>
       </c>
@@ -3027,7 +3045,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>206</v>
       </c>
@@ -3065,7 +3083,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>212</v>
       </c>
@@ -3103,7 +3121,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16">
+    <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
         <v>213</v>
       </c>
@@ -3138,7 +3156,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16">
+    <row r="36" spans="1:14">
       <c r="A36" s="1" t="s">
         <v>209</v>
       </c>
@@ -3173,7 +3191,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16">
+    <row r="37" spans="1:14">
       <c r="A37" s="1" t="s">
         <v>210</v>
       </c>
@@ -3211,7 +3229,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16">
+    <row r="38" spans="1:14">
       <c r="A38" s="1" t="s">
         <v>207</v>
       </c>
@@ -3249,7 +3267,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16">
+    <row r="39" spans="1:14">
       <c r="A39" s="1" t="s">
         <v>208</v>
       </c>
@@ -3287,7 +3305,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16">
+    <row r="40" spans="1:14">
       <c r="A40" s="1" t="s">
         <v>211</v>
       </c>
@@ -3325,7 +3343,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16">
+    <row r="41" spans="1:14">
       <c r="A41" s="1" t="s">
         <v>216</v>
       </c>
@@ -3363,7 +3381,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16">
+    <row r="42" spans="1:14">
       <c r="A42" s="1" t="s">
         <v>217</v>
       </c>
@@ -3398,7 +3416,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16">
+    <row r="43" spans="1:14">
       <c r="A43" s="1" t="s">
         <v>223</v>
       </c>
@@ -3433,7 +3451,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16">
+    <row r="44" spans="1:14">
       <c r="A44" s="1" t="s">
         <v>225</v>
       </c>
@@ -3468,7 +3486,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="16">
+    <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
         <v>234</v>
       </c>
@@ -3506,7 +3524,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="16">
+    <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
         <v>255</v>
       </c>
@@ -3538,7 +3556,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="16">
+    <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
         <v>256</v>
       </c>
@@ -3570,7 +3588,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="16">
+    <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
         <v>257</v>
       </c>
@@ -3602,7 +3620,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="16">
+    <row r="49" spans="1:14">
       <c r="A49" s="1" t="s">
         <v>261</v>
       </c>
@@ -3634,7 +3652,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="16">
+    <row r="50" spans="1:14">
       <c r="A50" s="1" t="s">
         <v>264</v>
       </c>
@@ -3666,7 +3684,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="16">
+    <row r="51" spans="1:14">
       <c r="A51" s="1" t="s">
         <v>263</v>
       </c>
@@ -3698,7 +3716,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="16">
+    <row r="52" spans="1:14">
       <c r="A52" s="1" t="s">
         <v>280</v>
       </c>
@@ -3718,7 +3736,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="16">
+    <row r="53" spans="1:14">
       <c r="A53" s="1" t="s">
         <v>283</v>
       </c>
@@ -3753,14 +3771,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="32" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
@@ -4271,6 +4289,22 @@
       </c>
       <c r="H37" t="s">
         <v>314</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B38" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B39" t="s">
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -4285,14 +4319,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="6" max="6" width="7.1640625" customWidth="1"/>

</xml_diff>

<commit_message>
addition of volumetric fraction of h2so4 in excel table
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Selina\Desktop\selinsch6\MatlabWD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE3B844-94E6-4E33-A37F-39BAAC5F0D6F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED9E3FF-346F-4A55-B18B-7F30A56D966A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="321">
   <si>
     <t>parvariable</t>
   </si>
@@ -990,6 +990,12 @@
   </si>
   <si>
     <t>ratio</t>
+  </si>
+  <si>
+    <t>Volumetric fraction H2SO4</t>
+  </si>
+  <si>
+    <t>frac_h2so4</t>
   </si>
 </sst>
 </file>
@@ -3772,7 +3778,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
@@ -4305,6 +4311,14 @@
       </c>
       <c r="B39" t="s">
         <v>318</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B40" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New line added for liquid flow in the nonideal case
</commit_message>
<xml_diff>
--- a/MatlabWD/Data.xlsx
+++ b/MatlabWD/Data.xlsx
@@ -1,33 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mithu/mithu/MatlabWD/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D083E826-1443-E441-A485-BF55357DE5D1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPOUNDS" sheetId="1" r:id="rId1"/>
     <sheet name="UNIT OPERATIONS" sheetId="2" r:id="rId2"/>
     <sheet name="STREAMS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="317">
   <si>
     <t>parvariable</t>
   </si>
@@ -972,16 +978,22 @@
   </si>
   <si>
     <t>Yaws</t>
+  </si>
+  <si>
+    <t>Liquid flow rate nonideal</t>
+  </si>
+  <si>
+    <t>Lreal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1315,194 +1327,194 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="188">
-    <cellStyle name="Insatisfaisant" xfId="93" builtinId="27"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="94" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="96" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="118" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="120" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="128" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="130" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="132" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="134" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="136" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="138" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="140" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="142" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="144" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="146" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="148" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="150" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="152" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="154" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="156" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="158" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="160" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="162" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="164" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="166" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="168" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="170" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="172" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="174" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="176" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="178" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="180" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="182" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="184" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="186" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="95" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="97" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="119" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="121" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="129" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="131" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="133" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="135" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="137" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="139" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="141" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="143" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="145" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="147" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="149" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="151" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="153" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="155" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="157" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="159" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="161" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="163" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="165" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="167" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="169" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="171" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="173" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="175" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="177" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="179" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="181" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="183" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="185" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="187" builtinId="9" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Schlecht" xfId="93" builtinId="27"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1806,21 +1818,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="47.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -1881,7 +1893,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1920,7 +1932,7 @@
       </c>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="16">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1964,7 +1976,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
@@ -2001,7 +2013,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:14" ht="16">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>119</v>
       </c>
@@ -2041,7 +2053,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="16">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>107</v>
       </c>
@@ -2079,7 +2091,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="16">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>108</v>
       </c>
@@ -2117,7 +2129,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>109</v>
       </c>
@@ -2155,7 +2167,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16">
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -2197,7 +2209,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="16">
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2216,7 +2228,7 @@
       <c r="L10" s="9"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:14" ht="16">
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>99</v>
       </c>
@@ -2256,7 +2268,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16">
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>105</v>
       </c>
@@ -2294,7 +2306,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16">
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>128</v>
       </c>
@@ -2326,7 +2338,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16">
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>126</v>
       </c>
@@ -2349,7 +2361,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="16">
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>143</v>
       </c>
@@ -2391,7 +2403,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="16">
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>144</v>
       </c>
@@ -2433,7 +2445,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="16">
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
         <v>147</v>
       </c>
@@ -2473,7 +2485,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="16">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>153</v>
       </c>
@@ -2511,7 +2523,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="16">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
         <v>154</v>
       </c>
@@ -2549,7 +2561,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="16">
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
         <v>159</v>
       </c>
@@ -2585,7 +2597,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="16">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
         <v>161</v>
       </c>
@@ -2621,7 +2633,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="16">
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
         <v>170</v>
       </c>
@@ -2659,7 +2671,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="16">
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
         <v>172</v>
       </c>
@@ -2697,7 +2709,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="16">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>174</v>
       </c>
@@ -2733,7 +2745,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="16">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
         <v>180</v>
       </c>
@@ -2768,7 +2780,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="16">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
         <v>194</v>
       </c>
@@ -2804,7 +2816,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="16">
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
         <v>195</v>
       </c>
@@ -2842,7 +2854,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="16">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
         <v>192</v>
       </c>
@@ -2880,7 +2892,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="16">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
         <v>193</v>
       </c>
@@ -2918,7 +2930,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="16">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
         <v>196</v>
       </c>
@@ -2956,7 +2968,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="16">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
         <v>202</v>
       </c>
@@ -2994,7 +3006,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="16">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
         <v>203</v>
       </c>
@@ -3029,7 +3041,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="16">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>199</v>
       </c>
@@ -3064,7 +3076,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="16">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>200</v>
       </c>
@@ -3102,7 +3114,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="16">
+    <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
         <v>197</v>
       </c>
@@ -3140,7 +3152,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="16">
+    <row r="36" spans="1:14">
       <c r="A36" s="1" t="s">
         <v>198</v>
       </c>
@@ -3178,7 +3190,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="16">
+    <row r="37" spans="1:14">
       <c r="A37" s="1" t="s">
         <v>201</v>
       </c>
@@ -3216,7 +3228,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="16">
+    <row r="38" spans="1:14">
       <c r="A38" s="1" t="s">
         <v>206</v>
       </c>
@@ -3254,7 +3266,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="16">
+    <row r="39" spans="1:14">
       <c r="A39" s="1" t="s">
         <v>207</v>
       </c>
@@ -3289,7 +3301,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="16">
+    <row r="40" spans="1:14">
       <c r="A40" s="1" t="s">
         <v>213</v>
       </c>
@@ -3324,7 +3336,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="16">
+    <row r="41" spans="1:14">
       <c r="A41" s="1" t="s">
         <v>215</v>
       </c>
@@ -3359,7 +3371,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="16">
+    <row r="42" spans="1:14">
       <c r="A42" s="1" t="s">
         <v>224</v>
       </c>
@@ -3397,7 +3409,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="16">
+    <row r="43" spans="1:14">
       <c r="A43" s="1" t="s">
         <v>245</v>
       </c>
@@ -3429,7 +3441,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="16">
+    <row r="44" spans="1:14">
       <c r="A44" s="1" t="s">
         <v>246</v>
       </c>
@@ -3461,7 +3473,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="16">
+    <row r="45" spans="1:14">
       <c r="A45" s="1" t="s">
         <v>247</v>
       </c>
@@ -3493,7 +3505,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="16">
+    <row r="46" spans="1:14">
       <c r="A46" s="1" t="s">
         <v>251</v>
       </c>
@@ -3525,7 +3537,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="16">
+    <row r="47" spans="1:14">
       <c r="A47" s="1" t="s">
         <v>254</v>
       </c>
@@ -3557,7 +3569,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="16">
+    <row r="48" spans="1:14">
       <c r="A48" s="1" t="s">
         <v>253</v>
       </c>
@@ -3589,7 +3601,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="16">
+    <row r="49" spans="1:14">
       <c r="A49" s="1" t="s">
         <v>270</v>
       </c>
@@ -3609,7 +3621,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="16">
+    <row r="50" spans="1:14">
       <c r="A50" s="1" t="s">
         <v>273</v>
       </c>
@@ -3644,14 +3656,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="32" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
@@ -4200,14 +4212,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="6" max="6" width="7.1640625" customWidth="1"/>
@@ -4380,7 +4392,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>518.1</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -5208,6 +5220,50 @@
       </c>
       <c r="C26">
         <v>1.05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B27" t="s">
+        <v>316</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>575.6</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>